<commit_message>
corrected mistake in dplyr 2
</commit_message>
<xml_diff>
--- a/compounding_growth_10_percent.xlsx
+++ b/compounding_growth_10_percent.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zablotski/Library/Mobile Documents/com~apple~CloudDocs/7. Hobby/programming and stats/yuzaR-Blog/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01FF51EA-3399-AF49-AFB4-ED07A229D95B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4A56C78-8249-5643-9CFF-412CF32CE91D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{EDD741CF-9DB9-2945-BF15-255A1807DC69}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="21">
   <si>
     <t>year</t>
   </si>
@@ -76,6 +76,18 @@
   </si>
   <si>
     <t>row_number</t>
+  </si>
+  <si>
+    <t>super_thanks</t>
+  </si>
+  <si>
+    <t>koji</t>
+  </si>
+  <si>
+    <t>total_earnings</t>
+  </si>
+  <si>
+    <t>difference</t>
   </si>
 </sst>
 </file>
@@ -431,18 +443,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6A4B67E-A70E-FF47-86DD-9BF22E85C9FF}">
-  <dimension ref="A1:E97"/>
+  <dimension ref="A1:I97"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="284" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -458,8 +477,20 @@
       <c r="E1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -475,8 +506,22 @@
       <c r="E2">
         <v>13.65</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <f>SUM(E2:G2)</f>
+        <v>13.65</v>
+      </c>
+      <c r="I2" s="1">
+        <f>H2-D2</f>
+        <v>-1.3499999999999996</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -493,8 +538,22 @@
       <c r="E3">
         <v>23.92</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3">
+        <v>4.93</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H4" si="0">SUM(E3:G3)</f>
+        <v>28.85</v>
+      </c>
+      <c r="I3" s="1">
+        <f t="shared" ref="I3:I9" si="1">H3-D3</f>
+        <v>12.350000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -511,8 +570,22 @@
       <c r="E4">
         <v>23.52</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>23.52</v>
+      </c>
+      <c r="I4" s="1">
+        <f t="shared" si="1"/>
+        <v>5.3699999999999974</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -526,8 +599,22 @@
         <f>D4*1.1</f>
         <v>19.965000000000003</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>19</v>
+      </c>
+      <c r="H5">
+        <f t="shared" ref="H5:H9" si="2">SUM(E5:G5)</f>
+        <v>19</v>
+      </c>
+      <c r="I5" s="1">
+        <f t="shared" si="1"/>
+        <v>-0.96500000000000341</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -538,11 +625,12 @@
         <v>8</v>
       </c>
       <c r="D6" s="1">
-        <f t="shared" ref="D6:D69" si="0">D5*1.1</f>
+        <f t="shared" ref="D6:D69" si="3">D5*1.1</f>
         <v>21.961500000000004</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -553,11 +641,12 @@
         <v>9</v>
       </c>
       <c r="D7" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>24.157650000000007</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -568,11 +657,12 @@
         <v>10</v>
       </c>
       <c r="D8" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>26.573415000000011</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -583,11 +673,12 @@
         <v>11</v>
       </c>
       <c r="D9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>29.230756500000016</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -598,11 +689,11 @@
         <v>12</v>
       </c>
       <c r="D10" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>32.153832150000021</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -613,11 +704,11 @@
         <v>13</v>
       </c>
       <c r="D11" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>35.369215365000024</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -628,11 +719,11 @@
         <v>14</v>
       </c>
       <c r="D12" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>38.906136901500027</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -643,11 +734,11 @@
         <v>15</v>
       </c>
       <c r="D13" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>42.796750591650031</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -658,11 +749,11 @@
         <v>4</v>
       </c>
       <c r="D14" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>47.07642565081504</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -673,11 +764,11 @@
         <v>5</v>
       </c>
       <c r="D15" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>51.784068215896546</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -688,7 +779,7 @@
         <v>6</v>
       </c>
       <c r="D16" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>56.962475037486207</v>
       </c>
     </row>
@@ -703,7 +794,7 @@
         <v>7</v>
       </c>
       <c r="D17" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>62.65872254123483</v>
       </c>
     </row>
@@ -718,7 +809,7 @@
         <v>8</v>
       </c>
       <c r="D18" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>68.924594795358317</v>
       </c>
     </row>
@@ -733,7 +824,7 @@
         <v>9</v>
       </c>
       <c r="D19" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>75.817054274894161</v>
       </c>
     </row>
@@ -748,7 +839,7 @@
         <v>10</v>
       </c>
       <c r="D20" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>83.398759702383586</v>
       </c>
     </row>
@@ -763,7 +854,7 @@
         <v>11</v>
       </c>
       <c r="D21" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>91.738635672621953</v>
       </c>
     </row>
@@ -778,7 +869,7 @@
         <v>12</v>
       </c>
       <c r="D22" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>100.91249923988416</v>
       </c>
     </row>
@@ -793,7 +884,7 @@
         <v>13</v>
       </c>
       <c r="D23" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>111.00374916387258</v>
       </c>
     </row>
@@ -808,7 +899,7 @@
         <v>14</v>
       </c>
       <c r="D24" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>122.10412408025985</v>
       </c>
     </row>
@@ -823,7 +914,7 @@
         <v>15</v>
       </c>
       <c r="D25" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>134.31453648828585</v>
       </c>
     </row>
@@ -838,7 +929,7 @@
         <v>4</v>
       </c>
       <c r="D26" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>147.74599013711446</v>
       </c>
     </row>
@@ -853,7 +944,7 @@
         <v>5</v>
       </c>
       <c r="D27" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>162.52058915082591</v>
       </c>
     </row>
@@ -868,7 +959,7 @@
         <v>6</v>
       </c>
       <c r="D28" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>178.77264806590853</v>
       </c>
     </row>
@@ -883,7 +974,7 @@
         <v>7</v>
       </c>
       <c r="D29" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>196.64991287249939</v>
       </c>
     </row>
@@ -898,7 +989,7 @@
         <v>8</v>
       </c>
       <c r="D30" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>216.31490415974935</v>
       </c>
     </row>
@@ -913,7 +1004,7 @@
         <v>9</v>
       </c>
       <c r="D31" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>237.9463945757243</v>
       </c>
     </row>
@@ -928,7 +1019,7 @@
         <v>10</v>
       </c>
       <c r="D32" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>261.74103403329673</v>
       </c>
     </row>
@@ -943,7 +1034,7 @@
         <v>11</v>
       </c>
       <c r="D33" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>287.91513743662642</v>
       </c>
     </row>
@@ -958,7 +1049,7 @@
         <v>12</v>
       </c>
       <c r="D34" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>316.7066511802891</v>
       </c>
     </row>
@@ -973,7 +1064,7 @@
         <v>13</v>
       </c>
       <c r="D35" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>348.37731629831802</v>
       </c>
     </row>
@@ -988,7 +1079,7 @@
         <v>14</v>
       </c>
       <c r="D36" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>383.21504792814983</v>
       </c>
     </row>
@@ -1003,7 +1094,7 @@
         <v>15</v>
       </c>
       <c r="D37" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>421.53655272096483</v>
       </c>
     </row>
@@ -1018,7 +1109,7 @@
         <v>4</v>
       </c>
       <c r="D38" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>463.69020799306134</v>
       </c>
     </row>
@@ -1033,7 +1124,7 @@
         <v>5</v>
       </c>
       <c r="D39" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>510.05922879236749</v>
       </c>
     </row>
@@ -1048,7 +1139,7 @@
         <v>6</v>
       </c>
       <c r="D40" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>561.06515167160433</v>
       </c>
     </row>
@@ -1063,7 +1154,7 @@
         <v>7</v>
       </c>
       <c r="D41" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>617.17166683876485</v>
       </c>
     </row>
@@ -1078,7 +1169,7 @@
         <v>8</v>
       </c>
       <c r="D42" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>678.88883352264133</v>
       </c>
     </row>
@@ -1093,7 +1184,7 @@
         <v>9</v>
       </c>
       <c r="D43" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>746.77771687490554</v>
       </c>
     </row>
@@ -1108,7 +1199,7 @@
         <v>10</v>
       </c>
       <c r="D44" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>821.45548856239611</v>
       </c>
     </row>
@@ -1123,7 +1214,7 @@
         <v>11</v>
       </c>
       <c r="D45" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>903.60103741863577</v>
       </c>
     </row>
@@ -1138,7 +1229,7 @@
         <v>12</v>
       </c>
       <c r="D46" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>993.96114116049944</v>
       </c>
     </row>
@@ -1153,7 +1244,7 @@
         <v>13</v>
       </c>
       <c r="D47" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1093.3572552765495</v>
       </c>
     </row>
@@ -1168,7 +1259,7 @@
         <v>14</v>
       </c>
       <c r="D48" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1202.6929808042046</v>
       </c>
     </row>
@@ -1183,7 +1274,7 @@
         <v>15</v>
       </c>
       <c r="D49" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1322.9622788846252</v>
       </c>
     </row>
@@ -1198,7 +1289,7 @@
         <v>4</v>
       </c>
       <c r="D50" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1455.2585067730879</v>
       </c>
     </row>
@@ -1213,7 +1304,7 @@
         <v>5</v>
       </c>
       <c r="D51" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1600.7843574503968</v>
       </c>
     </row>
@@ -1228,7 +1319,7 @@
         <v>6</v>
       </c>
       <c r="D52" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1760.8627931954366</v>
       </c>
     </row>
@@ -1243,7 +1334,7 @@
         <v>7</v>
       </c>
       <c r="D53" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1936.9490725149803</v>
       </c>
     </row>
@@ -1258,7 +1349,7 @@
         <v>8</v>
       </c>
       <c r="D54" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>2130.6439797664784</v>
       </c>
     </row>
@@ -1273,7 +1364,7 @@
         <v>9</v>
       </c>
       <c r="D55" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>2343.7083777431267</v>
       </c>
     </row>
@@ -1288,7 +1379,7 @@
         <v>10</v>
       </c>
       <c r="D56" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>2578.0792155174395</v>
       </c>
     </row>
@@ -1303,7 +1394,7 @@
         <v>11</v>
       </c>
       <c r="D57" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>2835.8871370691836</v>
       </c>
     </row>
@@ -1318,7 +1409,7 @@
         <v>12</v>
       </c>
       <c r="D58" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>3119.4758507761021</v>
       </c>
     </row>
@@ -1333,7 +1424,7 @@
         <v>13</v>
       </c>
       <c r="D59" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>3431.4234358537128</v>
       </c>
     </row>
@@ -1348,7 +1439,7 @@
         <v>14</v>
       </c>
       <c r="D60" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>3774.5657794390845</v>
       </c>
     </row>
@@ -1363,7 +1454,7 @@
         <v>15</v>
       </c>
       <c r="D61" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>4152.0223573829935</v>
       </c>
     </row>
@@ -1378,7 +1469,7 @@
         <v>4</v>
       </c>
       <c r="D62" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>4567.2245931212929</v>
       </c>
     </row>
@@ -1393,7 +1484,7 @@
         <v>5</v>
       </c>
       <c r="D63" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5023.9470524334229</v>
       </c>
     </row>
@@ -1408,7 +1499,7 @@
         <v>6</v>
       </c>
       <c r="D64" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5526.3417576767652</v>
       </c>
     </row>
@@ -1423,7 +1514,7 @@
         <v>7</v>
       </c>
       <c r="D65" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>6078.9759334444425</v>
       </c>
     </row>
@@ -1438,7 +1529,7 @@
         <v>8</v>
       </c>
       <c r="D66" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>6686.8735267888869</v>
       </c>
     </row>
@@ -1453,7 +1544,7 @@
         <v>9</v>
       </c>
       <c r="D67" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>7355.5608794677764</v>
       </c>
     </row>
@@ -1468,7 +1559,7 @@
         <v>10</v>
       </c>
       <c r="D68" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>8091.1169674145549</v>
       </c>
     </row>
@@ -1483,7 +1574,7 @@
         <v>11</v>
       </c>
       <c r="D69" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>8900.2286641560113</v>
       </c>
     </row>
@@ -1498,7 +1589,7 @@
         <v>12</v>
       </c>
       <c r="D70" s="1">
-        <f t="shared" ref="D70:D97" si="1">D69*1.1</f>
+        <f t="shared" ref="D70:D97" si="4">D69*1.1</f>
         <v>9790.2515305716133</v>
       </c>
     </row>
@@ -1513,7 +1604,7 @@
         <v>13</v>
       </c>
       <c r="D71" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>10769.276683628776</v>
       </c>
     </row>
@@ -1528,7 +1619,7 @@
         <v>14</v>
       </c>
       <c r="D72" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>11846.204351991653</v>
       </c>
     </row>
@@ -1543,7 +1634,7 @@
         <v>15</v>
       </c>
       <c r="D73" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>13030.824787190819</v>
       </c>
     </row>
@@ -1558,7 +1649,7 @@
         <v>4</v>
       </c>
       <c r="D74" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>14333.907265909902</v>
       </c>
     </row>
@@ -1573,7 +1664,7 @@
         <v>5</v>
       </c>
       <c r="D75" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>15767.297992500893</v>
       </c>
     </row>
@@ -1588,7 +1679,7 @@
         <v>6</v>
       </c>
       <c r="D76" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>17344.027791750985</v>
       </c>
     </row>
@@ -1603,7 +1694,7 @@
         <v>7</v>
       </c>
       <c r="D77" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>19078.430570926084</v>
       </c>
     </row>
@@ -1618,7 +1709,7 @@
         <v>8</v>
       </c>
       <c r="D78" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>20986.273628018695</v>
       </c>
     </row>
@@ -1633,7 +1724,7 @@
         <v>9</v>
       </c>
       <c r="D79" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>23084.900990820566</v>
       </c>
     </row>
@@ -1648,7 +1739,7 @@
         <v>10</v>
       </c>
       <c r="D80" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>25393.391089902623</v>
       </c>
     </row>
@@ -1663,7 +1754,7 @@
         <v>11</v>
       </c>
       <c r="D81" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>27932.730198892888</v>
       </c>
     </row>
@@ -1678,7 +1769,7 @@
         <v>12</v>
       </c>
       <c r="D82" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>30726.003218782178</v>
       </c>
     </row>
@@ -1693,7 +1784,7 @@
         <v>13</v>
       </c>
       <c r="D83" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>33798.603540660399</v>
       </c>
     </row>
@@ -1708,7 +1799,7 @@
         <v>14</v>
       </c>
       <c r="D84" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>37178.463894726439</v>
       </c>
     </row>
@@ -1723,7 +1814,7 @@
         <v>15</v>
       </c>
       <c r="D85" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>40896.310284199084</v>
       </c>
     </row>
@@ -1738,7 +1829,7 @@
         <v>4</v>
       </c>
       <c r="D86" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>44985.941312618997</v>
       </c>
     </row>
@@ -1753,7 +1844,7 @@
         <v>5</v>
       </c>
       <c r="D87" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>49484.535443880901</v>
       </c>
     </row>
@@ -1768,7 +1859,7 @@
         <v>6</v>
       </c>
       <c r="D88" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>54432.988988268997</v>
       </c>
     </row>
@@ -1783,7 +1874,7 @@
         <v>7</v>
       </c>
       <c r="D89" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>59876.287887095903</v>
       </c>
     </row>
@@ -1798,7 +1889,7 @@
         <v>8</v>
       </c>
       <c r="D90" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>65863.916675805493</v>
       </c>
     </row>
@@ -1813,7 +1904,7 @@
         <v>9</v>
       </c>
       <c r="D91" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>72450.308343386045</v>
       </c>
     </row>
@@ -1828,7 +1919,7 @@
         <v>10</v>
       </c>
       <c r="D92" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>79695.339177724658</v>
       </c>
     </row>
@@ -1843,7 +1934,7 @@
         <v>11</v>
       </c>
       <c r="D93" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>87664.873095497125</v>
       </c>
     </row>
@@ -1858,7 +1949,7 @@
         <v>12</v>
       </c>
       <c r="D94" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>96431.360405046842</v>
       </c>
     </row>
@@ -1873,7 +1964,7 @@
         <v>13</v>
       </c>
       <c r="D95" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>106074.49644555153</v>
       </c>
     </row>
@@ -1888,7 +1979,7 @@
         <v>14</v>
       </c>
       <c r="D96" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>116681.94609010669</v>
       </c>
     </row>
@@ -1903,7 +1994,7 @@
         <v>15</v>
       </c>
       <c r="D97" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>128350.14069911737</v>
       </c>
     </row>

</xml_diff>

<commit_message>
small new post dplyr 4
</commit_message>
<xml_diff>
--- a/compounding_growth_10_percent.xlsx
+++ b/compounding_growth_10_percent.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zablotski/Library/Mobile Documents/com~apple~CloudDocs/7. Hobby/programming and stats/yuzaR-Blog/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4A56C78-8249-5643-9CFF-412CF32CE91D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A462076-15C7-0345-AA8A-6FAD7959D366}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{EDD741CF-9DB9-2945-BF15-255A1807DC69}"/>
   </bookViews>
@@ -445,8 +445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6A4B67E-A70E-FF47-86DD-9BF22E85C9FF}">
   <dimension ref="A1:I97"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="284" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="284" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -513,7 +513,7 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <f>SUM(E2:G2)</f>
+        <f>E2+G2</f>
         <v>13.65</v>
       </c>
       <c r="I2" s="1">
@@ -545,12 +545,12 @@
         <v>0</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H4" si="0">SUM(E3:G3)</f>
-        <v>28.85</v>
+        <f>E3+G3</f>
+        <v>23.92</v>
       </c>
       <c r="I3" s="1">
-        <f t="shared" ref="I3:I9" si="1">H3-D3</f>
-        <v>12.350000000000001</v>
+        <f t="shared" ref="I3:I6" si="0">H3-D3</f>
+        <v>7.4200000000000017</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -577,11 +577,11 @@
         <v>0</v>
       </c>
       <c r="H4">
+        <f>E4+G4</f>
+        <v>23.52</v>
+      </c>
+      <c r="I4" s="1">
         <f t="shared" si="0"/>
-        <v>23.52</v>
-      </c>
-      <c r="I4" s="1">
-        <f t="shared" si="1"/>
         <v>5.3699999999999974</v>
       </c>
     </row>
@@ -599,6 +599,9 @@
         <f>D4*1.1</f>
         <v>19.965000000000003</v>
       </c>
+      <c r="E5">
+        <v>24.69</v>
+      </c>
       <c r="F5">
         <v>0</v>
       </c>
@@ -606,12 +609,12 @@
         <v>19</v>
       </c>
       <c r="H5">
-        <f t="shared" ref="H5:H9" si="2">SUM(E5:G5)</f>
-        <v>19</v>
+        <f>E5+G5</f>
+        <v>43.69</v>
       </c>
       <c r="I5" s="1">
-        <f t="shared" si="1"/>
-        <v>-0.96500000000000341</v>
+        <f t="shared" si="0"/>
+        <v>23.724999999999994</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -625,10 +628,26 @@
         <v>8</v>
       </c>
       <c r="D6" s="1">
-        <f t="shared" ref="D6:D69" si="3">D5*1.1</f>
+        <f t="shared" ref="D6:D69" si="1">D5*1.1</f>
         <v>21.961500000000004</v>
       </c>
-      <c r="I6" s="1"/>
+      <c r="E6">
+        <v>9</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <f t="shared" ref="H6:H12" si="2">E6+G6</f>
+        <v>9</v>
+      </c>
+      <c r="I6" s="1">
+        <f t="shared" si="0"/>
+        <v>-12.961500000000004</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
@@ -641,7 +660,7 @@
         <v>9</v>
       </c>
       <c r="D7" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>24.157650000000007</v>
       </c>
       <c r="I7" s="1"/>
@@ -657,7 +676,7 @@
         <v>10</v>
       </c>
       <c r="D8" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>26.573415000000011</v>
       </c>
       <c r="I8" s="1"/>
@@ -673,7 +692,7 @@
         <v>11</v>
       </c>
       <c r="D9" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>29.230756500000016</v>
       </c>
       <c r="I9" s="1"/>
@@ -689,7 +708,7 @@
         <v>12</v>
       </c>
       <c r="D10" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>32.153832150000021</v>
       </c>
     </row>
@@ -704,7 +723,7 @@
         <v>13</v>
       </c>
       <c r="D11" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>35.369215365000024</v>
       </c>
     </row>
@@ -719,7 +738,7 @@
         <v>14</v>
       </c>
       <c r="D12" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>38.906136901500027</v>
       </c>
     </row>
@@ -734,7 +753,7 @@
         <v>15</v>
       </c>
       <c r="D13" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>42.796750591650031</v>
       </c>
     </row>
@@ -749,7 +768,7 @@
         <v>4</v>
       </c>
       <c r="D14" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>47.07642565081504</v>
       </c>
     </row>
@@ -764,7 +783,7 @@
         <v>5</v>
       </c>
       <c r="D15" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>51.784068215896546</v>
       </c>
     </row>
@@ -779,7 +798,7 @@
         <v>6</v>
       </c>
       <c r="D16" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>56.962475037486207</v>
       </c>
     </row>
@@ -794,7 +813,7 @@
         <v>7</v>
       </c>
       <c r="D17" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>62.65872254123483</v>
       </c>
     </row>
@@ -809,7 +828,7 @@
         <v>8</v>
       </c>
       <c r="D18" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>68.924594795358317</v>
       </c>
     </row>
@@ -824,7 +843,7 @@
         <v>9</v>
       </c>
       <c r="D19" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>75.817054274894161</v>
       </c>
     </row>
@@ -839,7 +858,7 @@
         <v>10</v>
       </c>
       <c r="D20" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>83.398759702383586</v>
       </c>
     </row>
@@ -854,7 +873,7 @@
         <v>11</v>
       </c>
       <c r="D21" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>91.738635672621953</v>
       </c>
     </row>
@@ -869,7 +888,7 @@
         <v>12</v>
       </c>
       <c r="D22" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>100.91249923988416</v>
       </c>
     </row>
@@ -884,7 +903,7 @@
         <v>13</v>
       </c>
       <c r="D23" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>111.00374916387258</v>
       </c>
     </row>
@@ -899,7 +918,7 @@
         <v>14</v>
       </c>
       <c r="D24" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>122.10412408025985</v>
       </c>
     </row>
@@ -914,7 +933,7 @@
         <v>15</v>
       </c>
       <c r="D25" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>134.31453648828585</v>
       </c>
     </row>
@@ -929,7 +948,7 @@
         <v>4</v>
       </c>
       <c r="D26" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>147.74599013711446</v>
       </c>
     </row>
@@ -944,7 +963,7 @@
         <v>5</v>
       </c>
       <c r="D27" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>162.52058915082591</v>
       </c>
     </row>
@@ -959,7 +978,7 @@
         <v>6</v>
       </c>
       <c r="D28" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>178.77264806590853</v>
       </c>
     </row>
@@ -974,7 +993,7 @@
         <v>7</v>
       </c>
       <c r="D29" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>196.64991287249939</v>
       </c>
     </row>
@@ -989,7 +1008,7 @@
         <v>8</v>
       </c>
       <c r="D30" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>216.31490415974935</v>
       </c>
     </row>
@@ -1004,7 +1023,7 @@
         <v>9</v>
       </c>
       <c r="D31" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>237.9463945757243</v>
       </c>
     </row>
@@ -1019,7 +1038,7 @@
         <v>10</v>
       </c>
       <c r="D32" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>261.74103403329673</v>
       </c>
     </row>
@@ -1034,7 +1053,7 @@
         <v>11</v>
       </c>
       <c r="D33" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>287.91513743662642</v>
       </c>
     </row>
@@ -1049,7 +1068,7 @@
         <v>12</v>
       </c>
       <c r="D34" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>316.7066511802891</v>
       </c>
     </row>
@@ -1064,7 +1083,7 @@
         <v>13</v>
       </c>
       <c r="D35" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>348.37731629831802</v>
       </c>
     </row>
@@ -1079,7 +1098,7 @@
         <v>14</v>
       </c>
       <c r="D36" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>383.21504792814983</v>
       </c>
     </row>
@@ -1094,7 +1113,7 @@
         <v>15</v>
       </c>
       <c r="D37" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>421.53655272096483</v>
       </c>
     </row>
@@ -1109,7 +1128,7 @@
         <v>4</v>
       </c>
       <c r="D38" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>463.69020799306134</v>
       </c>
     </row>
@@ -1124,7 +1143,7 @@
         <v>5</v>
       </c>
       <c r="D39" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>510.05922879236749</v>
       </c>
     </row>
@@ -1139,7 +1158,7 @@
         <v>6</v>
       </c>
       <c r="D40" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>561.06515167160433</v>
       </c>
     </row>
@@ -1154,7 +1173,7 @@
         <v>7</v>
       </c>
       <c r="D41" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>617.17166683876485</v>
       </c>
     </row>
@@ -1169,7 +1188,7 @@
         <v>8</v>
       </c>
       <c r="D42" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>678.88883352264133</v>
       </c>
     </row>
@@ -1184,7 +1203,7 @@
         <v>9</v>
       </c>
       <c r="D43" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>746.77771687490554</v>
       </c>
     </row>
@@ -1199,7 +1218,7 @@
         <v>10</v>
       </c>
       <c r="D44" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>821.45548856239611</v>
       </c>
     </row>
@@ -1214,7 +1233,7 @@
         <v>11</v>
       </c>
       <c r="D45" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>903.60103741863577</v>
       </c>
     </row>
@@ -1229,7 +1248,7 @@
         <v>12</v>
       </c>
       <c r="D46" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>993.96114116049944</v>
       </c>
     </row>
@@ -1244,7 +1263,7 @@
         <v>13</v>
       </c>
       <c r="D47" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>1093.3572552765495</v>
       </c>
     </row>
@@ -1259,7 +1278,7 @@
         <v>14</v>
       </c>
       <c r="D48" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>1202.6929808042046</v>
       </c>
     </row>
@@ -1274,7 +1293,7 @@
         <v>15</v>
       </c>
       <c r="D49" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>1322.9622788846252</v>
       </c>
     </row>
@@ -1289,7 +1308,7 @@
         <v>4</v>
       </c>
       <c r="D50" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>1455.2585067730879</v>
       </c>
     </row>
@@ -1304,7 +1323,7 @@
         <v>5</v>
       </c>
       <c r="D51" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>1600.7843574503968</v>
       </c>
     </row>
@@ -1319,7 +1338,7 @@
         <v>6</v>
       </c>
       <c r="D52" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>1760.8627931954366</v>
       </c>
     </row>
@@ -1334,7 +1353,7 @@
         <v>7</v>
       </c>
       <c r="D53" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>1936.9490725149803</v>
       </c>
     </row>
@@ -1349,7 +1368,7 @@
         <v>8</v>
       </c>
       <c r="D54" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>2130.6439797664784</v>
       </c>
     </row>
@@ -1364,7 +1383,7 @@
         <v>9</v>
       </c>
       <c r="D55" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>2343.7083777431267</v>
       </c>
     </row>
@@ -1379,7 +1398,7 @@
         <v>10</v>
       </c>
       <c r="D56" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>2578.0792155174395</v>
       </c>
     </row>
@@ -1394,7 +1413,7 @@
         <v>11</v>
       </c>
       <c r="D57" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>2835.8871370691836</v>
       </c>
     </row>
@@ -1409,7 +1428,7 @@
         <v>12</v>
       </c>
       <c r="D58" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>3119.4758507761021</v>
       </c>
     </row>
@@ -1424,7 +1443,7 @@
         <v>13</v>
       </c>
       <c r="D59" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>3431.4234358537128</v>
       </c>
     </row>
@@ -1439,7 +1458,7 @@
         <v>14</v>
       </c>
       <c r="D60" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>3774.5657794390845</v>
       </c>
     </row>
@@ -1454,7 +1473,7 @@
         <v>15</v>
       </c>
       <c r="D61" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>4152.0223573829935</v>
       </c>
     </row>
@@ -1469,7 +1488,7 @@
         <v>4</v>
       </c>
       <c r="D62" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>4567.2245931212929</v>
       </c>
     </row>
@@ -1484,7 +1503,7 @@
         <v>5</v>
       </c>
       <c r="D63" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>5023.9470524334229</v>
       </c>
     </row>
@@ -1499,7 +1518,7 @@
         <v>6</v>
       </c>
       <c r="D64" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>5526.3417576767652</v>
       </c>
     </row>
@@ -1514,7 +1533,7 @@
         <v>7</v>
       </c>
       <c r="D65" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>6078.9759334444425</v>
       </c>
     </row>
@@ -1529,7 +1548,7 @@
         <v>8</v>
       </c>
       <c r="D66" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>6686.8735267888869</v>
       </c>
     </row>
@@ -1544,7 +1563,7 @@
         <v>9</v>
       </c>
       <c r="D67" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>7355.5608794677764</v>
       </c>
     </row>
@@ -1559,7 +1578,7 @@
         <v>10</v>
       </c>
       <c r="D68" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>8091.1169674145549</v>
       </c>
     </row>
@@ -1574,7 +1593,7 @@
         <v>11</v>
       </c>
       <c r="D69" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>8900.2286641560113</v>
       </c>
     </row>
@@ -1589,7 +1608,7 @@
         <v>12</v>
       </c>
       <c r="D70" s="1">
-        <f t="shared" ref="D70:D97" si="4">D69*1.1</f>
+        <f t="shared" ref="D70:D97" si="3">D69*1.1</f>
         <v>9790.2515305716133</v>
       </c>
     </row>
@@ -1604,7 +1623,7 @@
         <v>13</v>
       </c>
       <c r="D71" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>10769.276683628776</v>
       </c>
     </row>
@@ -1619,7 +1638,7 @@
         <v>14</v>
       </c>
       <c r="D72" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>11846.204351991653</v>
       </c>
     </row>
@@ -1634,7 +1653,7 @@
         <v>15</v>
       </c>
       <c r="D73" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>13030.824787190819</v>
       </c>
     </row>
@@ -1649,7 +1668,7 @@
         <v>4</v>
       </c>
       <c r="D74" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>14333.907265909902</v>
       </c>
     </row>
@@ -1664,7 +1683,7 @@
         <v>5</v>
       </c>
       <c r="D75" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>15767.297992500893</v>
       </c>
     </row>
@@ -1679,7 +1698,7 @@
         <v>6</v>
       </c>
       <c r="D76" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>17344.027791750985</v>
       </c>
     </row>
@@ -1694,7 +1713,7 @@
         <v>7</v>
       </c>
       <c r="D77" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>19078.430570926084</v>
       </c>
     </row>
@@ -1709,7 +1728,7 @@
         <v>8</v>
       </c>
       <c r="D78" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>20986.273628018695</v>
       </c>
     </row>
@@ -1724,7 +1743,7 @@
         <v>9</v>
       </c>
       <c r="D79" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>23084.900990820566</v>
       </c>
     </row>
@@ -1739,7 +1758,7 @@
         <v>10</v>
       </c>
       <c r="D80" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>25393.391089902623</v>
       </c>
     </row>
@@ -1754,7 +1773,7 @@
         <v>11</v>
       </c>
       <c r="D81" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>27932.730198892888</v>
       </c>
     </row>
@@ -1769,7 +1788,7 @@
         <v>12</v>
       </c>
       <c r="D82" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>30726.003218782178</v>
       </c>
     </row>
@@ -1784,7 +1803,7 @@
         <v>13</v>
       </c>
       <c r="D83" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>33798.603540660399</v>
       </c>
     </row>
@@ -1799,7 +1818,7 @@
         <v>14</v>
       </c>
       <c r="D84" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>37178.463894726439</v>
       </c>
     </row>
@@ -1814,7 +1833,7 @@
         <v>15</v>
       </c>
       <c r="D85" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>40896.310284199084</v>
       </c>
     </row>
@@ -1829,7 +1848,7 @@
         <v>4</v>
       </c>
       <c r="D86" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>44985.941312618997</v>
       </c>
     </row>
@@ -1844,7 +1863,7 @@
         <v>5</v>
       </c>
       <c r="D87" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>49484.535443880901</v>
       </c>
     </row>
@@ -1859,7 +1878,7 @@
         <v>6</v>
       </c>
       <c r="D88" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>54432.988988268997</v>
       </c>
     </row>
@@ -1874,7 +1893,7 @@
         <v>7</v>
       </c>
       <c r="D89" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>59876.287887095903</v>
       </c>
     </row>
@@ -1889,7 +1908,7 @@
         <v>8</v>
       </c>
       <c r="D90" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>65863.916675805493</v>
       </c>
     </row>
@@ -1904,7 +1923,7 @@
         <v>9</v>
       </c>
       <c r="D91" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>72450.308343386045</v>
       </c>
     </row>
@@ -1919,7 +1938,7 @@
         <v>10</v>
       </c>
       <c r="D92" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>79695.339177724658</v>
       </c>
     </row>
@@ -1934,7 +1953,7 @@
         <v>11</v>
       </c>
       <c r="D93" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>87664.873095497125</v>
       </c>
     </row>
@@ -1949,7 +1968,7 @@
         <v>12</v>
       </c>
       <c r="D94" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>96431.360405046842</v>
       </c>
     </row>
@@ -1964,7 +1983,7 @@
         <v>13</v>
       </c>
       <c r="D95" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>106074.49644555153</v>
       </c>
     </row>
@@ -1979,7 +1998,7 @@
         <v>14</v>
       </c>
       <c r="D96" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>116681.94609010669</v>
       </c>
     </row>
@@ -1994,7 +2013,7 @@
         <v>15</v>
       </c>
       <c r="D97" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>128350.14069911737</v>
       </c>
     </row>

</xml_diff>

<commit_message>
just small in between commit
</commit_message>
<xml_diff>
--- a/compounding_growth_10_percent.xlsx
+++ b/compounding_growth_10_percent.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zablotski/Library/Mobile Documents/com~apple~CloudDocs/7. Hobby/programming and stats/yuzaR-Blog/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A462076-15C7-0345-AA8A-6FAD7959D366}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BE0C5B9-0E11-C64C-8708-A1885911643B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{EDD741CF-9DB9-2945-BF15-255A1807DC69}"/>
   </bookViews>
@@ -446,7 +446,7 @@
   <dimension ref="A1:I97"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="284" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -549,7 +549,7 @@
         <v>23.92</v>
       </c>
       <c r="I3" s="1">
-        <f t="shared" ref="I3:I6" si="0">H3-D3</f>
+        <f t="shared" ref="I3:I7" si="0">H3-D3</f>
         <v>7.4200000000000017</v>
       </c>
     </row>
@@ -632,7 +632,7 @@
         <v>21.961500000000004</v>
       </c>
       <c r="E6">
-        <v>9</v>
+        <v>25.93</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -641,12 +641,12 @@
         <v>0</v>
       </c>
       <c r="H6">
-        <f t="shared" ref="H6:H12" si="2">E6+G6</f>
-        <v>9</v>
+        <f t="shared" ref="H6:H7" si="2">E6+G6</f>
+        <v>25.93</v>
       </c>
       <c r="I6" s="1">
         <f t="shared" si="0"/>
-        <v>-12.961500000000004</v>
+        <v>3.9684999999999953</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -663,7 +663,20 @@
         <f t="shared" si="1"/>
         <v>24.157650000000007</v>
       </c>
-      <c r="I7" s="1"/>
+      <c r="E7">
+        <v>0.86</v>
+      </c>
+      <c r="G7">
+        <v>9.5</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="2"/>
+        <v>10.36</v>
+      </c>
+      <c r="I7" s="1">
+        <f t="shared" si="0"/>
+        <v>-13.797650000000008</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">

</xml_diff>

<commit_message>
new post dplyr on steroids
</commit_message>
<xml_diff>
--- a/compounding_growth_10_percent.xlsx
+++ b/compounding_growth_10_percent.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zablotski/Library/Mobile Documents/com~apple~CloudDocs/7. Hobby/programming and stats/yuzaR-Blog/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BE0C5B9-0E11-C64C-8708-A1885911643B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C615346-10D0-A14D-89BC-B8E9266F1463}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{EDD741CF-9DB9-2945-BF15-255A1807DC69}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="22">
   <si>
     <t>year</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>difference</t>
+  </si>
+  <si>
+    <t>Consulting</t>
   </si>
 </sst>
 </file>
@@ -443,10 +446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6A4B67E-A70E-FF47-86DD-9BF22E85C9FF}">
-  <dimension ref="A1:I97"/>
+  <dimension ref="A1:J97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="284" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" zoomScale="284" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -458,10 +461,11 @@
     <col min="5" max="5" width="6.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" customWidth="1"/>
+    <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -484,13 +488,16 @@
         <v>18</v>
       </c>
       <c r="H1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" t="s">
         <v>19</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -513,15 +520,18 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <f>E2+G2</f>
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <f>E2+F2+G2+H2</f>
         <v>13.65</v>
       </c>
-      <c r="I2" s="1">
-        <f>H2-D2</f>
+      <c r="J2" s="1">
+        <f>I2-D2</f>
         <v>-1.3499999999999996</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -545,15 +555,18 @@
         <v>0</v>
       </c>
       <c r="H3">
-        <f>E3+G3</f>
-        <v>23.92</v>
-      </c>
-      <c r="I3" s="1">
-        <f t="shared" ref="I3:I7" si="0">H3-D3</f>
-        <v>7.4200000000000017</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I13" si="0">E3+F3+G3+H3</f>
+        <v>28.85</v>
+      </c>
+      <c r="J3" s="1">
+        <f t="shared" ref="J3:J4" si="1">I3-D3</f>
+        <v>12.350000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -577,15 +590,18 @@
         <v>0</v>
       </c>
       <c r="H4">
-        <f>E4+G4</f>
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="0"/>
         <v>23.52</v>
       </c>
-      <c r="I4" s="1">
-        <f t="shared" si="0"/>
+      <c r="J4" s="1">
+        <f t="shared" si="1"/>
         <v>5.3699999999999974</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -609,15 +625,18 @@
         <v>19</v>
       </c>
       <c r="H5">
-        <f>E5+G5</f>
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="0"/>
         <v>43.69</v>
       </c>
-      <c r="I5" s="1">
-        <f t="shared" si="0"/>
+      <c r="J5" s="1">
+        <f>I5-D5</f>
         <v>23.724999999999994</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -628,7 +647,7 @@
         <v>8</v>
       </c>
       <c r="D6" s="1">
-        <f t="shared" ref="D6:D69" si="1">D5*1.1</f>
+        <f t="shared" ref="D6:D69" si="2">D5*1.1</f>
         <v>21.961500000000004</v>
       </c>
       <c r="E6">
@@ -641,15 +660,18 @@
         <v>0</v>
       </c>
       <c r="H6">
-        <f t="shared" ref="H6:H7" si="2">E6+G6</f>
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="0"/>
         <v>25.93</v>
       </c>
-      <c r="I6" s="1">
-        <f t="shared" si="0"/>
+      <c r="J6" s="1">
+        <f>I6-D6</f>
         <v>3.9684999999999953</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -660,25 +682,31 @@
         <v>9</v>
       </c>
       <c r="D7" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>24.157650000000007</v>
       </c>
       <c r="E7">
-        <v>0.86</v>
+        <v>19.05</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
       </c>
       <c r="G7">
         <v>9.5</v>
       </c>
       <c r="H7">
-        <f t="shared" si="2"/>
-        <v>10.36</v>
-      </c>
-      <c r="I7" s="1">
+        <v>250</v>
+      </c>
+      <c r="I7">
         <f t="shared" si="0"/>
-        <v>-13.797650000000008</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+        <v>278.55</v>
+      </c>
+      <c r="J7" s="1">
+        <f>I7-D7</f>
+        <v>254.39234999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -689,12 +717,22 @@
         <v>10</v>
       </c>
       <c r="D8" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>26.573415000000011</v>
       </c>
-      <c r="I8" s="1"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J8" s="1">
+        <f t="shared" ref="J8:J13" si="3">I8-D8</f>
+        <v>-26.573415000000011</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -705,12 +743,22 @@
         <v>11</v>
       </c>
       <c r="D9" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>29.230756500000016</v>
       </c>
-      <c r="I9" s="1"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J9" s="1">
+        <f t="shared" si="3"/>
+        <v>-29.230756500000016</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -721,11 +769,22 @@
         <v>12</v>
       </c>
       <c r="D10" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>32.153832150000021</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J10" s="1">
+        <f t="shared" si="3"/>
+        <v>-32.153832150000021</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -736,11 +795,22 @@
         <v>13</v>
       </c>
       <c r="D11" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>35.369215365000024</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J11" s="1">
+        <f t="shared" si="3"/>
+        <v>-35.369215365000024</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -751,11 +821,22 @@
         <v>14</v>
       </c>
       <c r="D12" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>38.906136901500027</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J12" s="1">
+        <f t="shared" si="3"/>
+        <v>-38.906136901500027</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -766,11 +847,22 @@
         <v>15</v>
       </c>
       <c r="D13" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>42.796750591650031</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J13" s="1">
+        <f t="shared" si="3"/>
+        <v>-42.796750591650031</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -781,11 +873,11 @@
         <v>4</v>
       </c>
       <c r="D14" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>47.07642565081504</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -796,11 +888,11 @@
         <v>5</v>
       </c>
       <c r="D15" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>51.784068215896546</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -811,7 +903,7 @@
         <v>6</v>
       </c>
       <c r="D16" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>56.962475037486207</v>
       </c>
     </row>
@@ -826,7 +918,7 @@
         <v>7</v>
       </c>
       <c r="D17" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>62.65872254123483</v>
       </c>
     </row>
@@ -841,7 +933,7 @@
         <v>8</v>
       </c>
       <c r="D18" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>68.924594795358317</v>
       </c>
     </row>
@@ -856,7 +948,7 @@
         <v>9</v>
       </c>
       <c r="D19" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>75.817054274894161</v>
       </c>
     </row>
@@ -871,7 +963,7 @@
         <v>10</v>
       </c>
       <c r="D20" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>83.398759702383586</v>
       </c>
     </row>
@@ -886,7 +978,7 @@
         <v>11</v>
       </c>
       <c r="D21" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>91.738635672621953</v>
       </c>
     </row>
@@ -901,7 +993,7 @@
         <v>12</v>
       </c>
       <c r="D22" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>100.91249923988416</v>
       </c>
     </row>
@@ -916,7 +1008,7 @@
         <v>13</v>
       </c>
       <c r="D23" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>111.00374916387258</v>
       </c>
     </row>
@@ -931,7 +1023,7 @@
         <v>14</v>
       </c>
       <c r="D24" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>122.10412408025985</v>
       </c>
     </row>
@@ -946,7 +1038,7 @@
         <v>15</v>
       </c>
       <c r="D25" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>134.31453648828585</v>
       </c>
     </row>
@@ -961,7 +1053,7 @@
         <v>4</v>
       </c>
       <c r="D26" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>147.74599013711446</v>
       </c>
     </row>
@@ -976,7 +1068,7 @@
         <v>5</v>
       </c>
       <c r="D27" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>162.52058915082591</v>
       </c>
     </row>
@@ -991,7 +1083,7 @@
         <v>6</v>
       </c>
       <c r="D28" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>178.77264806590853</v>
       </c>
     </row>
@@ -1006,7 +1098,7 @@
         <v>7</v>
       </c>
       <c r="D29" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>196.64991287249939</v>
       </c>
     </row>
@@ -1021,7 +1113,7 @@
         <v>8</v>
       </c>
       <c r="D30" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>216.31490415974935</v>
       </c>
     </row>
@@ -1036,7 +1128,7 @@
         <v>9</v>
       </c>
       <c r="D31" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>237.9463945757243</v>
       </c>
     </row>
@@ -1051,7 +1143,7 @@
         <v>10</v>
       </c>
       <c r="D32" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>261.74103403329673</v>
       </c>
     </row>
@@ -1066,7 +1158,7 @@
         <v>11</v>
       </c>
       <c r="D33" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>287.91513743662642</v>
       </c>
     </row>
@@ -1081,7 +1173,7 @@
         <v>12</v>
       </c>
       <c r="D34" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>316.7066511802891</v>
       </c>
     </row>
@@ -1096,7 +1188,7 @@
         <v>13</v>
       </c>
       <c r="D35" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>348.37731629831802</v>
       </c>
     </row>
@@ -1111,7 +1203,7 @@
         <v>14</v>
       </c>
       <c r="D36" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>383.21504792814983</v>
       </c>
     </row>
@@ -1126,7 +1218,7 @@
         <v>15</v>
       </c>
       <c r="D37" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>421.53655272096483</v>
       </c>
     </row>
@@ -1141,7 +1233,7 @@
         <v>4</v>
       </c>
       <c r="D38" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>463.69020799306134</v>
       </c>
     </row>
@@ -1156,7 +1248,7 @@
         <v>5</v>
       </c>
       <c r="D39" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>510.05922879236749</v>
       </c>
     </row>
@@ -1171,7 +1263,7 @@
         <v>6</v>
       </c>
       <c r="D40" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>561.06515167160433</v>
       </c>
     </row>
@@ -1186,7 +1278,7 @@
         <v>7</v>
       </c>
       <c r="D41" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>617.17166683876485</v>
       </c>
     </row>
@@ -1201,7 +1293,7 @@
         <v>8</v>
       </c>
       <c r="D42" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>678.88883352264133</v>
       </c>
     </row>
@@ -1216,7 +1308,7 @@
         <v>9</v>
       </c>
       <c r="D43" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>746.77771687490554</v>
       </c>
     </row>
@@ -1231,7 +1323,7 @@
         <v>10</v>
       </c>
       <c r="D44" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>821.45548856239611</v>
       </c>
     </row>
@@ -1246,7 +1338,7 @@
         <v>11</v>
       </c>
       <c r="D45" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>903.60103741863577</v>
       </c>
     </row>
@@ -1261,7 +1353,7 @@
         <v>12</v>
       </c>
       <c r="D46" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>993.96114116049944</v>
       </c>
     </row>
@@ -1276,7 +1368,7 @@
         <v>13</v>
       </c>
       <c r="D47" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1093.3572552765495</v>
       </c>
     </row>
@@ -1291,7 +1383,7 @@
         <v>14</v>
       </c>
       <c r="D48" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1202.6929808042046</v>
       </c>
     </row>
@@ -1306,7 +1398,7 @@
         <v>15</v>
       </c>
       <c r="D49" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1322.9622788846252</v>
       </c>
     </row>
@@ -1321,7 +1413,7 @@
         <v>4</v>
       </c>
       <c r="D50" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1455.2585067730879</v>
       </c>
     </row>
@@ -1336,7 +1428,7 @@
         <v>5</v>
       </c>
       <c r="D51" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1600.7843574503968</v>
       </c>
     </row>
@@ -1351,7 +1443,7 @@
         <v>6</v>
       </c>
       <c r="D52" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1760.8627931954366</v>
       </c>
     </row>
@@ -1366,7 +1458,7 @@
         <v>7</v>
       </c>
       <c r="D53" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1936.9490725149803</v>
       </c>
     </row>
@@ -1381,7 +1473,7 @@
         <v>8</v>
       </c>
       <c r="D54" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2130.6439797664784</v>
       </c>
     </row>
@@ -1396,7 +1488,7 @@
         <v>9</v>
       </c>
       <c r="D55" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2343.7083777431267</v>
       </c>
     </row>
@@ -1411,7 +1503,7 @@
         <v>10</v>
       </c>
       <c r="D56" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2578.0792155174395</v>
       </c>
     </row>
@@ -1426,7 +1518,7 @@
         <v>11</v>
       </c>
       <c r="D57" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2835.8871370691836</v>
       </c>
     </row>
@@ -1441,7 +1533,7 @@
         <v>12</v>
       </c>
       <c r="D58" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3119.4758507761021</v>
       </c>
     </row>
@@ -1456,7 +1548,7 @@
         <v>13</v>
       </c>
       <c r="D59" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3431.4234358537128</v>
       </c>
     </row>
@@ -1471,7 +1563,7 @@
         <v>14</v>
       </c>
       <c r="D60" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3774.5657794390845</v>
       </c>
     </row>
@@ -1486,7 +1578,7 @@
         <v>15</v>
       </c>
       <c r="D61" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4152.0223573829935</v>
       </c>
     </row>
@@ -1501,7 +1593,7 @@
         <v>4</v>
       </c>
       <c r="D62" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4567.2245931212929</v>
       </c>
     </row>
@@ -1516,7 +1608,7 @@
         <v>5</v>
       </c>
       <c r="D63" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5023.9470524334229</v>
       </c>
     </row>
@@ -1531,7 +1623,7 @@
         <v>6</v>
       </c>
       <c r="D64" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5526.3417576767652</v>
       </c>
     </row>
@@ -1546,7 +1638,7 @@
         <v>7</v>
       </c>
       <c r="D65" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6078.9759334444425</v>
       </c>
     </row>
@@ -1561,7 +1653,7 @@
         <v>8</v>
       </c>
       <c r="D66" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6686.8735267888869</v>
       </c>
     </row>
@@ -1576,7 +1668,7 @@
         <v>9</v>
       </c>
       <c r="D67" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7355.5608794677764</v>
       </c>
     </row>
@@ -1591,7 +1683,7 @@
         <v>10</v>
       </c>
       <c r="D68" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8091.1169674145549</v>
       </c>
     </row>
@@ -1606,7 +1698,7 @@
         <v>11</v>
       </c>
       <c r="D69" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8900.2286641560113</v>
       </c>
     </row>
@@ -1621,7 +1713,7 @@
         <v>12</v>
       </c>
       <c r="D70" s="1">
-        <f t="shared" ref="D70:D97" si="3">D69*1.1</f>
+        <f t="shared" ref="D70:D97" si="4">D69*1.1</f>
         <v>9790.2515305716133</v>
       </c>
     </row>
@@ -1636,7 +1728,7 @@
         <v>13</v>
       </c>
       <c r="D71" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>10769.276683628776</v>
       </c>
     </row>
@@ -1651,7 +1743,7 @@
         <v>14</v>
       </c>
       <c r="D72" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>11846.204351991653</v>
       </c>
     </row>
@@ -1666,7 +1758,7 @@
         <v>15</v>
       </c>
       <c r="D73" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>13030.824787190819</v>
       </c>
     </row>
@@ -1681,7 +1773,7 @@
         <v>4</v>
       </c>
       <c r="D74" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>14333.907265909902</v>
       </c>
     </row>
@@ -1696,7 +1788,7 @@
         <v>5</v>
       </c>
       <c r="D75" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>15767.297992500893</v>
       </c>
     </row>
@@ -1711,7 +1803,7 @@
         <v>6</v>
       </c>
       <c r="D76" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>17344.027791750985</v>
       </c>
     </row>
@@ -1726,7 +1818,7 @@
         <v>7</v>
       </c>
       <c r="D77" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>19078.430570926084</v>
       </c>
     </row>
@@ -1741,7 +1833,7 @@
         <v>8</v>
       </c>
       <c r="D78" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>20986.273628018695</v>
       </c>
     </row>
@@ -1756,7 +1848,7 @@
         <v>9</v>
       </c>
       <c r="D79" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>23084.900990820566</v>
       </c>
     </row>
@@ -1771,7 +1863,7 @@
         <v>10</v>
       </c>
       <c r="D80" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>25393.391089902623</v>
       </c>
     </row>
@@ -1786,7 +1878,7 @@
         <v>11</v>
       </c>
       <c r="D81" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>27932.730198892888</v>
       </c>
     </row>
@@ -1801,7 +1893,7 @@
         <v>12</v>
       </c>
       <c r="D82" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>30726.003218782178</v>
       </c>
     </row>
@@ -1816,7 +1908,7 @@
         <v>13</v>
       </c>
       <c r="D83" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>33798.603540660399</v>
       </c>
     </row>
@@ -1831,7 +1923,7 @@
         <v>14</v>
       </c>
       <c r="D84" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>37178.463894726439</v>
       </c>
     </row>
@@ -1846,7 +1938,7 @@
         <v>15</v>
       </c>
       <c r="D85" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>40896.310284199084</v>
       </c>
     </row>
@@ -1861,7 +1953,7 @@
         <v>4</v>
       </c>
       <c r="D86" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>44985.941312618997</v>
       </c>
     </row>
@@ -1876,7 +1968,7 @@
         <v>5</v>
       </c>
       <c r="D87" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>49484.535443880901</v>
       </c>
     </row>
@@ -1891,7 +1983,7 @@
         <v>6</v>
       </c>
       <c r="D88" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>54432.988988268997</v>
       </c>
     </row>
@@ -1906,7 +1998,7 @@
         <v>7</v>
       </c>
       <c r="D89" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>59876.287887095903</v>
       </c>
     </row>
@@ -1921,7 +2013,7 @@
         <v>8</v>
       </c>
       <c r="D90" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>65863.916675805493</v>
       </c>
     </row>
@@ -1936,7 +2028,7 @@
         <v>9</v>
       </c>
       <c r="D91" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>72450.308343386045</v>
       </c>
     </row>
@@ -1951,7 +2043,7 @@
         <v>10</v>
       </c>
       <c r="D92" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>79695.339177724658</v>
       </c>
     </row>
@@ -1966,7 +2058,7 @@
         <v>11</v>
       </c>
       <c r="D93" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>87664.873095497125</v>
       </c>
     </row>
@@ -1981,7 +2073,7 @@
         <v>12</v>
       </c>
       <c r="D94" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>96431.360405046842</v>
       </c>
     </row>
@@ -1996,7 +2088,7 @@
         <v>13</v>
       </c>
       <c r="D95" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>106074.49644555153</v>
       </c>
     </row>
@@ -2011,7 +2103,7 @@
         <v>14</v>
       </c>
       <c r="D96" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>116681.94609010669</v>
       </c>
     </row>
@@ -2026,7 +2118,7 @@
         <v>15</v>
       </c>
       <c r="D97" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>128350.14069911737</v>
       </c>
     </row>

</xml_diff>

<commit_message>
data wringling 4 small update
</commit_message>
<xml_diff>
--- a/compounding_growth_10_percent.xlsx
+++ b/compounding_growth_10_percent.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zablotski/Library/Mobile Documents/com~apple~CloudDocs/7. Hobby/programming and stats/yuzaR-Blog/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C615346-10D0-A14D-89BC-B8E9266F1463}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F13994C-BDD3-ED4E-A566-8949210E86B3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{EDD741CF-9DB9-2945-BF15-255A1807DC69}"/>
   </bookViews>
@@ -34,9 +34,6 @@
   </si>
   <si>
     <t>projected</t>
-  </si>
-  <si>
-    <t>earned</t>
   </si>
   <si>
     <t>Jan</t>
@@ -91,6 +88,9 @@
   </si>
   <si>
     <t>Consulting</t>
+  </si>
+  <si>
+    <t>adds</t>
   </si>
 </sst>
 </file>
@@ -449,7 +449,7 @@
   <dimension ref="A1:J97"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="284" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -467,7 +467,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -479,22 +479,22 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
         <v>17</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" t="s">
         <v>18</v>
       </c>
-      <c r="H1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>19</v>
-      </c>
-      <c r="J1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -505,7 +505,7 @@
         <v>2023</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D2" s="1">
         <v>15</v>
@@ -539,7 +539,7 @@
         <v>2023</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D3" s="1">
         <f>D2*1.1</f>
@@ -574,7 +574,7 @@
         <v>2023</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D4" s="1">
         <f>D3*1.1</f>
@@ -609,7 +609,7 @@
         <v>2023</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D5" s="1">
         <f>D4*1.1</f>
@@ -644,7 +644,7 @@
         <v>2023</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6" s="1">
         <f t="shared" ref="D6:D69" si="2">D5*1.1</f>
@@ -679,14 +679,14 @@
         <v>2023</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D7" s="1">
         <f t="shared" si="2"/>
         <v>24.157650000000007</v>
       </c>
       <c r="E7">
-        <v>19.05</v>
+        <v>22.96</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -699,11 +699,11 @@
       </c>
       <c r="I7">
         <f t="shared" si="0"/>
-        <v>278.55</v>
+        <v>282.45999999999998</v>
       </c>
       <c r="J7" s="1">
         <f>I7-D7</f>
-        <v>254.39234999999999</v>
+        <v>258.30234999999999</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -714,7 +714,7 @@
         <v>2023</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D8" s="1">
         <f t="shared" si="2"/>
@@ -740,7 +740,7 @@
         <v>2023</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D9" s="1">
         <f t="shared" si="2"/>
@@ -766,7 +766,7 @@
         <v>2023</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D10" s="1">
         <f t="shared" si="2"/>
@@ -792,7 +792,7 @@
         <v>2023</v>
       </c>
       <c r="C11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D11" s="1">
         <f t="shared" si="2"/>
@@ -818,7 +818,7 @@
         <v>2023</v>
       </c>
       <c r="C12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D12" s="1">
         <f t="shared" si="2"/>
@@ -844,7 +844,7 @@
         <v>2023</v>
       </c>
       <c r="C13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D13" s="1">
         <f t="shared" si="2"/>
@@ -870,7 +870,7 @@
         <v>2024</v>
       </c>
       <c r="C14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D14" s="1">
         <f t="shared" si="2"/>
@@ -885,7 +885,7 @@
         <v>2024</v>
       </c>
       <c r="C15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D15" s="1">
         <f t="shared" si="2"/>
@@ -900,7 +900,7 @@
         <v>2024</v>
       </c>
       <c r="C16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D16" s="1">
         <f t="shared" si="2"/>
@@ -915,7 +915,7 @@
         <v>2024</v>
       </c>
       <c r="C17" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D17" s="1">
         <f t="shared" si="2"/>
@@ -930,7 +930,7 @@
         <v>2024</v>
       </c>
       <c r="C18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D18" s="1">
         <f t="shared" si="2"/>
@@ -945,7 +945,7 @@
         <v>2024</v>
       </c>
       <c r="C19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D19" s="1">
         <f t="shared" si="2"/>
@@ -960,7 +960,7 @@
         <v>2024</v>
       </c>
       <c r="C20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D20" s="1">
         <f t="shared" si="2"/>
@@ -975,7 +975,7 @@
         <v>2024</v>
       </c>
       <c r="C21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D21" s="1">
         <f t="shared" si="2"/>
@@ -990,7 +990,7 @@
         <v>2024</v>
       </c>
       <c r="C22" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D22" s="1">
         <f t="shared" si="2"/>
@@ -1005,7 +1005,7 @@
         <v>2024</v>
       </c>
       <c r="C23" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D23" s="1">
         <f t="shared" si="2"/>
@@ -1020,7 +1020,7 @@
         <v>2024</v>
       </c>
       <c r="C24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D24" s="1">
         <f t="shared" si="2"/>
@@ -1035,7 +1035,7 @@
         <v>2024</v>
       </c>
       <c r="C25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D25" s="1">
         <f t="shared" si="2"/>
@@ -1050,7 +1050,7 @@
         <v>2025</v>
       </c>
       <c r="C26" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D26" s="1">
         <f t="shared" si="2"/>
@@ -1065,7 +1065,7 @@
         <v>2025</v>
       </c>
       <c r="C27" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D27" s="1">
         <f t="shared" si="2"/>
@@ -1080,7 +1080,7 @@
         <v>2025</v>
       </c>
       <c r="C28" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D28" s="1">
         <f t="shared" si="2"/>
@@ -1095,7 +1095,7 @@
         <v>2025</v>
       </c>
       <c r="C29" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D29" s="1">
         <f t="shared" si="2"/>
@@ -1110,7 +1110,7 @@
         <v>2025</v>
       </c>
       <c r="C30" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D30" s="1">
         <f t="shared" si="2"/>
@@ -1125,7 +1125,7 @@
         <v>2025</v>
       </c>
       <c r="C31" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D31" s="1">
         <f t="shared" si="2"/>
@@ -1140,7 +1140,7 @@
         <v>2025</v>
       </c>
       <c r="C32" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D32" s="1">
         <f t="shared" si="2"/>
@@ -1155,7 +1155,7 @@
         <v>2025</v>
       </c>
       <c r="C33" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D33" s="1">
         <f t="shared" si="2"/>
@@ -1170,7 +1170,7 @@
         <v>2025</v>
       </c>
       <c r="C34" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D34" s="1">
         <f t="shared" si="2"/>
@@ -1185,7 +1185,7 @@
         <v>2025</v>
       </c>
       <c r="C35" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D35" s="1">
         <f t="shared" si="2"/>
@@ -1200,7 +1200,7 @@
         <v>2025</v>
       </c>
       <c r="C36" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D36" s="1">
         <f t="shared" si="2"/>
@@ -1215,7 +1215,7 @@
         <v>2025</v>
       </c>
       <c r="C37" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D37" s="1">
         <f t="shared" si="2"/>
@@ -1230,7 +1230,7 @@
         <v>2026</v>
       </c>
       <c r="C38" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D38" s="1">
         <f t="shared" si="2"/>
@@ -1245,7 +1245,7 @@
         <v>2026</v>
       </c>
       <c r="C39" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D39" s="1">
         <f t="shared" si="2"/>
@@ -1260,7 +1260,7 @@
         <v>2026</v>
       </c>
       <c r="C40" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D40" s="1">
         <f t="shared" si="2"/>
@@ -1275,7 +1275,7 @@
         <v>2026</v>
       </c>
       <c r="C41" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D41" s="1">
         <f t="shared" si="2"/>
@@ -1290,7 +1290,7 @@
         <v>2026</v>
       </c>
       <c r="C42" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D42" s="1">
         <f t="shared" si="2"/>
@@ -1305,7 +1305,7 @@
         <v>2026</v>
       </c>
       <c r="C43" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D43" s="1">
         <f t="shared" si="2"/>
@@ -1320,7 +1320,7 @@
         <v>2026</v>
       </c>
       <c r="C44" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D44" s="1">
         <f t="shared" si="2"/>
@@ -1335,7 +1335,7 @@
         <v>2026</v>
       </c>
       <c r="C45" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D45" s="1">
         <f t="shared" si="2"/>
@@ -1350,7 +1350,7 @@
         <v>2026</v>
       </c>
       <c r="C46" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D46" s="1">
         <f t="shared" si="2"/>
@@ -1365,7 +1365,7 @@
         <v>2026</v>
       </c>
       <c r="C47" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D47" s="1">
         <f t="shared" si="2"/>
@@ -1380,7 +1380,7 @@
         <v>2026</v>
       </c>
       <c r="C48" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D48" s="1">
         <f t="shared" si="2"/>
@@ -1395,7 +1395,7 @@
         <v>2026</v>
       </c>
       <c r="C49" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D49" s="1">
         <f t="shared" si="2"/>
@@ -1410,7 +1410,7 @@
         <v>2027</v>
       </c>
       <c r="C50" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D50" s="1">
         <f t="shared" si="2"/>
@@ -1425,7 +1425,7 @@
         <v>2027</v>
       </c>
       <c r="C51" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D51" s="1">
         <f t="shared" si="2"/>
@@ -1440,7 +1440,7 @@
         <v>2027</v>
       </c>
       <c r="C52" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D52" s="1">
         <f t="shared" si="2"/>
@@ -1455,7 +1455,7 @@
         <v>2027</v>
       </c>
       <c r="C53" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D53" s="1">
         <f t="shared" si="2"/>
@@ -1470,7 +1470,7 @@
         <v>2027</v>
       </c>
       <c r="C54" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D54" s="1">
         <f t="shared" si="2"/>
@@ -1485,7 +1485,7 @@
         <v>2027</v>
       </c>
       <c r="C55" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D55" s="1">
         <f t="shared" si="2"/>
@@ -1500,7 +1500,7 @@
         <v>2027</v>
       </c>
       <c r="C56" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D56" s="1">
         <f t="shared" si="2"/>
@@ -1515,7 +1515,7 @@
         <v>2027</v>
       </c>
       <c r="C57" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D57" s="1">
         <f t="shared" si="2"/>
@@ -1530,7 +1530,7 @@
         <v>2027</v>
       </c>
       <c r="C58" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D58" s="1">
         <f t="shared" si="2"/>
@@ -1545,7 +1545,7 @@
         <v>2027</v>
       </c>
       <c r="C59" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D59" s="1">
         <f t="shared" si="2"/>
@@ -1560,7 +1560,7 @@
         <v>2027</v>
       </c>
       <c r="C60" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D60" s="1">
         <f t="shared" si="2"/>
@@ -1575,7 +1575,7 @@
         <v>2027</v>
       </c>
       <c r="C61" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D61" s="1">
         <f t="shared" si="2"/>
@@ -1590,7 +1590,7 @@
         <v>2028</v>
       </c>
       <c r="C62" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D62" s="1">
         <f t="shared" si="2"/>
@@ -1605,7 +1605,7 @@
         <v>2028</v>
       </c>
       <c r="C63" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D63" s="1">
         <f t="shared" si="2"/>
@@ -1620,7 +1620,7 @@
         <v>2028</v>
       </c>
       <c r="C64" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D64" s="1">
         <f t="shared" si="2"/>
@@ -1635,7 +1635,7 @@
         <v>2028</v>
       </c>
       <c r="C65" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D65" s="1">
         <f t="shared" si="2"/>
@@ -1650,7 +1650,7 @@
         <v>2028</v>
       </c>
       <c r="C66" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D66" s="1">
         <f t="shared" si="2"/>
@@ -1665,7 +1665,7 @@
         <v>2028</v>
       </c>
       <c r="C67" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D67" s="1">
         <f t="shared" si="2"/>
@@ -1680,7 +1680,7 @@
         <v>2028</v>
       </c>
       <c r="C68" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D68" s="1">
         <f t="shared" si="2"/>
@@ -1695,7 +1695,7 @@
         <v>2028</v>
       </c>
       <c r="C69" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D69" s="1">
         <f t="shared" si="2"/>
@@ -1710,7 +1710,7 @@
         <v>2028</v>
       </c>
       <c r="C70" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D70" s="1">
         <f t="shared" ref="D70:D97" si="4">D69*1.1</f>
@@ -1725,7 +1725,7 @@
         <v>2028</v>
       </c>
       <c r="C71" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D71" s="1">
         <f t="shared" si="4"/>
@@ -1740,7 +1740,7 @@
         <v>2028</v>
       </c>
       <c r="C72" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D72" s="1">
         <f t="shared" si="4"/>
@@ -1755,7 +1755,7 @@
         <v>2028</v>
       </c>
       <c r="C73" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D73" s="1">
         <f t="shared" si="4"/>
@@ -1770,7 +1770,7 @@
         <v>2029</v>
       </c>
       <c r="C74" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D74" s="1">
         <f t="shared" si="4"/>
@@ -1785,7 +1785,7 @@
         <v>2029</v>
       </c>
       <c r="C75" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D75" s="1">
         <f t="shared" si="4"/>
@@ -1800,7 +1800,7 @@
         <v>2029</v>
       </c>
       <c r="C76" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D76" s="1">
         <f t="shared" si="4"/>
@@ -1815,7 +1815,7 @@
         <v>2029</v>
       </c>
       <c r="C77" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D77" s="1">
         <f t="shared" si="4"/>
@@ -1830,7 +1830,7 @@
         <v>2029</v>
       </c>
       <c r="C78" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D78" s="1">
         <f t="shared" si="4"/>
@@ -1845,7 +1845,7 @@
         <v>2029</v>
       </c>
       <c r="C79" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D79" s="1">
         <f t="shared" si="4"/>
@@ -1860,7 +1860,7 @@
         <v>2029</v>
       </c>
       <c r="C80" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D80" s="1">
         <f t="shared" si="4"/>
@@ -1875,7 +1875,7 @@
         <v>2029</v>
       </c>
       <c r="C81" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D81" s="1">
         <f t="shared" si="4"/>
@@ -1890,7 +1890,7 @@
         <v>2029</v>
       </c>
       <c r="C82" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D82" s="1">
         <f t="shared" si="4"/>
@@ -1905,7 +1905,7 @@
         <v>2029</v>
       </c>
       <c r="C83" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D83" s="1">
         <f t="shared" si="4"/>
@@ -1920,7 +1920,7 @@
         <v>2029</v>
       </c>
       <c r="C84" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D84" s="1">
         <f t="shared" si="4"/>
@@ -1935,7 +1935,7 @@
         <v>2029</v>
       </c>
       <c r="C85" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D85" s="1">
         <f t="shared" si="4"/>
@@ -1950,7 +1950,7 @@
         <v>2030</v>
       </c>
       <c r="C86" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D86" s="1">
         <f t="shared" si="4"/>
@@ -1965,7 +1965,7 @@
         <v>2030</v>
       </c>
       <c r="C87" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D87" s="1">
         <f t="shared" si="4"/>
@@ -1980,7 +1980,7 @@
         <v>2030</v>
       </c>
       <c r="C88" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D88" s="1">
         <f t="shared" si="4"/>
@@ -1995,7 +1995,7 @@
         <v>2030</v>
       </c>
       <c r="C89" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D89" s="1">
         <f t="shared" si="4"/>
@@ -2010,7 +2010,7 @@
         <v>2030</v>
       </c>
       <c r="C90" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D90" s="1">
         <f t="shared" si="4"/>
@@ -2025,7 +2025,7 @@
         <v>2030</v>
       </c>
       <c r="C91" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D91" s="1">
         <f t="shared" si="4"/>
@@ -2040,7 +2040,7 @@
         <v>2030</v>
       </c>
       <c r="C92" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D92" s="1">
         <f t="shared" si="4"/>
@@ -2055,7 +2055,7 @@
         <v>2030</v>
       </c>
       <c r="C93" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D93" s="1">
         <f t="shared" si="4"/>
@@ -2070,7 +2070,7 @@
         <v>2030</v>
       </c>
       <c r="C94" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D94" s="1">
         <f t="shared" si="4"/>
@@ -2085,7 +2085,7 @@
         <v>2030</v>
       </c>
       <c r="C95" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D95" s="1">
         <f t="shared" si="4"/>
@@ -2100,7 +2100,7 @@
         <v>2030</v>
       </c>
       <c r="C96" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D96" s="1">
         <f t="shared" si="4"/>
@@ -2115,7 +2115,7 @@
         <v>2030</v>
       </c>
       <c r="C97" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D97" s="1">
         <f t="shared" si="4"/>

</xml_diff>

<commit_message>
added link to the third video in dplyr on steroids post
</commit_message>
<xml_diff>
--- a/compounding_growth_10_percent.xlsx
+++ b/compounding_growth_10_percent.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zablotski/Library/Mobile Documents/com~apple~CloudDocs/7. Hobby/programming and stats/yuzaR-Blog/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F13994C-BDD3-ED4E-A566-8949210E86B3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE4A0882-4957-6F4D-AF3A-05DBACC80B53}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{EDD741CF-9DB9-2945-BF15-255A1807DC69}"/>
   </bookViews>
@@ -449,7 +449,7 @@
   <dimension ref="A1:J97"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="284" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -695,15 +695,15 @@
         <v>9.5</v>
       </c>
       <c r="H7">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="I7">
         <f t="shared" si="0"/>
-        <v>282.45999999999998</v>
+        <v>32.46</v>
       </c>
       <c r="J7" s="1">
         <f>I7-D7</f>
-        <v>258.30234999999999</v>
+        <v>8.3023499999999935</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -720,16 +720,25 @@
         <f t="shared" si="2"/>
         <v>26.573415000000011</v>
       </c>
+      <c r="E8">
+        <v>9.18</v>
+      </c>
       <c r="F8">
         <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>250</v>
       </c>
       <c r="I8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>259.18</v>
       </c>
       <c r="J8" s="1">
         <f t="shared" ref="J8:J13" si="3">I8-D8</f>
-        <v>-26.573415000000011</v>
+        <v>232.606585</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
new post on bar plots
</commit_message>
<xml_diff>
--- a/compounding_growth_10_percent.xlsx
+++ b/compounding_growth_10_percent.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zablotski/Library/Mobile Documents/com~apple~CloudDocs/7. Hobby/programming and stats/yuzaR-Blog/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE4A0882-4957-6F4D-AF3A-05DBACC80B53}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48919B97-091A-4E47-9DE9-5051C74F6523}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{EDD741CF-9DB9-2945-BF15-255A1807DC69}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="keywords" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="103">
   <si>
     <t>year</t>
   </si>
@@ -91,6 +92,249 @@
   </si>
   <si>
     <t>adds</t>
+  </si>
+  <si>
+    <t>Keyword</t>
+  </si>
+  <si>
+    <t>Monthly search volume</t>
+  </si>
+  <si>
+    <t>Low range</t>
+  </si>
+  <si>
+    <t>High range</t>
+  </si>
+  <si>
+    <t>Competition</t>
+  </si>
+  <si>
+    <t>ai</t>
+  </si>
+  <si>
+    <t>$0.81</t>
+  </si>
+  <si>
+    <t>$2.75</t>
+  </si>
+  <si>
+    <t>MEDIUM</t>
+  </si>
+  <si>
+    <t>artificial intelligence</t>
+  </si>
+  <si>
+    <t>$0.98</t>
+  </si>
+  <si>
+    <t>$3.44</t>
+  </si>
+  <si>
+    <t>LOW</t>
+  </si>
+  <si>
+    <t>data analytics</t>
+  </si>
+  <si>
+    <t>$3.75</t>
+  </si>
+  <si>
+    <t>$11.89</t>
+  </si>
+  <si>
+    <t>data analyst</t>
+  </si>
+  <si>
+    <t>computational science</t>
+  </si>
+  <si>
+    <t>$4.77</t>
+  </si>
+  <si>
+    <t>$15.66</t>
+  </si>
+  <si>
+    <t>machine learning</t>
+  </si>
+  <si>
+    <t>$2.26</t>
+  </si>
+  <si>
+    <t>$7.26</t>
+  </si>
+  <si>
+    <t>data science</t>
+  </si>
+  <si>
+    <t>$3.31</t>
+  </si>
+  <si>
+    <t>$9.97</t>
+  </si>
+  <si>
+    <t>datascience</t>
+  </si>
+  <si>
+    <t>programming</t>
+  </si>
+  <si>
+    <t>$2.76</t>
+  </si>
+  <si>
+    <t>$9.23</t>
+  </si>
+  <si>
+    <t>coding bootcamp</t>
+  </si>
+  <si>
+    <t>$10.27</t>
+  </si>
+  <si>
+    <t>$24.61</t>
+  </si>
+  <si>
+    <t>data bricks</t>
+  </si>
+  <si>
+    <t>$27.38</t>
+  </si>
+  <si>
+    <t>$1,000.00</t>
+  </si>
+  <si>
+    <t>business analytics</t>
+  </si>
+  <si>
+    <t>$2.57</t>
+  </si>
+  <si>
+    <t>$10.89</t>
+  </si>
+  <si>
+    <t>online data analytics degree</t>
+  </si>
+  <si>
+    <t>$14.52</t>
+  </si>
+  <si>
+    <t>$57.07</t>
+  </si>
+  <si>
+    <t>google data studio</t>
+  </si>
+  <si>
+    <t>$3.74</t>
+  </si>
+  <si>
+    <t>$20.52</t>
+  </si>
+  <si>
+    <t>data center</t>
+  </si>
+  <si>
+    <t>$5.33</t>
+  </si>
+  <si>
+    <t>$22.51</t>
+  </si>
+  <si>
+    <t>analysis of data</t>
+  </si>
+  <si>
+    <t>$4.12</t>
+  </si>
+  <si>
+    <t>$11.43</t>
+  </si>
+  <si>
+    <t>certified data analyst</t>
+  </si>
+  <si>
+    <t>$6.22</t>
+  </si>
+  <si>
+    <t>$18.32</t>
+  </si>
+  <si>
+    <t>data mining</t>
+  </si>
+  <si>
+    <t>$3.02</t>
+  </si>
+  <si>
+    <t>$28.86</t>
+  </si>
+  <si>
+    <t>data visualization</t>
+  </si>
+  <si>
+    <t>$3.49</t>
+  </si>
+  <si>
+    <t>$11.58</t>
+  </si>
+  <si>
+    <t>master's in data science</t>
+  </si>
+  <si>
+    <t>$9.41</t>
+  </si>
+  <si>
+    <t>$36.96</t>
+  </si>
+  <si>
+    <t>certified data scientist</t>
+  </si>
+  <si>
+    <t>$6.86</t>
+  </si>
+  <si>
+    <t>$16.24</t>
+  </si>
+  <si>
+    <t>data analytics degrees</t>
+  </si>
+  <si>
+    <t>$9.69</t>
+  </si>
+  <si>
+    <t>$36.58</t>
+  </si>
+  <si>
+    <t>online master's in data science</t>
+  </si>
+  <si>
+    <t>$12.09</t>
+  </si>
+  <si>
+    <t>$41.62</t>
+  </si>
+  <si>
+    <t>data science programming</t>
+  </si>
+  <si>
+    <t>$8.63</t>
+  </si>
+  <si>
+    <t>$28.32</t>
+  </si>
+  <si>
+    <t>data science degrees</t>
+  </si>
+  <si>
+    <t>$7.14</t>
+  </si>
+  <si>
+    <t>$24.75</t>
+  </si>
+  <si>
+    <t>data analytics masters online</t>
+  </si>
+  <si>
+    <t>$17.92</t>
+  </si>
+  <si>
+    <t>$58.58</t>
   </si>
 </sst>
 </file>
@@ -100,13 +344,36 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val=".AppleSystemUIFont"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF404040"/>
+      <name val="Unify Sans"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val=".AppleSystemUIFont"/>
     </font>
   </fonts>
   <fills count="2">
@@ -129,9 +396,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -448,11 +719,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6A4B67E-A70E-FF47-86DD-9BF22E85C9FF}">
   <dimension ref="A1:J97"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="284" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" zoomScale="178" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.1640625" bestFit="1" customWidth="1"/>
@@ -465,7 +736,7 @@
     <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -497,7 +768,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10">
       <c r="A2">
         <v>1</v>
       </c>
@@ -531,7 +802,7 @@
         <v>-1.3499999999999996</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10">
       <c r="A3">
         <v>2</v>
       </c>
@@ -566,7 +837,7 @@
         <v>12.350000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10">
       <c r="A4">
         <v>3</v>
       </c>
@@ -601,7 +872,7 @@
         <v>5.3699999999999974</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10">
       <c r="A5">
         <v>4</v>
       </c>
@@ -636,7 +907,7 @@
         <v>23.724999999999994</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10">
       <c r="A6">
         <v>5</v>
       </c>
@@ -651,7 +922,7 @@
         <v>21.961500000000004</v>
       </c>
       <c r="E6">
-        <v>25.93</v>
+        <v>25.88</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -664,14 +935,14 @@
       </c>
       <c r="I6">
         <f t="shared" si="0"/>
-        <v>25.93</v>
+        <v>25.88</v>
       </c>
       <c r="J6" s="1">
         <f>I6-D6</f>
-        <v>3.9684999999999953</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+        <v>3.9184999999999945</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7">
         <v>6</v>
       </c>
@@ -686,7 +957,7 @@
         <v>24.157650000000007</v>
       </c>
       <c r="E7">
-        <v>22.96</v>
+        <v>22.77</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -695,18 +966,18 @@
         <v>9.5</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="I7">
         <f t="shared" si="0"/>
-        <v>32.46</v>
+        <v>282.27</v>
       </c>
       <c r="J7" s="1">
         <f>I7-D7</f>
-        <v>8.3023499999999935</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+        <v>258.11234999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8">
         <v>7</v>
       </c>
@@ -721,7 +992,7 @@
         <v>26.573415000000011</v>
       </c>
       <c r="E8">
-        <v>9.18</v>
+        <v>35.22</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -730,18 +1001,18 @@
         <v>0</v>
       </c>
       <c r="H8">
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="I8">
         <f t="shared" si="0"/>
-        <v>259.18</v>
+        <v>35.22</v>
       </c>
       <c r="J8" s="1">
         <f t="shared" ref="J8:J13" si="3">I8-D8</f>
-        <v>232.606585</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+        <v>8.6465849999999875</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9">
         <v>8</v>
       </c>
@@ -755,19 +1026,28 @@
         <f t="shared" si="2"/>
         <v>29.230756500000016</v>
       </c>
+      <c r="E9">
+        <v>17.97</v>
+      </c>
       <c r="F9">
         <v>0</v>
       </c>
+      <c r="G9">
+        <v>9.5</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
       <c r="I9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>27.47</v>
       </c>
       <c r="J9" s="1">
         <f t="shared" si="3"/>
-        <v>-29.230756500000016</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+        <v>-1.7607565000000172</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10">
         <v>9</v>
       </c>
@@ -793,7 +1073,7 @@
         <v>-32.153832150000021</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10">
       <c r="A11">
         <v>10</v>
       </c>
@@ -819,7 +1099,7 @@
         <v>-35.369215365000024</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10">
       <c r="A12">
         <v>11</v>
       </c>
@@ -845,7 +1125,7 @@
         <v>-38.906136901500027</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10">
       <c r="A13">
         <v>12</v>
       </c>
@@ -871,7 +1151,7 @@
         <v>-42.796750591650031</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10">
       <c r="A14">
         <v>13</v>
       </c>
@@ -886,7 +1166,7 @@
         <v>47.07642565081504</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10">
       <c r="A15">
         <v>14</v>
       </c>
@@ -901,7 +1181,7 @@
         <v>51.784068215896546</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10">
       <c r="A16">
         <v>15</v>
       </c>
@@ -916,7 +1196,7 @@
         <v>56.962475037486207</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4">
       <c r="A17">
         <v>16</v>
       </c>
@@ -931,7 +1211,7 @@
         <v>62.65872254123483</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4">
       <c r="A18">
         <v>17</v>
       </c>
@@ -946,7 +1226,7 @@
         <v>68.924594795358317</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4">
       <c r="A19">
         <v>18</v>
       </c>
@@ -961,7 +1241,7 @@
         <v>75.817054274894161</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4">
       <c r="A20">
         <v>19</v>
       </c>
@@ -976,7 +1256,7 @@
         <v>83.398759702383586</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4">
       <c r="A21">
         <v>20</v>
       </c>
@@ -991,7 +1271,7 @@
         <v>91.738635672621953</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1006,7 +1286,7 @@
         <v>100.91249923988416</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1021,7 +1301,7 @@
         <v>111.00374916387258</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1036,7 +1316,7 @@
         <v>122.10412408025985</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1051,7 +1331,7 @@
         <v>134.31453648828585</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1066,7 +1346,7 @@
         <v>147.74599013711446</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1081,7 +1361,7 @@
         <v>162.52058915082591</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1096,7 +1376,7 @@
         <v>178.77264806590853</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1111,7 +1391,7 @@
         <v>196.64991287249939</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1126,7 +1406,7 @@
         <v>216.31490415974935</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1141,7 +1421,7 @@
         <v>237.9463945757243</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1156,7 +1436,7 @@
         <v>261.74103403329673</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1171,7 +1451,7 @@
         <v>287.91513743662642</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1186,7 +1466,7 @@
         <v>316.7066511802891</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1201,7 +1481,7 @@
         <v>348.37731629831802</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1216,7 +1496,7 @@
         <v>383.21504792814983</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1231,7 +1511,7 @@
         <v>421.53655272096483</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1246,7 +1526,7 @@
         <v>463.69020799306134</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1261,7 +1541,7 @@
         <v>510.05922879236749</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1276,7 +1556,7 @@
         <v>561.06515167160433</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1291,7 +1571,7 @@
         <v>617.17166683876485</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1306,7 +1586,7 @@
         <v>678.88883352264133</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1321,7 +1601,7 @@
         <v>746.77771687490554</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1336,7 +1616,7 @@
         <v>821.45548856239611</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1351,7 +1631,7 @@
         <v>903.60103741863577</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1366,7 +1646,7 @@
         <v>993.96114116049944</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1381,7 +1661,7 @@
         <v>1093.3572552765495</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1396,7 +1676,7 @@
         <v>1202.6929808042046</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1411,7 +1691,7 @@
         <v>1322.9622788846252</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4">
       <c r="A50">
         <v>49</v>
       </c>
@@ -1426,7 +1706,7 @@
         <v>1455.2585067730879</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4">
       <c r="A51">
         <v>50</v>
       </c>
@@ -1441,7 +1721,7 @@
         <v>1600.7843574503968</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4">
       <c r="A52">
         <v>51</v>
       </c>
@@ -1456,7 +1736,7 @@
         <v>1760.8627931954366</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4">
       <c r="A53">
         <v>52</v>
       </c>
@@ -1471,7 +1751,7 @@
         <v>1936.9490725149803</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4">
       <c r="A54">
         <v>53</v>
       </c>
@@ -1486,7 +1766,7 @@
         <v>2130.6439797664784</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4">
       <c r="A55">
         <v>54</v>
       </c>
@@ -1501,7 +1781,7 @@
         <v>2343.7083777431267</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4">
       <c r="A56">
         <v>55</v>
       </c>
@@ -1516,7 +1796,7 @@
         <v>2578.0792155174395</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4">
       <c r="A57">
         <v>56</v>
       </c>
@@ -1531,7 +1811,7 @@
         <v>2835.8871370691836</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4">
       <c r="A58">
         <v>57</v>
       </c>
@@ -1546,7 +1826,7 @@
         <v>3119.4758507761021</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4">
       <c r="A59">
         <v>58</v>
       </c>
@@ -1561,7 +1841,7 @@
         <v>3431.4234358537128</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4">
       <c r="A60">
         <v>59</v>
       </c>
@@ -1576,7 +1856,7 @@
         <v>3774.5657794390845</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4">
       <c r="A61">
         <v>60</v>
       </c>
@@ -1591,7 +1871,7 @@
         <v>4152.0223573829935</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4">
       <c r="A62">
         <v>61</v>
       </c>
@@ -1606,7 +1886,7 @@
         <v>4567.2245931212929</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4">
       <c r="A63">
         <v>62</v>
       </c>
@@ -1621,7 +1901,7 @@
         <v>5023.9470524334229</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4">
       <c r="A64">
         <v>63</v>
       </c>
@@ -1636,7 +1916,7 @@
         <v>5526.3417576767652</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4">
       <c r="A65">
         <v>64</v>
       </c>
@@ -1651,7 +1931,7 @@
         <v>6078.9759334444425</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4">
       <c r="A66">
         <v>65</v>
       </c>
@@ -1666,7 +1946,7 @@
         <v>6686.8735267888869</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4">
       <c r="A67">
         <v>66</v>
       </c>
@@ -1681,7 +1961,7 @@
         <v>7355.5608794677764</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:4">
       <c r="A68">
         <v>67</v>
       </c>
@@ -1696,7 +1976,7 @@
         <v>8091.1169674145549</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:4">
       <c r="A69">
         <v>68</v>
       </c>
@@ -1711,7 +1991,7 @@
         <v>8900.2286641560113</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4">
       <c r="A70">
         <v>69</v>
       </c>
@@ -1726,7 +2006,7 @@
         <v>9790.2515305716133</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4">
       <c r="A71">
         <v>70</v>
       </c>
@@ -1741,7 +2021,7 @@
         <v>10769.276683628776</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:4">
       <c r="A72">
         <v>71</v>
       </c>
@@ -1756,7 +2036,7 @@
         <v>11846.204351991653</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:4">
       <c r="A73">
         <v>72</v>
       </c>
@@ -1771,7 +2051,7 @@
         <v>13030.824787190819</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:4">
       <c r="A74">
         <v>73</v>
       </c>
@@ -1786,7 +2066,7 @@
         <v>14333.907265909902</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:4">
       <c r="A75">
         <v>74</v>
       </c>
@@ -1801,7 +2081,7 @@
         <v>15767.297992500893</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:4">
       <c r="A76">
         <v>75</v>
       </c>
@@ -1816,7 +2096,7 @@
         <v>17344.027791750985</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:4">
       <c r="A77">
         <v>76</v>
       </c>
@@ -1831,7 +2111,7 @@
         <v>19078.430570926084</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:4">
       <c r="A78">
         <v>77</v>
       </c>
@@ -1846,7 +2126,7 @@
         <v>20986.273628018695</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:4">
       <c r="A79">
         <v>78</v>
       </c>
@@ -1861,7 +2141,7 @@
         <v>23084.900990820566</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:4">
       <c r="A80">
         <v>79</v>
       </c>
@@ -1876,7 +2156,7 @@
         <v>25393.391089902623</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:4">
       <c r="A81">
         <v>80</v>
       </c>
@@ -1891,7 +2171,7 @@
         <v>27932.730198892888</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:4">
       <c r="A82">
         <v>81</v>
       </c>
@@ -1906,7 +2186,7 @@
         <v>30726.003218782178</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:4">
       <c r="A83">
         <v>82</v>
       </c>
@@ -1921,7 +2201,7 @@
         <v>33798.603540660399</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:4">
       <c r="A84">
         <v>83</v>
       </c>
@@ -1936,7 +2216,7 @@
         <v>37178.463894726439</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:4">
       <c r="A85">
         <v>84</v>
       </c>
@@ -1951,7 +2231,7 @@
         <v>40896.310284199084</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:4">
       <c r="A86">
         <v>85</v>
       </c>
@@ -1966,7 +2246,7 @@
         <v>44985.941312618997</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:4">
       <c r="A87">
         <v>86</v>
       </c>
@@ -1981,7 +2261,7 @@
         <v>49484.535443880901</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:4">
       <c r="A88">
         <v>87</v>
       </c>
@@ -1996,7 +2276,7 @@
         <v>54432.988988268997</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:4">
       <c r="A89">
         <v>88</v>
       </c>
@@ -2011,7 +2291,7 @@
         <v>59876.287887095903</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:4">
       <c r="A90">
         <v>89</v>
       </c>
@@ -2026,7 +2306,7 @@
         <v>65863.916675805493</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:4">
       <c r="A91">
         <v>90</v>
       </c>
@@ -2041,7 +2321,7 @@
         <v>72450.308343386045</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:4">
       <c r="A92">
         <v>91</v>
       </c>
@@ -2056,7 +2336,7 @@
         <v>79695.339177724658</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:4">
       <c r="A93">
         <v>92</v>
       </c>
@@ -2071,7 +2351,7 @@
         <v>87664.873095497125</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:4">
       <c r="A94">
         <v>93</v>
       </c>
@@ -2086,7 +2366,7 @@
         <v>96431.360405046842</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:4">
       <c r="A95">
         <v>94</v>
       </c>
@@ -2101,7 +2381,7 @@
         <v>106074.49644555153</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:4">
       <c r="A96">
         <v>95</v>
       </c>
@@ -2116,7 +2396,7 @@
         <v>116681.94609010669</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:4">
       <c r="A97">
         <v>96</v>
       </c>
@@ -2134,4 +2414,486 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18B478A7-EA3A-EE42-9B5F-0F93A4B2BAA6}">
+  <dimension ref="A1:E27"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" zoomScale="156" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="33.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="17">
+      <c r="A1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="18">
+      <c r="A2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="4">
+        <v>823</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="18">
+      <c r="A3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="4">
+        <v>301</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="17">
+      <c r="A4" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="5">
+        <v>246</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="17">
+      <c r="A5" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="5">
+        <v>246</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="17">
+      <c r="A6" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="5">
+        <v>135</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="18">
+      <c r="A7" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="4">
+        <v>110</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="17">
+      <c r="A8" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="5">
+        <v>110</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="17">
+      <c r="A9" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="5">
+        <v>110</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="17">
+      <c r="A10" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="5">
+        <v>110</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="17">
+      <c r="A11" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="5">
+        <v>90.5</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="17">
+      <c r="A12" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" s="5">
+        <v>74</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="17">
+      <c r="A13" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" s="5">
+        <v>60.5</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="17">
+      <c r="A14" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" s="5">
+        <v>60.5</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="17">
+      <c r="A15" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" s="5">
+        <v>49.5</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="17">
+      <c r="A16" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" s="5">
+        <v>33.1</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="17">
+      <c r="A17" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B17" s="5">
+        <v>33.1</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="17">
+      <c r="A18" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B18" s="5">
+        <v>27.1</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="17">
+      <c r="A19" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B19" s="5">
+        <v>27.1</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="17">
+      <c r="A20" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B20" s="5">
+        <v>27.1</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="17">
+      <c r="A21" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B21" s="5">
+        <v>9.9</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="17">
+      <c r="A22" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B22" s="5">
+        <v>6.6</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="17">
+      <c r="A23" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B23" s="5">
+        <v>6.6</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="17">
+      <c r="A24" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B24" s="5">
+        <v>5.4</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="17">
+      <c r="A25" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B25" s="5">
+        <v>5.4</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="17">
+      <c r="A26" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B26" s="5">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="17">
+      <c r="A27" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B27" s="5">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
new thumbnail for sjPlot
</commit_message>
<xml_diff>
--- a/compounding_growth_10_percent.xlsx
+++ b/compounding_growth_10_percent.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zablotski/Library/Mobile Documents/com~apple~CloudDocs/7. Hobby/programming and stats/yuzaR-Blog/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCAD22BD-2FB4-AF43-B4CE-9F2B071A3DB3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F1A6A5C-EAA4-4141-B089-C1F93A9FECB2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{EDD741CF-9DB9-2945-BF15-255A1807DC69}"/>
   </bookViews>
@@ -738,7 +738,7 @@
   <dimension ref="A1:P97"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="144" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -847,7 +847,7 @@
       </c>
       <c r="L2">
         <f>SUM(E2:E13)</f>
-        <v>187.62</v>
+        <v>188.52</v>
       </c>
       <c r="M2">
         <f>SUM(F2:F13)</f>
@@ -863,7 +863,7 @@
       </c>
       <c r="P2">
         <f>SUM(I2:I13)</f>
-        <v>480.55000000000007</v>
+        <v>481.45000000000005</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -1094,7 +1094,7 @@
         <v>29.230756500000016</v>
       </c>
       <c r="E9">
-        <v>17.97</v>
+        <v>18.87</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -1107,11 +1107,11 @@
       </c>
       <c r="I9">
         <f t="shared" si="0"/>
-        <v>27.47</v>
+        <v>28.37</v>
       </c>
       <c r="J9" s="1">
         <f t="shared" si="3"/>
-        <v>-1.7607565000000172</v>
+        <v>-0.86075650000001502</v>
       </c>
     </row>
     <row r="10" spans="1:16">

</xml_diff>

<commit_message>
small improvement in barplots
</commit_message>
<xml_diff>
--- a/compounding_growth_10_percent.xlsx
+++ b/compounding_growth_10_percent.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zablotski/Library/Mobile Documents/com~apple~CloudDocs/7. Hobby/programming and stats/yuzaR-Blog/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F1A6A5C-EAA4-4141-B089-C1F93A9FECB2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{256FE9AC-6BBE-8A4B-909A-0B502A23027D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{EDD741CF-9DB9-2945-BF15-255A1807DC69}"/>
   </bookViews>
@@ -402,7 +402,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -410,17 +410,109 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -738,7 +830,7 @@
   <dimension ref="A1:P97"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="144" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -759,7 +851,7 @@
     <col min="15" max="15" width="14.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" ht="17" thickBot="1">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -810,775 +902,1140 @@
       </c>
     </row>
     <row r="2" spans="1:16">
-      <c r="A2">
+      <c r="A2" s="6">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="7">
         <v>2023</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="8">
         <v>15</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="7">
         <v>13.65</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="7">
         <v>0</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="7">
         <v>0</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="7">
         <v>0</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="7">
         <f>E2+F2+G2+H2</f>
         <v>13.65</v>
       </c>
-      <c r="J2" s="1">
+      <c r="J2" s="8">
         <f>I2-D2</f>
         <v>-1.3499999999999996</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="7">
         <v>2023</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="7">
         <f>SUM(E2:E13)</f>
-        <v>188.52</v>
-      </c>
-      <c r="M2">
+        <v>192.18</v>
+      </c>
+      <c r="M2" s="7">
         <f>SUM(F2:F13)</f>
         <v>4.93</v>
       </c>
-      <c r="N2">
+      <c r="N2" s="7">
         <f>SUM(G2:G13)</f>
         <v>38</v>
       </c>
-      <c r="O2">
+      <c r="O2" s="7">
         <f>SUM(H2:H13)</f>
         <v>250</v>
       </c>
-      <c r="P2">
+      <c r="P2" s="9">
         <f>SUM(I2:I13)</f>
-        <v>481.45000000000005</v>
+        <v>485.11</v>
       </c>
     </row>
     <row r="3" spans="1:16">
-      <c r="A3">
+      <c r="A3" s="10">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="11">
         <v>2023</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="12">
         <f>D2*1.1</f>
         <v>16.5</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="11">
         <v>23.92</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="11">
         <v>4.93</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="11">
         <v>0</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="11">
         <v>0</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="11">
         <f t="shared" ref="I3:I13" si="0">E3+F3+G3+H3</f>
         <v>28.85</v>
       </c>
-      <c r="J3" s="1">
+      <c r="J3" s="12">
         <f t="shared" ref="J3:J4" si="1">I3-D3</f>
         <v>12.350000000000001</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="11">
         <v>2024</v>
       </c>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="13"/>
     </row>
     <row r="4" spans="1:16">
-      <c r="A4">
+      <c r="A4" s="10">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="11">
         <v>2023</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="12">
         <f>D3*1.1</f>
         <v>18.150000000000002</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="11">
         <v>23.52</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="11">
         <v>0</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="11">
         <v>0</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="11">
         <v>0</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="11">
         <f t="shared" si="0"/>
         <v>23.52</v>
       </c>
-      <c r="J4" s="1">
+      <c r="J4" s="12">
         <f t="shared" si="1"/>
         <v>5.3699999999999974</v>
       </c>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="13"/>
     </row>
     <row r="5" spans="1:16">
-      <c r="A5">
+      <c r="A5" s="10">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="11">
         <v>2023</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="12">
         <f>D4*1.1</f>
         <v>19.965000000000003</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="11">
         <v>24.69</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="11">
         <v>0</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="11">
         <v>19</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="11">
         <v>0</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="11">
         <f t="shared" si="0"/>
         <v>43.69</v>
       </c>
-      <c r="J5" s="1">
+      <c r="J5" s="12">
         <f>I5-D5</f>
         <v>23.724999999999994</v>
       </c>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="13"/>
     </row>
     <row r="6" spans="1:16">
-      <c r="A6">
+      <c r="A6" s="10">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="11">
         <v>2023</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="12">
         <f t="shared" ref="D6:D69" si="2">D5*1.1</f>
         <v>21.961500000000004</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="11">
         <v>25.88</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="11">
         <v>0</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="11">
         <v>0</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="11">
         <v>0</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="11">
         <f t="shared" si="0"/>
         <v>25.88</v>
       </c>
-      <c r="J6" s="1">
+      <c r="J6" s="12">
         <f>I6-D6</f>
         <v>3.9184999999999945</v>
       </c>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="13"/>
     </row>
     <row r="7" spans="1:16">
-      <c r="A7">
+      <c r="A7" s="10">
         <v>6</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="11">
         <v>2023</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="12">
         <f t="shared" si="2"/>
         <v>24.157650000000007</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="11">
         <v>22.77</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="11">
         <v>0</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="11">
         <v>9.5</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="11">
         <v>250</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="11">
         <f t="shared" si="0"/>
         <v>282.27</v>
       </c>
-      <c r="J7" s="1">
+      <c r="J7" s="12">
         <f>I7-D7</f>
         <v>258.11234999999999</v>
       </c>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="11"/>
+      <c r="P7" s="13"/>
     </row>
     <row r="8" spans="1:16">
-      <c r="A8">
+      <c r="A8" s="10">
         <v>7</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="11">
         <v>2023</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="12">
         <f t="shared" si="2"/>
         <v>26.573415000000011</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="11">
         <v>35.22</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="11">
         <v>0</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="11">
         <v>0</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="11">
         <v>0</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="11">
         <f t="shared" si="0"/>
         <v>35.22</v>
       </c>
-      <c r="J8" s="1">
+      <c r="J8" s="12">
         <f t="shared" ref="J8:J13" si="3">I8-D8</f>
         <v>8.6465849999999875</v>
       </c>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="11"/>
+      <c r="P8" s="13"/>
     </row>
     <row r="9" spans="1:16">
-      <c r="A9">
+      <c r="A9" s="10">
         <v>8</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="11">
         <v>2023</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="12">
         <f t="shared" si="2"/>
         <v>29.230756500000016</v>
       </c>
-      <c r="E9">
-        <v>18.87</v>
-      </c>
-      <c r="F9">
+      <c r="E9" s="11">
+        <v>22.53</v>
+      </c>
+      <c r="F9" s="11">
         <v>0</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="11">
         <v>9.5</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="11">
         <v>0</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="11">
         <f t="shared" si="0"/>
-        <v>28.37</v>
-      </c>
-      <c r="J9" s="1">
+        <v>32.03</v>
+      </c>
+      <c r="J9" s="12">
         <f t="shared" si="3"/>
-        <v>-0.86075650000001502</v>
-      </c>
+        <v>2.7992434999999851</v>
+      </c>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="11"/>
+      <c r="P9" s="13"/>
     </row>
     <row r="10" spans="1:16">
-      <c r="A10">
+      <c r="A10" s="10">
         <v>9</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="11">
         <v>2023</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="12">
         <f t="shared" si="2"/>
         <v>32.153832150000021</v>
       </c>
-      <c r="F10">
+      <c r="E10" s="11"/>
+      <c r="F10" s="11">
         <v>0</v>
       </c>
-      <c r="I10">
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J10" s="1">
+      <c r="J10" s="12">
         <f t="shared" si="3"/>
         <v>-32.153832150000021</v>
       </c>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="11"/>
+      <c r="P10" s="13"/>
     </row>
     <row r="11" spans="1:16">
-      <c r="A11">
+      <c r="A11" s="10">
         <v>10</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="11">
         <v>2023</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="12">
         <f t="shared" si="2"/>
         <v>35.369215365000024</v>
       </c>
-      <c r="F11">
+      <c r="E11" s="11"/>
+      <c r="F11" s="11">
         <v>0</v>
       </c>
-      <c r="I11">
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J11" s="1">
+      <c r="J11" s="12">
         <f t="shared" si="3"/>
         <v>-35.369215365000024</v>
       </c>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
+      <c r="O11" s="11"/>
+      <c r="P11" s="13"/>
     </row>
     <row r="12" spans="1:16">
-      <c r="A12">
+      <c r="A12" s="10">
         <v>11</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="11">
         <v>2023</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="12">
         <f t="shared" si="2"/>
         <v>38.906136901500027</v>
       </c>
-      <c r="F12">
+      <c r="E12" s="11"/>
+      <c r="F12" s="11">
         <v>0</v>
       </c>
-      <c r="I12">
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J12" s="1">
+      <c r="J12" s="12">
         <f t="shared" si="3"/>
         <v>-38.906136901500027</v>
       </c>
-    </row>
-    <row r="13" spans="1:16">
-      <c r="A13">
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="11"/>
+      <c r="P12" s="13"/>
+    </row>
+    <row r="13" spans="1:16" ht="17" thickBot="1">
+      <c r="A13" s="14">
         <v>12</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="15">
         <v>2023</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13" s="16">
         <f t="shared" si="2"/>
         <v>42.796750591650031</v>
       </c>
-      <c r="F13">
+      <c r="E13" s="15"/>
+      <c r="F13" s="15">
         <v>0</v>
       </c>
-      <c r="I13">
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J13" s="1">
+      <c r="J13" s="16">
         <f t="shared" si="3"/>
         <v>-42.796750591650031</v>
       </c>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="15"/>
+      <c r="O13" s="15"/>
+      <c r="P13" s="17"/>
     </row>
     <row r="14" spans="1:16">
-      <c r="A14">
+      <c r="A14" s="6">
         <v>13</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="7">
         <v>2024</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14" s="8">
         <f t="shared" si="2"/>
         <v>47.07642565081504</v>
       </c>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="9"/>
     </row>
     <row r="15" spans="1:16">
-      <c r="A15">
+      <c r="A15" s="10">
         <v>14</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="11">
         <v>2024</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15" s="12">
         <f t="shared" si="2"/>
         <v>51.784068215896546</v>
       </c>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="11"/>
+      <c r="M15" s="11"/>
+      <c r="N15" s="11"/>
+      <c r="O15" s="11"/>
+      <c r="P15" s="13"/>
     </row>
     <row r="16" spans="1:16">
-      <c r="A16">
+      <c r="A16" s="10">
         <v>15</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="11">
         <v>2024</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16" s="12">
         <f t="shared" si="2"/>
         <v>56.962475037486207</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17">
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
+      <c r="N16" s="11"/>
+      <c r="O16" s="11"/>
+      <c r="P16" s="13"/>
+    </row>
+    <row r="17" spans="1:16">
+      <c r="A17" s="10">
         <v>16</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="11">
         <v>2024</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D17" s="12">
         <f t="shared" si="2"/>
         <v>62.65872254123483</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18">
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="11"/>
+      <c r="M17" s="11"/>
+      <c r="N17" s="11"/>
+      <c r="O17" s="11"/>
+      <c r="P17" s="13"/>
+    </row>
+    <row r="18" spans="1:16">
+      <c r="A18" s="10">
         <v>17</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="11">
         <v>2024</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D18" s="12">
         <f t="shared" si="2"/>
         <v>68.924594795358317</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19">
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="11"/>
+      <c r="N18" s="11"/>
+      <c r="O18" s="11"/>
+      <c r="P18" s="13"/>
+    </row>
+    <row r="19" spans="1:16">
+      <c r="A19" s="10">
         <v>18</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="11">
         <v>2024</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D19" s="12">
         <f t="shared" si="2"/>
         <v>75.817054274894161</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20">
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="11"/>
+      <c r="N19" s="11"/>
+      <c r="O19" s="11"/>
+      <c r="P19" s="13"/>
+    </row>
+    <row r="20" spans="1:16">
+      <c r="A20" s="10">
         <v>19</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="11">
         <v>2024</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D20" s="12">
         <f t="shared" si="2"/>
         <v>83.398759702383586</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21">
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="11"/>
+      <c r="N20" s="11"/>
+      <c r="O20" s="11"/>
+      <c r="P20" s="13"/>
+    </row>
+    <row r="21" spans="1:16">
+      <c r="A21" s="10">
         <v>20</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="11">
         <v>2024</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D21" s="12">
         <f t="shared" si="2"/>
         <v>91.738635672621953</v>
       </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22">
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="11"/>
+      <c r="N21" s="11"/>
+      <c r="O21" s="11"/>
+      <c r="P21" s="13"/>
+    </row>
+    <row r="22" spans="1:16">
+      <c r="A22" s="10">
         <v>21</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="11">
         <v>2024</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D22" s="1">
+      <c r="D22" s="12">
         <f t="shared" si="2"/>
         <v>100.91249923988416</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23">
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="11"/>
+      <c r="M22" s="11"/>
+      <c r="N22" s="11"/>
+      <c r="O22" s="11"/>
+      <c r="P22" s="13"/>
+    </row>
+    <row r="23" spans="1:16">
+      <c r="A23" s="10">
         <v>22</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="11">
         <v>2024</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D23" s="1">
+      <c r="D23" s="12">
         <f t="shared" si="2"/>
         <v>111.00374916387258</v>
       </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24">
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="11"/>
+      <c r="L23" s="11"/>
+      <c r="M23" s="11"/>
+      <c r="N23" s="11"/>
+      <c r="O23" s="11"/>
+      <c r="P23" s="13"/>
+    </row>
+    <row r="24" spans="1:16">
+      <c r="A24" s="10">
         <v>23</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="11">
         <v>2024</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D24" s="1">
+      <c r="D24" s="12">
         <f t="shared" si="2"/>
         <v>122.10412408025985</v>
       </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25">
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="11"/>
+      <c r="L24" s="11"/>
+      <c r="M24" s="11"/>
+      <c r="N24" s="11"/>
+      <c r="O24" s="11"/>
+      <c r="P24" s="13"/>
+    </row>
+    <row r="25" spans="1:16" ht="17" thickBot="1">
+      <c r="A25" s="14">
         <v>24</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="15">
         <v>2024</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="D25" s="1">
+      <c r="D25" s="16">
         <f t="shared" si="2"/>
         <v>134.31453648828585</v>
       </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26">
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="15"/>
+      <c r="I25" s="15"/>
+      <c r="J25" s="15"/>
+      <c r="K25" s="15"/>
+      <c r="L25" s="15"/>
+      <c r="M25" s="15"/>
+      <c r="N25" s="15"/>
+      <c r="O25" s="15"/>
+      <c r="P25" s="17"/>
+    </row>
+    <row r="26" spans="1:16">
+      <c r="A26" s="6">
         <v>25</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="7">
         <v>2025</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D26" s="1">
+      <c r="D26" s="8">
         <f t="shared" si="2"/>
         <v>147.74599013711446</v>
       </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27">
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="7"/>
+      <c r="L26" s="7"/>
+      <c r="M26" s="7"/>
+      <c r="N26" s="7"/>
+      <c r="O26" s="7"/>
+      <c r="P26" s="9"/>
+    </row>
+    <row r="27" spans="1:16">
+      <c r="A27" s="10">
         <v>26</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="11">
         <v>2025</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D27" s="1">
+      <c r="D27" s="12">
         <f t="shared" si="2"/>
         <v>162.52058915082591</v>
       </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28">
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="11"/>
+      <c r="K27" s="11"/>
+      <c r="L27" s="11"/>
+      <c r="M27" s="11"/>
+      <c r="N27" s="11"/>
+      <c r="O27" s="11"/>
+      <c r="P27" s="13"/>
+    </row>
+    <row r="28" spans="1:16">
+      <c r="A28" s="10">
         <v>27</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="11">
         <v>2025</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D28" s="1">
+      <c r="D28" s="12">
         <f t="shared" si="2"/>
         <v>178.77264806590853</v>
       </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29">
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="11"/>
+      <c r="K28" s="11"/>
+      <c r="L28" s="11"/>
+      <c r="M28" s="11"/>
+      <c r="N28" s="11"/>
+      <c r="O28" s="11"/>
+      <c r="P28" s="13"/>
+    </row>
+    <row r="29" spans="1:16">
+      <c r="A29" s="10">
         <v>28</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="11">
         <v>2025</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D29" s="1">
+      <c r="D29" s="12">
         <f t="shared" si="2"/>
         <v>196.64991287249939</v>
       </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30">
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="11"/>
+      <c r="J29" s="11"/>
+      <c r="K29" s="11"/>
+      <c r="L29" s="11"/>
+      <c r="M29" s="11"/>
+      <c r="N29" s="11"/>
+      <c r="O29" s="11"/>
+      <c r="P29" s="13"/>
+    </row>
+    <row r="30" spans="1:16">
+      <c r="A30" s="10">
         <v>29</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="11">
         <v>2025</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D30" s="1">
+      <c r="D30" s="12">
         <f t="shared" si="2"/>
         <v>216.31490415974935</v>
       </c>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31">
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="11"/>
+      <c r="J30" s="11"/>
+      <c r="K30" s="11"/>
+      <c r="L30" s="11"/>
+      <c r="M30" s="11"/>
+      <c r="N30" s="11"/>
+      <c r="O30" s="11"/>
+      <c r="P30" s="13"/>
+    </row>
+    <row r="31" spans="1:16">
+      <c r="A31" s="10">
         <v>30</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="11">
         <v>2025</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D31" s="1">
+      <c r="D31" s="12">
         <f t="shared" si="2"/>
         <v>237.9463945757243</v>
       </c>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32">
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="11"/>
+      <c r="J31" s="11"/>
+      <c r="K31" s="11"/>
+      <c r="L31" s="11"/>
+      <c r="M31" s="11"/>
+      <c r="N31" s="11"/>
+      <c r="O31" s="11"/>
+      <c r="P31" s="13"/>
+    </row>
+    <row r="32" spans="1:16">
+      <c r="A32" s="10">
         <v>31</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="11">
         <v>2025</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D32" s="1">
+      <c r="D32" s="12">
         <f t="shared" si="2"/>
         <v>261.74103403329673</v>
       </c>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33">
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="11"/>
+      <c r="J32" s="11"/>
+      <c r="K32" s="11"/>
+      <c r="L32" s="11"/>
+      <c r="M32" s="11"/>
+      <c r="N32" s="11"/>
+      <c r="O32" s="11"/>
+      <c r="P32" s="13"/>
+    </row>
+    <row r="33" spans="1:16">
+      <c r="A33" s="10">
         <v>32</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="11">
         <v>2025</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D33" s="1">
+      <c r="D33" s="12">
         <f t="shared" si="2"/>
         <v>287.91513743662642</v>
       </c>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34">
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="11"/>
+      <c r="J33" s="11"/>
+      <c r="K33" s="11"/>
+      <c r="L33" s="11"/>
+      <c r="M33" s="11"/>
+      <c r="N33" s="11"/>
+      <c r="O33" s="11"/>
+      <c r="P33" s="13"/>
+    </row>
+    <row r="34" spans="1:16">
+      <c r="A34" s="10">
         <v>33</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="11">
         <v>2025</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D34" s="1">
+      <c r="D34" s="12">
         <f t="shared" si="2"/>
         <v>316.7066511802891</v>
       </c>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35">
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="11"/>
+      <c r="I34" s="11"/>
+      <c r="J34" s="11"/>
+      <c r="K34" s="11"/>
+      <c r="L34" s="11"/>
+      <c r="M34" s="11"/>
+      <c r="N34" s="11"/>
+      <c r="O34" s="11"/>
+      <c r="P34" s="13"/>
+    </row>
+    <row r="35" spans="1:16">
+      <c r="A35" s="10">
         <v>34</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="11">
         <v>2025</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D35" s="1">
+      <c r="D35" s="12">
         <f t="shared" si="2"/>
         <v>348.37731629831802</v>
       </c>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36">
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="11"/>
+      <c r="I35" s="11"/>
+      <c r="J35" s="11"/>
+      <c r="K35" s="11"/>
+      <c r="L35" s="11"/>
+      <c r="M35" s="11"/>
+      <c r="N35" s="11"/>
+      <c r="O35" s="11"/>
+      <c r="P35" s="13"/>
+    </row>
+    <row r="36" spans="1:16">
+      <c r="A36" s="10">
         <v>35</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="11">
         <v>2025</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D36" s="1">
+      <c r="D36" s="12">
         <f t="shared" si="2"/>
         <v>383.21504792814983</v>
       </c>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37">
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
+      <c r="G36" s="11"/>
+      <c r="H36" s="11"/>
+      <c r="I36" s="11"/>
+      <c r="J36" s="11"/>
+      <c r="K36" s="11"/>
+      <c r="L36" s="11"/>
+      <c r="M36" s="11"/>
+      <c r="N36" s="11"/>
+      <c r="O36" s="11"/>
+      <c r="P36" s="13"/>
+    </row>
+    <row r="37" spans="1:16" ht="17" thickBot="1">
+      <c r="A37" s="14">
         <v>36</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="15">
         <v>2025</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="D37" s="1">
+      <c r="D37" s="16">
         <f t="shared" si="2"/>
         <v>421.53655272096483</v>
       </c>
-    </row>
-    <row r="38" spans="1:4">
+      <c r="E37" s="15"/>
+      <c r="F37" s="15"/>
+      <c r="G37" s="15"/>
+      <c r="H37" s="15"/>
+      <c r="I37" s="15"/>
+      <c r="J37" s="15"/>
+      <c r="K37" s="15"/>
+      <c r="L37" s="15"/>
+      <c r="M37" s="15"/>
+      <c r="N37" s="15"/>
+      <c r="O37" s="15"/>
+      <c r="P37" s="17"/>
+    </row>
+    <row r="38" spans="1:16">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1593,7 +2050,7 @@
         <v>463.69020799306134</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:16">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1608,7 +2065,7 @@
         <v>510.05922879236749</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:16">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1623,7 +2080,7 @@
         <v>561.06515167160433</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:16">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1638,7 +2095,7 @@
         <v>617.17166683876485</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:16">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1653,7 +2110,7 @@
         <v>678.88883352264133</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:16">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1668,7 +2125,7 @@
         <v>746.77771687490554</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:16">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1683,7 +2140,7 @@
         <v>821.45548856239611</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:16">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1698,7 +2155,7 @@
         <v>903.60103741863577</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:16">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1713,7 +2170,7 @@
         <v>993.96114116049944</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:16">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1728,7 +2185,7 @@
         <v>1093.3572552765495</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:16">
       <c r="A48">
         <v>47</v>
       </c>

</xml_diff>

<commit_message>
added video link barplots
</commit_message>
<xml_diff>
--- a/compounding_growth_10_percent.xlsx
+++ b/compounding_growth_10_percent.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zablotski/Library/Mobile Documents/com~apple~CloudDocs/7. Hobby/programming and stats/yuzaR-Blog/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{256FE9AC-6BBE-8A4B-909A-0B502A23027D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3A452AD-AAB5-2C46-9979-4C2DD3D6B6D0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{EDD741CF-9DB9-2945-BF15-255A1807DC69}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="111">
   <si>
     <t>year</t>
   </si>
@@ -73,9 +73,6 @@
     <t>Dez</t>
   </si>
   <si>
-    <t>row_number</t>
-  </si>
-  <si>
     <t>super_thanks</t>
   </si>
   <si>
@@ -353,6 +350,15 @@
   </si>
   <si>
     <t>years_total</t>
+  </si>
+  <si>
+    <t>sponsorship</t>
+  </si>
+  <si>
+    <t>years_sponsorship</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -494,7 +500,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -513,6 +519,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -827,33 +834,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6A4B67E-A70E-FF47-86DD-9BF22E85C9FF}">
-  <dimension ref="A1:P97"/>
+  <dimension ref="A1:R97"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="144" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.1640625" customWidth="1"/>
-    <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="17" thickBot="1">
+    <row r="1" spans="1:18" ht="17" thickBot="1">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>110</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -865,43 +876,49 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
         <v>16</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
+        <v>105</v>
+      </c>
+      <c r="I1" t="s">
+        <v>108</v>
+      </c>
+      <c r="J1" t="s">
         <v>17</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" t="s">
+        <v>101</v>
+      </c>
+      <c r="M1" t="s">
+        <v>102</v>
+      </c>
+      <c r="N1" t="s">
+        <v>103</v>
+      </c>
+      <c r="O1" t="s">
+        <v>104</v>
+      </c>
+      <c r="P1" t="s">
         <v>106</v>
       </c>
-      <c r="I1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K1" t="s">
-        <v>102</v>
-      </c>
-      <c r="L1" t="s">
-        <v>103</v>
-      </c>
-      <c r="M1" t="s">
-        <v>104</v>
-      </c>
-      <c r="N1" t="s">
-        <v>105</v>
-      </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
+        <v>109</v>
+      </c>
+      <c r="R1" t="s">
         <v>107</v>
       </c>
-      <c r="P1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16">
+    </row>
+    <row r="2" spans="1:18">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -927,38 +944,44 @@
         <v>0</v>
       </c>
       <c r="I2" s="7">
+        <v>0</v>
+      </c>
+      <c r="J2" s="7">
         <f>E2+F2+G2+H2</f>
         <v>13.65</v>
       </c>
-      <c r="J2" s="8">
-        <f>I2-D2</f>
+      <c r="K2" s="8">
+        <f>J2-D2</f>
         <v>-1.3499999999999996</v>
       </c>
-      <c r="K2" s="7">
+      <c r="L2" s="7">
         <v>2023</v>
       </c>
-      <c r="L2" s="7">
+      <c r="M2" s="7">
         <f>SUM(E2:E13)</f>
-        <v>192.18</v>
-      </c>
-      <c r="M2" s="7">
+        <v>193.6</v>
+      </c>
+      <c r="N2" s="7">
         <f>SUM(F2:F13)</f>
         <v>4.93</v>
       </c>
-      <c r="N2" s="7">
+      <c r="O2" s="7">
         <f>SUM(G2:G13)</f>
         <v>38</v>
       </c>
-      <c r="O2" s="7">
+      <c r="P2" s="7">
         <f>SUM(H2:H13)</f>
         <v>250</v>
       </c>
-      <c r="P2" s="9">
-        <f>SUM(I2:I13)</f>
-        <v>485.11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16">
+      <c r="Q2" s="7">
+        <v>0</v>
+      </c>
+      <c r="R2" s="9">
+        <f>SUM(J2:J13)</f>
+        <v>486.53000000000003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
       <c r="A3" s="10">
         <v>2</v>
       </c>
@@ -984,24 +1007,28 @@
       <c r="H3" s="11">
         <v>0</v>
       </c>
-      <c r="I3" s="11">
-        <f t="shared" ref="I3:I13" si="0">E3+F3+G3+H3</f>
+      <c r="I3" s="18">
+        <v>0</v>
+      </c>
+      <c r="J3" s="11">
+        <f t="shared" ref="J3:J9" si="0">E3+F3+G3+H3</f>
         <v>28.85</v>
       </c>
-      <c r="J3" s="12">
-        <f t="shared" ref="J3:J4" si="1">I3-D3</f>
+      <c r="K3" s="12">
+        <f t="shared" ref="K3:K4" si="1">J3-D3</f>
         <v>12.350000000000001</v>
       </c>
-      <c r="K3" s="11">
+      <c r="L3" s="11">
         <v>2024</v>
       </c>
-      <c r="L3" s="11"/>
       <c r="M3" s="11"/>
       <c r="N3" s="11"/>
       <c r="O3" s="11"/>
-      <c r="P3" s="13"/>
-    </row>
-    <row r="4" spans="1:16">
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="13"/>
+    </row>
+    <row r="4" spans="1:18">
       <c r="A4" s="10">
         <v>3</v>
       </c>
@@ -1027,22 +1054,26 @@
       <c r="H4" s="11">
         <v>0</v>
       </c>
-      <c r="I4" s="11">
+      <c r="I4" s="18">
+        <v>0</v>
+      </c>
+      <c r="J4" s="11">
         <f t="shared" si="0"/>
         <v>23.52</v>
       </c>
-      <c r="J4" s="12">
+      <c r="K4" s="12">
         <f t="shared" si="1"/>
         <v>5.3699999999999974</v>
       </c>
-      <c r="K4" s="11"/>
       <c r="L4" s="11"/>
       <c r="M4" s="11"/>
       <c r="N4" s="11"/>
       <c r="O4" s="11"/>
-      <c r="P4" s="13"/>
-    </row>
-    <row r="5" spans="1:16">
+      <c r="P4" s="11"/>
+      <c r="Q4" s="11"/>
+      <c r="R4" s="13"/>
+    </row>
+    <row r="5" spans="1:18">
       <c r="A5" s="10">
         <v>4</v>
       </c>
@@ -1068,22 +1099,26 @@
       <c r="H5" s="11">
         <v>0</v>
       </c>
-      <c r="I5" s="11">
+      <c r="I5" s="18">
+        <v>0</v>
+      </c>
+      <c r="J5" s="11">
         <f t="shared" si="0"/>
         <v>43.69</v>
       </c>
-      <c r="J5" s="12">
-        <f>I5-D5</f>
+      <c r="K5" s="12">
+        <f>J5-D5</f>
         <v>23.724999999999994</v>
       </c>
-      <c r="K5" s="11"/>
       <c r="L5" s="11"/>
       <c r="M5" s="11"/>
       <c r="N5" s="11"/>
       <c r="O5" s="11"/>
-      <c r="P5" s="13"/>
-    </row>
-    <row r="6" spans="1:16">
+      <c r="P5" s="11"/>
+      <c r="Q5" s="11"/>
+      <c r="R5" s="13"/>
+    </row>
+    <row r="6" spans="1:18">
       <c r="A6" s="10">
         <v>5</v>
       </c>
@@ -1109,22 +1144,26 @@
       <c r="H6" s="11">
         <v>0</v>
       </c>
-      <c r="I6" s="11">
+      <c r="I6" s="18">
+        <v>0</v>
+      </c>
+      <c r="J6" s="11">
         <f t="shared" si="0"/>
         <v>25.88</v>
       </c>
-      <c r="J6" s="12">
-        <f>I6-D6</f>
+      <c r="K6" s="12">
+        <f>J6-D6</f>
         <v>3.9184999999999945</v>
       </c>
-      <c r="K6" s="11"/>
       <c r="L6" s="11"/>
       <c r="M6" s="11"/>
       <c r="N6" s="11"/>
       <c r="O6" s="11"/>
-      <c r="P6" s="13"/>
-    </row>
-    <row r="7" spans="1:16">
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11"/>
+      <c r="R6" s="13"/>
+    </row>
+    <row r="7" spans="1:18">
       <c r="A7" s="10">
         <v>6</v>
       </c>
@@ -1150,22 +1189,26 @@
       <c r="H7" s="11">
         <v>250</v>
       </c>
-      <c r="I7" s="11">
+      <c r="I7" s="18">
+        <v>0</v>
+      </c>
+      <c r="J7" s="11">
         <f t="shared" si="0"/>
         <v>282.27</v>
       </c>
-      <c r="J7" s="12">
-        <f>I7-D7</f>
+      <c r="K7" s="12">
+        <f>J7-D7</f>
         <v>258.11234999999999</v>
       </c>
-      <c r="K7" s="11"/>
       <c r="L7" s="11"/>
       <c r="M7" s="11"/>
       <c r="N7" s="11"/>
       <c r="O7" s="11"/>
-      <c r="P7" s="13"/>
-    </row>
-    <row r="8" spans="1:16">
+      <c r="P7" s="11"/>
+      <c r="Q7" s="11"/>
+      <c r="R7" s="13"/>
+    </row>
+    <row r="8" spans="1:18">
       <c r="A8" s="10">
         <v>7</v>
       </c>
@@ -1191,22 +1234,26 @@
       <c r="H8" s="11">
         <v>0</v>
       </c>
-      <c r="I8" s="11">
+      <c r="I8" s="18">
+        <v>0</v>
+      </c>
+      <c r="J8" s="11">
         <f t="shared" si="0"/>
         <v>35.22</v>
       </c>
-      <c r="J8" s="12">
-        <f t="shared" ref="J8:J13" si="3">I8-D8</f>
+      <c r="K8" s="12">
+        <f t="shared" ref="K8:K13" si="3">J8-D8</f>
         <v>8.6465849999999875</v>
       </c>
-      <c r="K8" s="11"/>
       <c r="L8" s="11"/>
       <c r="M8" s="11"/>
       <c r="N8" s="11"/>
       <c r="O8" s="11"/>
-      <c r="P8" s="13"/>
-    </row>
-    <row r="9" spans="1:16">
+      <c r="P8" s="11"/>
+      <c r="Q8" s="11"/>
+      <c r="R8" s="13"/>
+    </row>
+    <row r="9" spans="1:18">
       <c r="A9" s="10">
         <v>8</v>
       </c>
@@ -1221,7 +1268,7 @@
         <v>29.230756500000016</v>
       </c>
       <c r="E9" s="11">
-        <v>22.53</v>
+        <v>23.95</v>
       </c>
       <c r="F9" s="11">
         <v>0</v>
@@ -1232,22 +1279,26 @@
       <c r="H9" s="11">
         <v>0</v>
       </c>
-      <c r="I9" s="11">
+      <c r="I9" s="18">
+        <v>0</v>
+      </c>
+      <c r="J9" s="11">
         <f t="shared" si="0"/>
-        <v>32.03</v>
-      </c>
-      <c r="J9" s="12">
+        <v>33.450000000000003</v>
+      </c>
+      <c r="K9" s="12">
         <f t="shared" si="3"/>
-        <v>2.7992434999999851</v>
-      </c>
-      <c r="K9" s="11"/>
+        <v>4.2192434999999868</v>
+      </c>
       <c r="L9" s="11"/>
       <c r="M9" s="11"/>
       <c r="N9" s="11"/>
       <c r="O9" s="11"/>
-      <c r="P9" s="13"/>
-    </row>
-    <row r="10" spans="1:16">
+      <c r="P9" s="11"/>
+      <c r="Q9" s="11"/>
+      <c r="R9" s="13"/>
+    </row>
+    <row r="10" spans="1:18">
       <c r="A10" s="10">
         <v>9</v>
       </c>
@@ -1262,27 +1313,24 @@
         <v>32.153832150000021</v>
       </c>
       <c r="E10" s="11"/>
-      <c r="F10" s="11">
-        <v>0</v>
-      </c>
+      <c r="F10" s="11"/>
       <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J10" s="12">
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="12">
         <f t="shared" si="3"/>
         <v>-32.153832150000021</v>
       </c>
-      <c r="K10" s="11"/>
       <c r="L10" s="11"/>
       <c r="M10" s="11"/>
       <c r="N10" s="11"/>
       <c r="O10" s="11"/>
-      <c r="P10" s="13"/>
-    </row>
-    <row r="11" spans="1:16">
+      <c r="P10" s="11"/>
+      <c r="Q10" s="11"/>
+      <c r="R10" s="13"/>
+    </row>
+    <row r="11" spans="1:18">
       <c r="A11" s="10">
         <v>10</v>
       </c>
@@ -1297,27 +1345,24 @@
         <v>35.369215365000024</v>
       </c>
       <c r="E11" s="11"/>
-      <c r="F11" s="11">
-        <v>0</v>
-      </c>
+      <c r="F11" s="11"/>
       <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J11" s="12">
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="12">
         <f t="shared" si="3"/>
         <v>-35.369215365000024</v>
       </c>
-      <c r="K11" s="11"/>
       <c r="L11" s="11"/>
       <c r="M11" s="11"/>
       <c r="N11" s="11"/>
       <c r="O11" s="11"/>
-      <c r="P11" s="13"/>
-    </row>
-    <row r="12" spans="1:16">
+      <c r="P11" s="11"/>
+      <c r="Q11" s="11"/>
+      <c r="R11" s="13"/>
+    </row>
+    <row r="12" spans="1:18">
       <c r="A12" s="10">
         <v>11</v>
       </c>
@@ -1332,27 +1377,24 @@
         <v>38.906136901500027</v>
       </c>
       <c r="E12" s="11"/>
-      <c r="F12" s="11">
-        <v>0</v>
-      </c>
+      <c r="F12" s="11"/>
       <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J12" s="12">
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="12">
         <f t="shared" si="3"/>
         <v>-38.906136901500027</v>
       </c>
-      <c r="K12" s="11"/>
       <c r="L12" s="11"/>
       <c r="M12" s="11"/>
       <c r="N12" s="11"/>
       <c r="O12" s="11"/>
-      <c r="P12" s="13"/>
-    </row>
-    <row r="13" spans="1:16" ht="17" thickBot="1">
+      <c r="P12" s="11"/>
+      <c r="Q12" s="11"/>
+      <c r="R12" s="13"/>
+    </row>
+    <row r="13" spans="1:18" ht="17" thickBot="1">
       <c r="A13" s="14">
         <v>12</v>
       </c>
@@ -1367,27 +1409,24 @@
         <v>42.796750591650031</v>
       </c>
       <c r="E13" s="15"/>
-      <c r="F13" s="15">
-        <v>0</v>
-      </c>
+      <c r="F13" s="15"/>
       <c r="G13" s="15"/>
       <c r="H13" s="15"/>
-      <c r="I13" s="15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J13" s="16">
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="16">
         <f t="shared" si="3"/>
         <v>-42.796750591650031</v>
       </c>
-      <c r="K13" s="15"/>
       <c r="L13" s="15"/>
       <c r="M13" s="15"/>
       <c r="N13" s="15"/>
       <c r="O13" s="15"/>
-      <c r="P13" s="17"/>
-    </row>
-    <row r="14" spans="1:16">
+      <c r="P13" s="15"/>
+      <c r="Q13" s="15"/>
+      <c r="R13" s="17"/>
+    </row>
+    <row r="14" spans="1:18">
       <c r="A14" s="6">
         <v>13</v>
       </c>
@@ -1412,9 +1451,11 @@
       <c r="M14" s="7"/>
       <c r="N14" s="7"/>
       <c r="O14" s="7"/>
-      <c r="P14" s="9"/>
-    </row>
-    <row r="15" spans="1:16">
+      <c r="P14" s="7"/>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="9"/>
+    </row>
+    <row r="15" spans="1:18">
       <c r="A15" s="10">
         <v>14</v>
       </c>
@@ -1439,9 +1480,11 @@
       <c r="M15" s="11"/>
       <c r="N15" s="11"/>
       <c r="O15" s="11"/>
-      <c r="P15" s="13"/>
-    </row>
-    <row r="16" spans="1:16">
+      <c r="P15" s="11"/>
+      <c r="Q15" s="11"/>
+      <c r="R15" s="13"/>
+    </row>
+    <row r="16" spans="1:18">
       <c r="A16" s="10">
         <v>15</v>
       </c>
@@ -1466,9 +1509,11 @@
       <c r="M16" s="11"/>
       <c r="N16" s="11"/>
       <c r="O16" s="11"/>
-      <c r="P16" s="13"/>
-    </row>
-    <row r="17" spans="1:16">
+      <c r="P16" s="11"/>
+      <c r="Q16" s="11"/>
+      <c r="R16" s="13"/>
+    </row>
+    <row r="17" spans="1:18">
       <c r="A17" s="10">
         <v>16</v>
       </c>
@@ -1493,9 +1538,11 @@
       <c r="M17" s="11"/>
       <c r="N17" s="11"/>
       <c r="O17" s="11"/>
-      <c r="P17" s="13"/>
-    </row>
-    <row r="18" spans="1:16">
+      <c r="P17" s="11"/>
+      <c r="Q17" s="11"/>
+      <c r="R17" s="13"/>
+    </row>
+    <row r="18" spans="1:18">
       <c r="A18" s="10">
         <v>17</v>
       </c>
@@ -1520,9 +1567,11 @@
       <c r="M18" s="11"/>
       <c r="N18" s="11"/>
       <c r="O18" s="11"/>
-      <c r="P18" s="13"/>
-    </row>
-    <row r="19" spans="1:16">
+      <c r="P18" s="11"/>
+      <c r="Q18" s="11"/>
+      <c r="R18" s="13"/>
+    </row>
+    <row r="19" spans="1:18">
       <c r="A19" s="10">
         <v>18</v>
       </c>
@@ -1547,9 +1596,11 @@
       <c r="M19" s="11"/>
       <c r="N19" s="11"/>
       <c r="O19" s="11"/>
-      <c r="P19" s="13"/>
-    </row>
-    <row r="20" spans="1:16">
+      <c r="P19" s="11"/>
+      <c r="Q19" s="11"/>
+      <c r="R19" s="13"/>
+    </row>
+    <row r="20" spans="1:18">
       <c r="A20" s="10">
         <v>19</v>
       </c>
@@ -1574,9 +1625,11 @@
       <c r="M20" s="11"/>
       <c r="N20" s="11"/>
       <c r="O20" s="11"/>
-      <c r="P20" s="13"/>
-    </row>
-    <row r="21" spans="1:16">
+      <c r="P20" s="11"/>
+      <c r="Q20" s="11"/>
+      <c r="R20" s="13"/>
+    </row>
+    <row r="21" spans="1:18">
       <c r="A21" s="10">
         <v>20</v>
       </c>
@@ -1601,9 +1654,11 @@
       <c r="M21" s="11"/>
       <c r="N21" s="11"/>
       <c r="O21" s="11"/>
-      <c r="P21" s="13"/>
-    </row>
-    <row r="22" spans="1:16">
+      <c r="P21" s="11"/>
+      <c r="Q21" s="11"/>
+      <c r="R21" s="13"/>
+    </row>
+    <row r="22" spans="1:18">
       <c r="A22" s="10">
         <v>21</v>
       </c>
@@ -1628,9 +1683,11 @@
       <c r="M22" s="11"/>
       <c r="N22" s="11"/>
       <c r="O22" s="11"/>
-      <c r="P22" s="13"/>
-    </row>
-    <row r="23" spans="1:16">
+      <c r="P22" s="11"/>
+      <c r="Q22" s="11"/>
+      <c r="R22" s="13"/>
+    </row>
+    <row r="23" spans="1:18">
       <c r="A23" s="10">
         <v>22</v>
       </c>
@@ -1655,9 +1712,11 @@
       <c r="M23" s="11"/>
       <c r="N23" s="11"/>
       <c r="O23" s="11"/>
-      <c r="P23" s="13"/>
-    </row>
-    <row r="24" spans="1:16">
+      <c r="P23" s="11"/>
+      <c r="Q23" s="11"/>
+      <c r="R23" s="13"/>
+    </row>
+    <row r="24" spans="1:18">
       <c r="A24" s="10">
         <v>23</v>
       </c>
@@ -1682,9 +1741,11 @@
       <c r="M24" s="11"/>
       <c r="N24" s="11"/>
       <c r="O24" s="11"/>
-      <c r="P24" s="13"/>
-    </row>
-    <row r="25" spans="1:16" ht="17" thickBot="1">
+      <c r="P24" s="11"/>
+      <c r="Q24" s="11"/>
+      <c r="R24" s="13"/>
+    </row>
+    <row r="25" spans="1:18" ht="17" thickBot="1">
       <c r="A25" s="14">
         <v>24</v>
       </c>
@@ -1709,9 +1770,11 @@
       <c r="M25" s="15"/>
       <c r="N25" s="15"/>
       <c r="O25" s="15"/>
-      <c r="P25" s="17"/>
-    </row>
-    <row r="26" spans="1:16">
+      <c r="P25" s="15"/>
+      <c r="Q25" s="15"/>
+      <c r="R25" s="17"/>
+    </row>
+    <row r="26" spans="1:18">
       <c r="A26" s="6">
         <v>25</v>
       </c>
@@ -1736,9 +1799,11 @@
       <c r="M26" s="7"/>
       <c r="N26" s="7"/>
       <c r="O26" s="7"/>
-      <c r="P26" s="9"/>
-    </row>
-    <row r="27" spans="1:16">
+      <c r="P26" s="7"/>
+      <c r="Q26" s="7"/>
+      <c r="R26" s="9"/>
+    </row>
+    <row r="27" spans="1:18">
       <c r="A27" s="10">
         <v>26</v>
       </c>
@@ -1763,9 +1828,11 @@
       <c r="M27" s="11"/>
       <c r="N27" s="11"/>
       <c r="O27" s="11"/>
-      <c r="P27" s="13"/>
-    </row>
-    <row r="28" spans="1:16">
+      <c r="P27" s="11"/>
+      <c r="Q27" s="11"/>
+      <c r="R27" s="13"/>
+    </row>
+    <row r="28" spans="1:18">
       <c r="A28" s="10">
         <v>27</v>
       </c>
@@ -1790,9 +1857,11 @@
       <c r="M28" s="11"/>
       <c r="N28" s="11"/>
       <c r="O28" s="11"/>
-      <c r="P28" s="13"/>
-    </row>
-    <row r="29" spans="1:16">
+      <c r="P28" s="11"/>
+      <c r="Q28" s="11"/>
+      <c r="R28" s="13"/>
+    </row>
+    <row r="29" spans="1:18">
       <c r="A29" s="10">
         <v>28</v>
       </c>
@@ -1817,9 +1886,11 @@
       <c r="M29" s="11"/>
       <c r="N29" s="11"/>
       <c r="O29" s="11"/>
-      <c r="P29" s="13"/>
-    </row>
-    <row r="30" spans="1:16">
+      <c r="P29" s="11"/>
+      <c r="Q29" s="11"/>
+      <c r="R29" s="13"/>
+    </row>
+    <row r="30" spans="1:18">
       <c r="A30" s="10">
         <v>29</v>
       </c>
@@ -1844,9 +1915,11 @@
       <c r="M30" s="11"/>
       <c r="N30" s="11"/>
       <c r="O30" s="11"/>
-      <c r="P30" s="13"/>
-    </row>
-    <row r="31" spans="1:16">
+      <c r="P30" s="11"/>
+      <c r="Q30" s="11"/>
+      <c r="R30" s="13"/>
+    </row>
+    <row r="31" spans="1:18">
       <c r="A31" s="10">
         <v>30</v>
       </c>
@@ -1871,9 +1944,11 @@
       <c r="M31" s="11"/>
       <c r="N31" s="11"/>
       <c r="O31" s="11"/>
-      <c r="P31" s="13"/>
-    </row>
-    <row r="32" spans="1:16">
+      <c r="P31" s="11"/>
+      <c r="Q31" s="11"/>
+      <c r="R31" s="13"/>
+    </row>
+    <row r="32" spans="1:18">
       <c r="A32" s="10">
         <v>31</v>
       </c>
@@ -1898,9 +1973,11 @@
       <c r="M32" s="11"/>
       <c r="N32" s="11"/>
       <c r="O32" s="11"/>
-      <c r="P32" s="13"/>
-    </row>
-    <row r="33" spans="1:16">
+      <c r="P32" s="11"/>
+      <c r="Q32" s="11"/>
+      <c r="R32" s="13"/>
+    </row>
+    <row r="33" spans="1:18">
       <c r="A33" s="10">
         <v>32</v>
       </c>
@@ -1925,9 +2002,11 @@
       <c r="M33" s="11"/>
       <c r="N33" s="11"/>
       <c r="O33" s="11"/>
-      <c r="P33" s="13"/>
-    </row>
-    <row r="34" spans="1:16">
+      <c r="P33" s="11"/>
+      <c r="Q33" s="11"/>
+      <c r="R33" s="13"/>
+    </row>
+    <row r="34" spans="1:18">
       <c r="A34" s="10">
         <v>33</v>
       </c>
@@ -1952,9 +2031,11 @@
       <c r="M34" s="11"/>
       <c r="N34" s="11"/>
       <c r="O34" s="11"/>
-      <c r="P34" s="13"/>
-    </row>
-    <row r="35" spans="1:16">
+      <c r="P34" s="11"/>
+      <c r="Q34" s="11"/>
+      <c r="R34" s="13"/>
+    </row>
+    <row r="35" spans="1:18">
       <c r="A35" s="10">
         <v>34</v>
       </c>
@@ -1979,9 +2060,11 @@
       <c r="M35" s="11"/>
       <c r="N35" s="11"/>
       <c r="O35" s="11"/>
-      <c r="P35" s="13"/>
-    </row>
-    <row r="36" spans="1:16">
+      <c r="P35" s="11"/>
+      <c r="Q35" s="11"/>
+      <c r="R35" s="13"/>
+    </row>
+    <row r="36" spans="1:18">
       <c r="A36" s="10">
         <v>35</v>
       </c>
@@ -2006,9 +2089,11 @@
       <c r="M36" s="11"/>
       <c r="N36" s="11"/>
       <c r="O36" s="11"/>
-      <c r="P36" s="13"/>
-    </row>
-    <row r="37" spans="1:16" ht="17" thickBot="1">
+      <c r="P36" s="11"/>
+      <c r="Q36" s="11"/>
+      <c r="R36" s="13"/>
+    </row>
+    <row r="37" spans="1:18" ht="17" thickBot="1">
       <c r="A37" s="14">
         <v>36</v>
       </c>
@@ -2033,9 +2118,11 @@
       <c r="M37" s="15"/>
       <c r="N37" s="15"/>
       <c r="O37" s="15"/>
-      <c r="P37" s="17"/>
-    </row>
-    <row r="38" spans="1:16">
+      <c r="P37" s="15"/>
+      <c r="Q37" s="15"/>
+      <c r="R37" s="17"/>
+    </row>
+    <row r="38" spans="1:18">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2050,7 +2137,7 @@
         <v>463.69020799306134</v>
       </c>
     </row>
-    <row r="39" spans="1:16">
+    <row r="39" spans="1:18">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2065,7 +2152,7 @@
         <v>510.05922879236749</v>
       </c>
     </row>
-    <row r="40" spans="1:16">
+    <row r="40" spans="1:18">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2080,7 +2167,7 @@
         <v>561.06515167160433</v>
       </c>
     </row>
-    <row r="41" spans="1:16">
+    <row r="41" spans="1:18">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2095,7 +2182,7 @@
         <v>617.17166683876485</v>
       </c>
     </row>
-    <row r="42" spans="1:16">
+    <row r="42" spans="1:18">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2110,7 +2197,7 @@
         <v>678.88883352264133</v>
       </c>
     </row>
-    <row r="43" spans="1:16">
+    <row r="43" spans="1:18">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2125,7 +2212,7 @@
         <v>746.77771687490554</v>
       </c>
     </row>
-    <row r="44" spans="1:16">
+    <row r="44" spans="1:18">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2140,7 +2227,7 @@
         <v>821.45548856239611</v>
       </c>
     </row>
-    <row r="45" spans="1:16">
+    <row r="45" spans="1:18">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2155,7 +2242,7 @@
         <v>903.60103741863577</v>
       </c>
     </row>
-    <row r="46" spans="1:16">
+    <row r="46" spans="1:18">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2170,7 +2257,7 @@
         <v>993.96114116049944</v>
       </c>
     </row>
-    <row r="47" spans="1:16">
+    <row r="47" spans="1:18">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2185,7 +2272,7 @@
         <v>1093.3572552765495</v>
       </c>
     </row>
-    <row r="48" spans="1:16">
+    <row r="48" spans="1:18">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2959,461 +3046,461 @@
   <sheetData>
     <row r="1" spans="1:5" ht="17">
       <c r="A1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="18">
       <c r="A2" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" s="4">
         <v>823</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="18">
       <c r="A3" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" s="4">
         <v>301</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>32</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="17">
       <c r="A4" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B4" s="5">
         <v>246</v>
       </c>
       <c r="C4" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>36</v>
-      </c>
       <c r="E4" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="17">
       <c r="A5" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5" s="5">
         <v>246</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>36</v>
-      </c>
       <c r="E5" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="17">
       <c r="A6" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B6" s="5">
         <v>135</v>
       </c>
       <c r="C6" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>40</v>
-      </c>
       <c r="E6" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="18">
       <c r="A7" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B7" s="4">
         <v>110</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>43</v>
-      </c>
       <c r="E7" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="17">
       <c r="A8" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8" s="5">
         <v>110</v>
       </c>
       <c r="C8" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>46</v>
-      </c>
       <c r="E8" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="17">
       <c r="A9" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B9" s="5">
         <v>110</v>
       </c>
       <c r="C9" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>46</v>
-      </c>
       <c r="E9" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="17">
       <c r="A10" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B10" s="5">
         <v>110</v>
       </c>
       <c r="C10" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>50</v>
-      </c>
       <c r="E10" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="17">
       <c r="A11" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B11" s="5">
         <v>90.5</v>
       </c>
       <c r="C11" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>53</v>
-      </c>
       <c r="E11" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="17">
       <c r="A12" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B12" s="5">
         <v>74</v>
       </c>
       <c r="C12" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>56</v>
-      </c>
       <c r="E12" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="17">
       <c r="A13" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B13" s="5">
         <v>60.5</v>
       </c>
       <c r="C13" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>59</v>
-      </c>
       <c r="E13" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="17">
       <c r="A14" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B14" s="5">
         <v>60.5</v>
       </c>
       <c r="C14" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="D14" s="5" t="s">
-        <v>62</v>
-      </c>
       <c r="E14" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="17">
       <c r="A15" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B15" s="5">
         <v>49.5</v>
       </c>
       <c r="C15" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="D15" s="5" t="s">
-        <v>65</v>
-      </c>
       <c r="E15" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="17">
       <c r="A16" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B16" s="5">
         <v>33.1</v>
       </c>
       <c r="C16" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="D16" s="5" t="s">
-        <v>68</v>
-      </c>
       <c r="E16" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="17">
       <c r="A17" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B17" s="5">
         <v>33.1</v>
       </c>
       <c r="C17" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="D17" s="5" t="s">
-        <v>71</v>
-      </c>
       <c r="E17" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="17">
       <c r="A18" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B18" s="5">
         <v>27.1</v>
       </c>
       <c r="C18" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D18" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="D18" s="5" t="s">
-        <v>74</v>
-      </c>
       <c r="E18" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="17">
       <c r="A19" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B19" s="5">
         <v>27.1</v>
       </c>
       <c r="C19" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="D19" s="5" t="s">
-        <v>77</v>
-      </c>
       <c r="E19" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="17">
       <c r="A20" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B20" s="5">
         <v>27.1</v>
       </c>
       <c r="C20" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="D20" s="5" t="s">
-        <v>80</v>
-      </c>
       <c r="E20" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="17">
       <c r="A21" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B21" s="5">
         <v>9.9</v>
       </c>
       <c r="C21" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D21" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="D21" s="5" t="s">
-        <v>83</v>
-      </c>
       <c r="E21" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="17">
       <c r="A22" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B22" s="5">
         <v>6.6</v>
       </c>
       <c r="C22" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D22" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="D22" s="5" t="s">
-        <v>86</v>
-      </c>
       <c r="E22" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="17">
       <c r="A23" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B23" s="5">
         <v>6.6</v>
       </c>
       <c r="C23" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D23" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="D23" s="5" t="s">
-        <v>89</v>
-      </c>
       <c r="E23" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="17">
       <c r="A24" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B24" s="5">
         <v>5.4</v>
       </c>
       <c r="C24" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D24" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="D24" s="5" t="s">
-        <v>92</v>
-      </c>
       <c r="E24" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="17">
       <c r="A25" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B25" s="5">
         <v>5.4</v>
       </c>
       <c r="C25" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D25" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="D25" s="5" t="s">
-        <v>95</v>
-      </c>
       <c r="E25" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="17">
       <c r="A26" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B26" s="5">
         <v>4.4000000000000004</v>
       </c>
       <c r="C26" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D26" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="D26" s="5" t="s">
-        <v>98</v>
-      </c>
       <c r="E26" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="17">
       <c r="A27" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B27" s="5">
         <v>4.4000000000000004</v>
       </c>
       <c r="C27" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D27" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="D27" s="5" t="s">
-        <v>101</v>
-      </c>
       <c r="E27" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
link for glmulti video
</commit_message>
<xml_diff>
--- a/compounding_growth_10_percent.xlsx
+++ b/compounding_growth_10_percent.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zablotski/Library/Mobile Documents/com~apple~CloudDocs/7. Hobby/programming and stats/yuzaR-Blog/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C4EA502-2A17-F444-88A0-0AC49DE02AD0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{029DC7BC-CA1A-E448-8F16-3DADC3FE454B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{EDD741CF-9DB9-2945-BF15-255A1807DC69}"/>
   </bookViews>
@@ -927,7 +927,7 @@
   <dimension ref="A1:R97"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="144" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1049,7 +1049,7 @@
       </c>
       <c r="M2" s="7">
         <f>SUM(E2:E13)</f>
-        <v>241.82</v>
+        <v>285.83999999999997</v>
       </c>
       <c r="N2" s="7">
         <f>SUM(F2:F13)</f>
@@ -1068,7 +1068,7 @@
       </c>
       <c r="R2" s="9">
         <f>SUM(J2:J13)</f>
-        <v>534.75000000000011</v>
+        <v>578.7700000000001</v>
       </c>
     </row>
     <row r="3" spans="1:18">
@@ -1101,7 +1101,7 @@
         <v>0</v>
       </c>
       <c r="J3" s="11">
-        <f t="shared" ref="J3:J10" si="0">E3+F3+G3+H3</f>
+        <f t="shared" ref="J3:J13" si="0">E3+F3+G3+H3</f>
         <v>28.85</v>
       </c>
       <c r="K3" s="12">
@@ -1403,7 +1403,7 @@
         <v>32.153832150000021</v>
       </c>
       <c r="E10" s="18">
-        <v>27.32</v>
+        <v>45.64</v>
       </c>
       <c r="F10" s="18">
         <v>0</v>
@@ -1419,11 +1419,11 @@
       </c>
       <c r="J10" s="18">
         <f t="shared" si="0"/>
-        <v>27.32</v>
+        <v>45.64</v>
       </c>
       <c r="K10" s="12">
         <f t="shared" si="3"/>
-        <v>-4.8338321500000205</v>
+        <v>13.48616784999998</v>
       </c>
       <c r="L10" s="11"/>
       <c r="M10" s="11"/>
@@ -1447,15 +1447,20 @@
         <f t="shared" si="2"/>
         <v>35.369215365000024</v>
       </c>
-      <c r="E11" s="11"/>
+      <c r="E11" s="18">
+        <v>25.7</v>
+      </c>
       <c r="F11" s="11"/>
       <c r="G11" s="11"/>
       <c r="H11" s="18"/>
       <c r="I11" s="18"/>
-      <c r="J11" s="11"/>
+      <c r="J11" s="18">
+        <f t="shared" si="0"/>
+        <v>25.7</v>
+      </c>
       <c r="K11" s="12">
         <f t="shared" si="3"/>
-        <v>-35.369215365000024</v>
+        <v>-9.6692153650000243</v>
       </c>
       <c r="L11" s="11"/>
       <c r="M11" s="11"/>
@@ -1484,7 +1489,10 @@
       <c r="G12" s="11"/>
       <c r="H12" s="18"/>
       <c r="I12" s="18"/>
-      <c r="J12" s="11"/>
+      <c r="J12" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="K12" s="12">
         <f t="shared" si="3"/>
         <v>-38.906136901500027</v>
@@ -1516,7 +1524,10 @@
       <c r="G13" s="15"/>
       <c r="H13" s="15"/>
       <c r="I13" s="15"/>
-      <c r="J13" s="15"/>
+      <c r="J13" s="18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="K13" s="16">
         <f t="shared" si="3"/>
         <v>-42.796750591650031</v>

</xml_diff>

<commit_message>
youtube link for scatter plot blog
</commit_message>
<xml_diff>
--- a/compounding_growth_10_percent.xlsx
+++ b/compounding_growth_10_percent.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zablotski/Library/Mobile Documents/com~apple~CloudDocs/7. Hobby/programming and stats/yuzaR-Blog/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{029DC7BC-CA1A-E448-8F16-3DADC3FE454B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{508A28C7-8583-9240-A3D9-7A8695F64164}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{EDD741CF-9DB9-2945-BF15-255A1807DC69}"/>
   </bookViews>
@@ -927,7 +927,7 @@
   <dimension ref="A1:R97"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="144" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1049,7 +1049,7 @@
       </c>
       <c r="M2" s="7">
         <f>SUM(E2:E13)</f>
-        <v>285.83999999999997</v>
+        <v>297.93</v>
       </c>
       <c r="N2" s="7">
         <f>SUM(F2:F13)</f>
@@ -1068,7 +1068,7 @@
       </c>
       <c r="R2" s="9">
         <f>SUM(J2:J13)</f>
-        <v>578.7700000000001</v>
+        <v>590.86</v>
       </c>
     </row>
     <row r="3" spans="1:18">
@@ -1448,7 +1448,7 @@
         <v>35.369215365000024</v>
       </c>
       <c r="E11" s="18">
-        <v>25.7</v>
+        <v>37.79</v>
       </c>
       <c r="F11" s="11"/>
       <c r="G11" s="11"/>
@@ -1456,11 +1456,11 @@
       <c r="I11" s="18"/>
       <c r="J11" s="18">
         <f t="shared" si="0"/>
-        <v>25.7</v>
+        <v>37.79</v>
       </c>
       <c r="K11" s="12">
         <f t="shared" si="3"/>
-        <v>-9.6692153650000243</v>
+        <v>2.4207846349999755</v>
       </c>
       <c r="L11" s="11"/>
       <c r="M11" s="11"/>

</xml_diff>

<commit_message>
new mac blog offline first trial
</commit_message>
<xml_diff>
--- a/compounding_growth_10_percent.xlsx
+++ b/compounding_growth_10_percent.xlsx
@@ -1,32 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zablotski/Library/Mobile Documents/com~apple~CloudDocs/7. Hobby/programming and stats/yuzaR-Blog/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85F4E70E-57C0-F749-8EA5-D9B38CCAD9D3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CA4CE6C-BC0C-FF4D-B2A7-01313168F1BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{EDD741CF-9DB9-2945-BF15-255A1807DC69}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="33600" windowHeight="20060" xr2:uid="{EDD741CF-9DB9-2945-BF15-255A1807DC69}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="keywords" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="113">
   <si>
     <t>year</t>
   </si>
@@ -359,6 +370,12 @@
   </si>
   <si>
     <t>id</t>
+  </si>
+  <si>
+    <t>years_total_projected</t>
+  </si>
+  <si>
+    <t>YOY GROWTH</t>
   </si>
 </sst>
 </file>
@@ -592,14 +609,11 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -610,6 +624,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" indent="4"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -667,7 +688,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-DE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -729,7 +750,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="de-DE"/>
+                <a:endParaRPr lang="en-DE"/>
               </a:p>
             </c:txPr>
             <c:showLegendKey val="0"/>
@@ -761,10 +782,10 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$13</c:f>
+              <c:f>Sheet1!$D$2:$D$16</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>15</c:v>
                 </c:pt>
@@ -800,6 +821,15 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>42.796750591650031</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>47.07642565081504</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>51.784068215896546</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>56.962475037486207</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -861,7 +891,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="de-DE"/>
+                <a:endParaRPr lang="en-DE"/>
               </a:p>
             </c:txPr>
             <c:showLegendKey val="0"/>
@@ -893,10 +923,10 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$2:$E$13</c:f>
+              <c:f>Sheet1!$E$2:$E$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>13.65</c:v>
                 </c:pt>
@@ -931,7 +961,10 @@
                   <c:v>63.76</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>48</c:v>
+                  <c:v>48.01</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>42.62</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -995,7 +1028,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-DE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1629694368"/>
@@ -1055,7 +1088,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-DE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1092,7 +1125,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1652,16 +1685,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>721430</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>202670</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>141110</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>79374</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>784929</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>167569</xdr:rowOff>
+      <xdr:colOff>670276</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>176388</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1986,9 +2019,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6A4B67E-A70E-FF47-86DD-9BF22E85C9FF}">
-  <dimension ref="A1:R97"/>
+  <dimension ref="A1:T97"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="144" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -2012,65 +2045,73 @@
     <col min="16" max="16" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="17" thickBot="1">
-      <c r="A1" t="s">
+    <row r="1" spans="1:20" ht="17" thickBot="1">
+      <c r="A1" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="B1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="9" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="2" spans="1:18">
+      <c r="S1" t="s">
+        <v>111</v>
+      </c>
+      <c r="T1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="17" thickBot="1">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -2111,7 +2152,7 @@
       </c>
       <c r="M2" s="7">
         <f>SUM(E2:E13)</f>
-        <v>421.46</v>
+        <v>421.46999999999997</v>
       </c>
       <c r="N2" s="7">
         <f>SUM(F2:F13)</f>
@@ -2130,495 +2171,504 @@
       </c>
       <c r="R2" s="9">
         <f>SUM(J2:J13)</f>
-        <v>714.3900000000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18">
+        <v>714.40000000000009</v>
+      </c>
+      <c r="S2" s="27">
+        <f>SUM(D2:D13)</f>
+        <v>320.76425650815014</v>
+      </c>
+      <c r="T2" s="28">
+        <f>(S3*100)/S2</f>
+        <v>313.84283767210036</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20">
       <c r="A3" s="10">
         <v>2</v>
       </c>
-      <c r="B3" s="11">
+      <c r="B3">
         <v>2023</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="12">
+      <c r="D3" s="1">
         <f>D2*1.1</f>
         <v>16.5</v>
       </c>
-      <c r="E3" s="11">
+      <c r="E3">
         <v>23.92</v>
       </c>
-      <c r="F3" s="11">
+      <c r="F3">
         <v>4.93</v>
       </c>
-      <c r="G3" s="11">
-        <v>0</v>
-      </c>
-      <c r="H3" s="11">
-        <v>0</v>
-      </c>
-      <c r="I3" s="18">
-        <v>0</v>
-      </c>
-      <c r="J3" s="11">
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
         <f t="shared" ref="J3:J13" si="0">E3+F3+G3+H3</f>
         <v>28.85</v>
       </c>
-      <c r="K3" s="12">
+      <c r="K3" s="1">
         <f t="shared" ref="K3:K4" si="1">J3-D3</f>
         <v>12.350000000000001</v>
       </c>
-      <c r="L3" s="11">
+      <c r="L3">
         <v>2024</v>
       </c>
-      <c r="M3" s="11"/>
-      <c r="N3" s="11"/>
-      <c r="O3" s="11"/>
-      <c r="P3" s="11"/>
-      <c r="Q3" s="11"/>
-      <c r="R3" s="13"/>
-    </row>
-    <row r="4" spans="1:18">
+      <c r="M3" s="7">
+        <f>SUM(E14:E25)</f>
+        <v>42.62</v>
+      </c>
+      <c r="N3" s="7">
+        <f t="shared" ref="N3:R3" si="2">SUM(F14:F25)</f>
+        <v>0</v>
+      </c>
+      <c r="O3" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P3" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q3" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R3" s="9">
+        <f t="shared" si="2"/>
+        <v>42.62</v>
+      </c>
+      <c r="S3" s="27">
+        <f>SUM(D14:D25)</f>
+        <v>1006.6956448629932</v>
+      </c>
+      <c r="T3" s="27">
+        <f t="shared" ref="T3:T4" si="3">(S4*100)/S3</f>
+        <v>313.8428376721003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20">
       <c r="A4" s="10">
         <v>3</v>
       </c>
-      <c r="B4" s="11">
+      <c r="B4">
         <v>2023</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="1">
         <f>D3*1.1</f>
         <v>18.150000000000002</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E4">
         <v>23.52</v>
       </c>
-      <c r="F4" s="11">
-        <v>0</v>
-      </c>
-      <c r="G4" s="11">
-        <v>0</v>
-      </c>
-      <c r="H4" s="11">
-        <v>0</v>
-      </c>
-      <c r="I4" s="18">
-        <v>0</v>
-      </c>
-      <c r="J4" s="11">
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
         <f t="shared" si="0"/>
         <v>23.52</v>
       </c>
-      <c r="K4" s="12">
+      <c r="K4" s="1">
         <f t="shared" si="1"/>
         <v>5.3699999999999974</v>
       </c>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="11"/>
-      <c r="O4" s="11"/>
-      <c r="P4" s="11"/>
-      <c r="Q4" s="11"/>
-      <c r="R4" s="13"/>
-    </row>
-    <row r="5" spans="1:18">
+      <c r="R4" s="11"/>
+      <c r="S4" s="27">
+        <f>SUM(D26:D37)</f>
+        <v>3159.4421785594668</v>
+      </c>
+      <c r="T4" s="27">
+        <f t="shared" si="3"/>
+        <v>313.84283767210019</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20">
       <c r="A5" s="10">
         <v>4</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B5">
         <v>2023</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="1">
         <f>D4*1.1</f>
         <v>19.965000000000003</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E5">
         <v>24.69</v>
       </c>
-      <c r="F5" s="11">
-        <v>0</v>
-      </c>
-      <c r="G5" s="11">
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
         <v>19</v>
       </c>
-      <c r="H5" s="11">
-        <v>0</v>
-      </c>
-      <c r="I5" s="18">
-        <v>0</v>
-      </c>
-      <c r="J5" s="11">
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
         <f t="shared" si="0"/>
         <v>43.69</v>
       </c>
-      <c r="K5" s="12">
+      <c r="K5" s="1">
         <f>J5-D5</f>
         <v>23.724999999999994</v>
       </c>
-      <c r="L5" s="11"/>
-      <c r="M5" s="11"/>
-      <c r="N5" s="11"/>
-      <c r="O5" s="11"/>
-      <c r="P5" s="11"/>
-      <c r="Q5" s="11"/>
-      <c r="R5" s="13"/>
-    </row>
-    <row r="6" spans="1:18">
+      <c r="R5" s="11"/>
+      <c r="S5" s="27">
+        <f>SUM(D38:D49)</f>
+        <v>9915.6829878002536</v>
+      </c>
+      <c r="T5" s="26"/>
+    </row>
+    <row r="6" spans="1:20">
       <c r="A6" s="10">
         <v>5</v>
       </c>
-      <c r="B6" s="11">
+      <c r="B6">
         <v>2023</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="12">
-        <f t="shared" ref="D6:D69" si="2">D5*1.1</f>
+      <c r="D6" s="1">
+        <f t="shared" ref="D6:D69" si="4">D5*1.1</f>
         <v>21.961500000000004</v>
       </c>
-      <c r="E6" s="11">
+      <c r="E6">
         <v>25.88</v>
       </c>
-      <c r="F6" s="11">
-        <v>0</v>
-      </c>
-      <c r="G6" s="11">
-        <v>0</v>
-      </c>
-      <c r="H6" s="11">
-        <v>0</v>
-      </c>
-      <c r="I6" s="18">
-        <v>0</v>
-      </c>
-      <c r="J6" s="11">
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
         <f t="shared" si="0"/>
         <v>25.88</v>
       </c>
-      <c r="K6" s="12">
+      <c r="K6" s="1">
         <f>J6-D6</f>
         <v>3.9184999999999945</v>
       </c>
-      <c r="L6" s="11"/>
-      <c r="M6" s="11"/>
-      <c r="N6" s="11"/>
-      <c r="O6" s="11"/>
-      <c r="P6" s="11"/>
-      <c r="Q6" s="11"/>
-      <c r="R6" s="13"/>
-    </row>
-    <row r="7" spans="1:18">
+      <c r="R6" s="11"/>
+      <c r="S6" s="27">
+        <f>SUM(D50:D61)</f>
+        <v>31119.66086348203</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20">
       <c r="A7" s="10">
         <v>6</v>
       </c>
-      <c r="B7" s="11">
+      <c r="B7">
         <v>2023</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="12">
-        <f t="shared" si="2"/>
+      <c r="D7" s="1">
+        <f t="shared" si="4"/>
         <v>24.157650000000007</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7">
         <v>22.77</v>
       </c>
-      <c r="F7" s="11">
-        <v>0</v>
-      </c>
-      <c r="G7" s="11">
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
         <v>9.5</v>
       </c>
-      <c r="H7" s="11">
+      <c r="H7">
         <v>250</v>
       </c>
-      <c r="I7" s="18">
-        <v>0</v>
-      </c>
-      <c r="J7" s="11">
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
         <f t="shared" si="0"/>
         <v>282.27</v>
       </c>
-      <c r="K7" s="12">
+      <c r="K7" s="1">
         <f>J7-D7</f>
         <v>258.11234999999999</v>
       </c>
-      <c r="L7" s="11"/>
-      <c r="M7" s="11"/>
-      <c r="N7" s="11"/>
-      <c r="O7" s="11"/>
-      <c r="P7" s="11"/>
-      <c r="Q7" s="11"/>
-      <c r="R7" s="13"/>
-    </row>
-    <row r="8" spans="1:18">
+      <c r="R7" s="11"/>
+    </row>
+    <row r="8" spans="1:20">
       <c r="A8" s="10">
         <v>7</v>
       </c>
-      <c r="B8" s="11">
+      <c r="B8">
         <v>2023</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="12">
-        <f t="shared" si="2"/>
+      <c r="D8" s="1">
+        <f t="shared" si="4"/>
         <v>26.573415000000011</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E8">
         <v>35.22</v>
       </c>
-      <c r="F8" s="11">
-        <v>0</v>
-      </c>
-      <c r="G8" s="11">
-        <v>0</v>
-      </c>
-      <c r="H8" s="11">
-        <v>0</v>
-      </c>
-      <c r="I8" s="18">
-        <v>0</v>
-      </c>
-      <c r="J8" s="11">
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
         <f t="shared" si="0"/>
         <v>35.22</v>
       </c>
-      <c r="K8" s="12">
-        <f t="shared" ref="K8:K13" si="3">J8-D8</f>
+      <c r="K8" s="1">
+        <f t="shared" ref="K8:K13" si="5">J8-D8</f>
         <v>8.6465849999999875</v>
       </c>
-      <c r="L8" s="11"/>
-      <c r="M8" s="11"/>
-      <c r="N8" s="11"/>
-      <c r="O8" s="11"/>
-      <c r="P8" s="11"/>
-      <c r="Q8" s="11"/>
-      <c r="R8" s="13"/>
-    </row>
-    <row r="9" spans="1:18">
+      <c r="R8" s="11"/>
+    </row>
+    <row r="9" spans="1:20">
       <c r="A9" s="10">
         <v>8</v>
       </c>
-      <c r="B9" s="11">
+      <c r="B9">
         <v>2023</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="12">
-        <f t="shared" si="2"/>
+      <c r="D9" s="1">
+        <f t="shared" si="4"/>
         <v>29.230756500000016</v>
       </c>
-      <c r="E9" s="11">
+      <c r="E9">
         <v>44.85</v>
       </c>
-      <c r="F9" s="11">
-        <v>0</v>
-      </c>
-      <c r="G9" s="11">
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
         <v>9.5</v>
       </c>
-      <c r="H9" s="11">
-        <v>0</v>
-      </c>
-      <c r="I9" s="18">
-        <v>0</v>
-      </c>
-      <c r="J9" s="11">
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
         <f t="shared" si="0"/>
         <v>54.35</v>
       </c>
-      <c r="K9" s="12">
-        <f t="shared" si="3"/>
+      <c r="K9" s="1">
+        <f t="shared" si="5"/>
         <v>25.119243499999985</v>
       </c>
-      <c r="L9" s="11"/>
-      <c r="M9" s="11"/>
-      <c r="N9" s="11"/>
-      <c r="O9" s="11"/>
-      <c r="P9" s="11"/>
-      <c r="Q9" s="11"/>
-      <c r="R9" s="13"/>
-    </row>
-    <row r="10" spans="1:18">
+      <c r="R9" s="11"/>
+    </row>
+    <row r="10" spans="1:20">
       <c r="A10" s="10">
         <v>9</v>
       </c>
-      <c r="B10" s="11">
+      <c r="B10">
         <v>2023</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="12">
-        <f t="shared" si="2"/>
+      <c r="D10" s="1">
+        <f t="shared" si="4"/>
         <v>32.153832150000021</v>
       </c>
-      <c r="E10" s="18">
+      <c r="E10">
         <v>45.64</v>
       </c>
-      <c r="F10" s="18">
-        <v>0</v>
-      </c>
-      <c r="G10" s="18">
-        <v>0</v>
-      </c>
-      <c r="H10" s="18">
-        <v>0</v>
-      </c>
-      <c r="I10" s="18">
-        <v>0</v>
-      </c>
-      <c r="J10" s="18">
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
         <f t="shared" si="0"/>
         <v>45.64</v>
       </c>
-      <c r="K10" s="12">
-        <f t="shared" si="3"/>
+      <c r="K10" s="1">
+        <f t="shared" si="5"/>
         <v>13.48616784999998</v>
       </c>
-      <c r="L10" s="11"/>
-      <c r="M10" s="11"/>
-      <c r="N10" s="11"/>
-      <c r="O10" s="11"/>
-      <c r="P10" s="11"/>
-      <c r="Q10" s="11"/>
-      <c r="R10" s="13"/>
-    </row>
-    <row r="11" spans="1:18">
+      <c r="R10" s="11"/>
+    </row>
+    <row r="11" spans="1:20">
       <c r="A11" s="10">
         <v>10</v>
       </c>
-      <c r="B11" s="11">
+      <c r="B11">
         <v>2023</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="12">
-        <f t="shared" si="2"/>
+      <c r="D11" s="1">
+        <f t="shared" si="4"/>
         <v>35.369215365000024</v>
       </c>
-      <c r="E11" s="18">
+      <c r="E11">
         <v>49.56</v>
       </c>
-      <c r="F11" s="18">
-        <v>0</v>
-      </c>
-      <c r="G11" s="18">
-        <v>0</v>
-      </c>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18">
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
         <f t="shared" si="0"/>
         <v>49.56</v>
       </c>
-      <c r="K11" s="12">
-        <f t="shared" si="3"/>
+      <c r="K11" s="1">
+        <f t="shared" si="5"/>
         <v>14.190784634999979</v>
       </c>
-      <c r="L11" s="11"/>
-      <c r="M11" s="11"/>
-      <c r="N11" s="11"/>
-      <c r="O11" s="11"/>
-      <c r="P11" s="11"/>
-      <c r="Q11" s="11"/>
-      <c r="R11" s="13"/>
-    </row>
-    <row r="12" spans="1:18">
+      <c r="R11" s="11"/>
+    </row>
+    <row r="12" spans="1:20">
       <c r="A12" s="10">
         <v>11</v>
       </c>
-      <c r="B12" s="11">
+      <c r="B12">
         <v>2023</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="12">
-        <f t="shared" si="2"/>
+      <c r="D12" s="1">
+        <f t="shared" si="4"/>
         <v>38.906136901500027</v>
       </c>
-      <c r="E12" s="18">
+      <c r="E12">
         <v>63.76</v>
       </c>
-      <c r="F12" s="18">
-        <v>0</v>
-      </c>
-      <c r="G12" s="18">
-        <v>0</v>
-      </c>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18">
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
         <f t="shared" si="0"/>
         <v>63.76</v>
       </c>
-      <c r="K12" s="12">
-        <f t="shared" si="3"/>
+      <c r="K12" s="1">
+        <f t="shared" si="5"/>
         <v>24.853863098499971</v>
       </c>
-      <c r="L12" s="11"/>
-      <c r="M12" s="11"/>
-      <c r="N12" s="11"/>
-      <c r="O12" s="11"/>
-      <c r="P12" s="11"/>
-      <c r="Q12" s="11"/>
-      <c r="R12" s="13"/>
-    </row>
-    <row r="13" spans="1:18" ht="17" thickBot="1">
-      <c r="A13" s="14">
+      <c r="R12" s="11"/>
+    </row>
+    <row r="13" spans="1:20" ht="17" thickBot="1">
+      <c r="A13" s="12">
         <v>12</v>
       </c>
-      <c r="B13" s="15">
+      <c r="B13" s="13">
         <v>2023</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="16">
-        <f t="shared" si="2"/>
+      <c r="D13" s="14">
+        <f t="shared" si="4"/>
         <v>42.796750591650031</v>
       </c>
-      <c r="E13" s="15">
-        <v>48</v>
-      </c>
-      <c r="F13" s="15">
-        <v>0</v>
-      </c>
-      <c r="G13" s="15">
-        <v>0</v>
-      </c>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="18">
+      <c r="E13" s="13">
+        <v>48.01</v>
+      </c>
+      <c r="F13" s="13">
+        <v>0</v>
+      </c>
+      <c r="G13" s="13">
+        <v>0</v>
+      </c>
+      <c r="H13" s="13">
+        <v>0</v>
+      </c>
+      <c r="I13" s="13">
+        <v>0</v>
+      </c>
+      <c r="J13" s="13">
         <f t="shared" si="0"/>
-        <v>48</v>
-      </c>
-      <c r="K13" s="16">
-        <f t="shared" si="3"/>
-        <v>5.2032494083499685</v>
-      </c>
-      <c r="L13" s="15"/>
-      <c r="M13" s="15"/>
-      <c r="N13" s="15"/>
-      <c r="O13" s="15"/>
-      <c r="P13" s="15"/>
-      <c r="Q13" s="15"/>
-      <c r="R13" s="17"/>
-    </row>
-    <row r="14" spans="1:18">
+        <v>48.01</v>
+      </c>
+      <c r="K13" s="14">
+        <f t="shared" si="5"/>
+        <v>5.2132494083499665</v>
+      </c>
+      <c r="L13" s="13"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="13"/>
+      <c r="O13" s="13"/>
+      <c r="P13" s="13"/>
+      <c r="Q13" s="13"/>
+      <c r="R13" s="15"/>
+    </row>
+    <row r="14" spans="1:20">
       <c r="A14" s="6">
         <v>13</v>
       </c>
@@ -2629,16 +2679,32 @@
         <v>3</v>
       </c>
       <c r="D14" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>47.07642565081504</v>
       </c>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
+      <c r="E14" s="7">
+        <v>42.62</v>
+      </c>
+      <c r="F14" s="7">
+        <v>0</v>
+      </c>
+      <c r="G14" s="7">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <f t="shared" ref="J14:J25" si="6">E14+F14+G14+H14</f>
+        <v>42.62</v>
+      </c>
+      <c r="K14" s="8">
+        <f t="shared" ref="K14:K25" si="7">J14-D14</f>
+        <v>-4.4564256508150422</v>
+      </c>
       <c r="L14" s="7"/>
       <c r="M14" s="7"/>
       <c r="N14" s="7"/>
@@ -2647,346 +2713,423 @@
       <c r="Q14" s="7"/>
       <c r="R14" s="9"/>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:20">
       <c r="A15" s="10">
         <v>14</v>
       </c>
-      <c r="B15" s="11">
+      <c r="B15">
         <v>2024</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" t="s">
         <v>4</v>
       </c>
-      <c r="D15" s="12">
-        <f t="shared" si="2"/>
+      <c r="D15" s="1">
+        <f t="shared" si="4"/>
         <v>51.784068215896546</v>
       </c>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="11"/>
-      <c r="L15" s="11"/>
-      <c r="M15" s="11"/>
-      <c r="N15" s="11"/>
-      <c r="O15" s="11"/>
-      <c r="P15" s="11"/>
-      <c r="Q15" s="11"/>
-      <c r="R15" s="13"/>
-    </row>
-    <row r="16" spans="1:18">
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K15" s="1">
+        <f t="shared" si="7"/>
+        <v>-51.784068215896546</v>
+      </c>
+      <c r="R15" s="11"/>
+    </row>
+    <row r="16" spans="1:20">
       <c r="A16" s="10">
         <v>15</v>
       </c>
-      <c r="B16" s="11">
+      <c r="B16">
         <v>2024</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="12">
-        <f t="shared" si="2"/>
+      <c r="D16" s="1">
+        <f t="shared" si="4"/>
         <v>56.962475037486207</v>
       </c>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="11"/>
-      <c r="L16" s="11"/>
-      <c r="M16" s="11"/>
-      <c r="N16" s="11"/>
-      <c r="O16" s="11"/>
-      <c r="P16" s="11"/>
-      <c r="Q16" s="11"/>
-      <c r="R16" s="13"/>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K16" s="1">
+        <f t="shared" si="7"/>
+        <v>-56.962475037486207</v>
+      </c>
+      <c r="R16" s="11"/>
     </row>
     <row r="17" spans="1:18">
       <c r="A17" s="10">
         <v>16</v>
       </c>
-      <c r="B17" s="11">
+      <c r="B17">
         <v>2024</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="12">
-        <f t="shared" si="2"/>
+      <c r="D17" s="1">
+        <f t="shared" si="4"/>
         <v>62.65872254123483</v>
       </c>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="11"/>
-      <c r="K17" s="11"/>
-      <c r="L17" s="11"/>
-      <c r="M17" s="11"/>
-      <c r="N17" s="11"/>
-      <c r="O17" s="11"/>
-      <c r="P17" s="11"/>
-      <c r="Q17" s="11"/>
-      <c r="R17" s="13"/>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K17" s="1">
+        <f t="shared" si="7"/>
+        <v>-62.65872254123483</v>
+      </c>
+      <c r="R17" s="11"/>
     </row>
     <row r="18" spans="1:18">
       <c r="A18" s="10">
         <v>17</v>
       </c>
-      <c r="B18" s="11">
+      <c r="B18">
         <v>2024</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="12">
-        <f t="shared" si="2"/>
+      <c r="D18" s="1">
+        <f t="shared" si="4"/>
         <v>68.924594795358317</v>
       </c>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="11"/>
-      <c r="K18" s="11"/>
-      <c r="L18" s="11"/>
-      <c r="M18" s="11"/>
-      <c r="N18" s="11"/>
-      <c r="O18" s="11"/>
-      <c r="P18" s="11"/>
-      <c r="Q18" s="11"/>
-      <c r="R18" s="13"/>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K18" s="1">
+        <f t="shared" si="7"/>
+        <v>-68.924594795358317</v>
+      </c>
+      <c r="R18" s="11"/>
     </row>
     <row r="19" spans="1:18">
       <c r="A19" s="10">
         <v>18</v>
       </c>
-      <c r="B19" s="11">
+      <c r="B19">
         <v>2024</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C19" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="12">
-        <f t="shared" si="2"/>
+      <c r="D19" s="1">
+        <f t="shared" si="4"/>
         <v>75.817054274894161</v>
       </c>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="11"/>
-      <c r="K19" s="11"/>
-      <c r="L19" s="11"/>
-      <c r="M19" s="11"/>
-      <c r="N19" s="11"/>
-      <c r="O19" s="11"/>
-      <c r="P19" s="11"/>
-      <c r="Q19" s="11"/>
-      <c r="R19" s="13"/>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K19" s="1">
+        <f t="shared" si="7"/>
+        <v>-75.817054274894161</v>
+      </c>
+      <c r="R19" s="11"/>
     </row>
     <row r="20" spans="1:18">
       <c r="A20" s="10">
         <v>19</v>
       </c>
-      <c r="B20" s="11">
+      <c r="B20">
         <v>2024</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C20" t="s">
         <v>9</v>
       </c>
-      <c r="D20" s="12">
-        <f t="shared" si="2"/>
+      <c r="D20" s="1">
+        <f t="shared" si="4"/>
         <v>83.398759702383586</v>
       </c>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="11"/>
-      <c r="K20" s="11"/>
-      <c r="L20" s="11"/>
-      <c r="M20" s="11"/>
-      <c r="N20" s="11"/>
-      <c r="O20" s="11"/>
-      <c r="P20" s="11"/>
-      <c r="Q20" s="11"/>
-      <c r="R20" s="13"/>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K20" s="1">
+        <f t="shared" si="7"/>
+        <v>-83.398759702383586</v>
+      </c>
+      <c r="R20" s="11"/>
     </row>
     <row r="21" spans="1:18">
       <c r="A21" s="10">
         <v>20</v>
       </c>
-      <c r="B21" s="11">
+      <c r="B21">
         <v>2024</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C21" t="s">
         <v>10</v>
       </c>
-      <c r="D21" s="12">
-        <f t="shared" si="2"/>
+      <c r="D21" s="1">
+        <f t="shared" si="4"/>
         <v>91.738635672621953</v>
       </c>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="11"/>
-      <c r="K21" s="11"/>
-      <c r="L21" s="11"/>
-      <c r="M21" s="11"/>
-      <c r="N21" s="11"/>
-      <c r="O21" s="11"/>
-      <c r="P21" s="11"/>
-      <c r="Q21" s="11"/>
-      <c r="R21" s="13"/>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K21" s="1">
+        <f t="shared" si="7"/>
+        <v>-91.738635672621953</v>
+      </c>
+      <c r="R21" s="11"/>
     </row>
     <row r="22" spans="1:18">
       <c r="A22" s="10">
         <v>21</v>
       </c>
-      <c r="B22" s="11">
+      <c r="B22">
         <v>2024</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C22" t="s">
         <v>11</v>
       </c>
-      <c r="D22" s="12">
-        <f t="shared" si="2"/>
+      <c r="D22" s="1">
+        <f t="shared" si="4"/>
         <v>100.91249923988416</v>
       </c>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="11"/>
-      <c r="K22" s="11"/>
-      <c r="L22" s="11"/>
-      <c r="M22" s="11"/>
-      <c r="N22" s="11"/>
-      <c r="O22" s="11"/>
-      <c r="P22" s="11"/>
-      <c r="Q22" s="11"/>
-      <c r="R22" s="13"/>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K22" s="1">
+        <f t="shared" si="7"/>
+        <v>-100.91249923988416</v>
+      </c>
+      <c r="R22" s="11"/>
     </row>
     <row r="23" spans="1:18">
       <c r="A23" s="10">
         <v>22</v>
       </c>
-      <c r="B23" s="11">
+      <c r="B23">
         <v>2024</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C23" t="s">
         <v>12</v>
       </c>
-      <c r="D23" s="12">
-        <f t="shared" si="2"/>
+      <c r="D23" s="1">
+        <f t="shared" si="4"/>
         <v>111.00374916387258</v>
       </c>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="11"/>
-      <c r="J23" s="11"/>
-      <c r="K23" s="11"/>
-      <c r="L23" s="11"/>
-      <c r="M23" s="11"/>
-      <c r="N23" s="11"/>
-      <c r="O23" s="11"/>
-      <c r="P23" s="11"/>
-      <c r="Q23" s="11"/>
-      <c r="R23" s="13"/>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K23" s="1">
+        <f t="shared" si="7"/>
+        <v>-111.00374916387258</v>
+      </c>
+      <c r="R23" s="11"/>
     </row>
     <row r="24" spans="1:18">
       <c r="A24" s="10">
         <v>23</v>
       </c>
-      <c r="B24" s="11">
+      <c r="B24">
         <v>2024</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="C24" t="s">
         <v>13</v>
       </c>
-      <c r="D24" s="12">
-        <f t="shared" si="2"/>
+      <c r="D24" s="1">
+        <f t="shared" si="4"/>
         <v>122.10412408025985</v>
       </c>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="11"/>
-      <c r="J24" s="11"/>
-      <c r="K24" s="11"/>
-      <c r="L24" s="11"/>
-      <c r="M24" s="11"/>
-      <c r="N24" s="11"/>
-      <c r="O24" s="11"/>
-      <c r="P24" s="11"/>
-      <c r="Q24" s="11"/>
-      <c r="R24" s="13"/>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K24" s="1">
+        <f t="shared" si="7"/>
+        <v>-122.10412408025985</v>
+      </c>
+      <c r="R24" s="11"/>
     </row>
     <row r="25" spans="1:18" ht="17" thickBot="1">
-      <c r="A25" s="14">
+      <c r="A25" s="12">
         <v>24</v>
       </c>
-      <c r="B25" s="15">
+      <c r="B25" s="13">
         <v>2024</v>
       </c>
-      <c r="C25" s="15" t="s">
+      <c r="C25" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D25" s="16">
-        <f t="shared" si="2"/>
+      <c r="D25" s="14">
+        <f t="shared" si="4"/>
         <v>134.31453648828585</v>
       </c>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="15"/>
-      <c r="H25" s="15"/>
-      <c r="I25" s="15"/>
-      <c r="J25" s="15"/>
-      <c r="K25" s="15"/>
-      <c r="L25" s="15"/>
-      <c r="M25" s="15"/>
-      <c r="N25" s="15"/>
-      <c r="O25" s="15"/>
-      <c r="P25" s="15"/>
-      <c r="Q25" s="15"/>
-      <c r="R25" s="17"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13">
+        <v>0</v>
+      </c>
+      <c r="G25" s="13">
+        <v>0</v>
+      </c>
+      <c r="H25" s="13">
+        <v>0</v>
+      </c>
+      <c r="I25" s="13">
+        <v>0</v>
+      </c>
+      <c r="J25" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K25" s="14">
+        <f t="shared" si="7"/>
+        <v>-134.31453648828585</v>
+      </c>
+      <c r="L25" s="13"/>
+      <c r="M25" s="13"/>
+      <c r="N25" s="13"/>
+      <c r="O25" s="13"/>
+      <c r="P25" s="13"/>
+      <c r="Q25" s="13"/>
+      <c r="R25" s="15"/>
     </row>
     <row r="26" spans="1:18">
-      <c r="A26" s="6">
+      <c r="A26" s="10">
         <v>25</v>
       </c>
-      <c r="B26" s="7">
+      <c r="B26">
         <v>2025</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C26" t="s">
         <v>3</v>
       </c>
-      <c r="D26" s="8">
-        <f t="shared" si="2"/>
+      <c r="D26" s="1">
+        <f t="shared" si="4"/>
         <v>147.74599013711446</v>
       </c>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
-      <c r="I26" s="7"/>
-      <c r="J26" s="7"/>
-      <c r="K26" s="7"/>
       <c r="L26" s="7"/>
       <c r="M26" s="7"/>
       <c r="N26" s="7"/>
@@ -2999,1016 +3142,613 @@
       <c r="A27" s="10">
         <v>26</v>
       </c>
-      <c r="B27" s="11">
+      <c r="B27">
         <v>2025</v>
       </c>
-      <c r="C27" s="11" t="s">
+      <c r="C27" t="s">
         <v>4</v>
       </c>
-      <c r="D27" s="12">
-        <f t="shared" si="2"/>
+      <c r="D27" s="1">
+        <f t="shared" si="4"/>
         <v>162.52058915082591</v>
       </c>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="11"/>
-      <c r="I27" s="11"/>
-      <c r="J27" s="11"/>
-      <c r="K27" s="11"/>
-      <c r="L27" s="11"/>
-      <c r="M27" s="11"/>
-      <c r="N27" s="11"/>
-      <c r="O27" s="11"/>
-      <c r="P27" s="11"/>
-      <c r="Q27" s="11"/>
-      <c r="R27" s="13"/>
+      <c r="R27" s="11"/>
     </row>
     <row r="28" spans="1:18">
       <c r="A28" s="10">
         <v>27</v>
       </c>
-      <c r="B28" s="11">
+      <c r="B28">
         <v>2025</v>
       </c>
-      <c r="C28" s="11" t="s">
+      <c r="C28" t="s">
         <v>5</v>
       </c>
-      <c r="D28" s="12">
-        <f t="shared" si="2"/>
+      <c r="D28" s="1">
+        <f t="shared" si="4"/>
         <v>178.77264806590853</v>
       </c>
-      <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="11"/>
-      <c r="I28" s="11"/>
-      <c r="J28" s="11"/>
-      <c r="K28" s="11"/>
-      <c r="L28" s="11"/>
-      <c r="M28" s="11"/>
-      <c r="N28" s="11"/>
-      <c r="O28" s="11"/>
-      <c r="P28" s="11"/>
-      <c r="Q28" s="11"/>
-      <c r="R28" s="13"/>
+      <c r="R28" s="11"/>
     </row>
     <row r="29" spans="1:18">
       <c r="A29" s="10">
         <v>28</v>
       </c>
-      <c r="B29" s="11">
+      <c r="B29">
         <v>2025</v>
       </c>
-      <c r="C29" s="11" t="s">
+      <c r="C29" t="s">
         <v>6</v>
       </c>
-      <c r="D29" s="12">
-        <f t="shared" si="2"/>
+      <c r="D29" s="1">
+        <f t="shared" si="4"/>
         <v>196.64991287249939</v>
       </c>
-      <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="11"/>
-      <c r="I29" s="11"/>
-      <c r="J29" s="11"/>
-      <c r="K29" s="11"/>
-      <c r="L29" s="11"/>
-      <c r="M29" s="11"/>
-      <c r="N29" s="11"/>
-      <c r="O29" s="11"/>
-      <c r="P29" s="11"/>
-      <c r="Q29" s="11"/>
-      <c r="R29" s="13"/>
+      <c r="R29" s="11"/>
     </row>
     <row r="30" spans="1:18">
       <c r="A30" s="10">
         <v>29</v>
       </c>
-      <c r="B30" s="11">
+      <c r="B30">
         <v>2025</v>
       </c>
-      <c r="C30" s="11" t="s">
+      <c r="C30" t="s">
         <v>7</v>
       </c>
-      <c r="D30" s="12">
-        <f t="shared" si="2"/>
+      <c r="D30" s="1">
+        <f t="shared" si="4"/>
         <v>216.31490415974935</v>
       </c>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11"/>
-      <c r="I30" s="11"/>
-      <c r="J30" s="11"/>
-      <c r="K30" s="11"/>
-      <c r="L30" s="11"/>
-      <c r="M30" s="11"/>
-      <c r="N30" s="11"/>
-      <c r="O30" s="11"/>
-      <c r="P30" s="11"/>
-      <c r="Q30" s="11"/>
-      <c r="R30" s="13"/>
+      <c r="R30" s="11"/>
     </row>
     <row r="31" spans="1:18">
       <c r="A31" s="10">
         <v>30</v>
       </c>
-      <c r="B31" s="11">
+      <c r="B31">
         <v>2025</v>
       </c>
-      <c r="C31" s="11" t="s">
+      <c r="C31" t="s">
         <v>8</v>
       </c>
-      <c r="D31" s="12">
-        <f t="shared" si="2"/>
+      <c r="D31" s="1">
+        <f t="shared" si="4"/>
         <v>237.9463945757243</v>
       </c>
-      <c r="E31" s="11"/>
-      <c r="F31" s="11"/>
-      <c r="G31" s="11"/>
-      <c r="H31" s="11"/>
-      <c r="I31" s="11"/>
-      <c r="J31" s="11"/>
-      <c r="K31" s="11"/>
-      <c r="L31" s="11"/>
-      <c r="M31" s="11"/>
-      <c r="N31" s="11"/>
-      <c r="O31" s="11"/>
-      <c r="P31" s="11"/>
-      <c r="Q31" s="11"/>
-      <c r="R31" s="13"/>
+      <c r="R31" s="11"/>
     </row>
     <row r="32" spans="1:18">
       <c r="A32" s="10">
         <v>31</v>
       </c>
-      <c r="B32" s="11">
+      <c r="B32">
         <v>2025</v>
       </c>
-      <c r="C32" s="11" t="s">
+      <c r="C32" t="s">
         <v>9</v>
       </c>
-      <c r="D32" s="12">
-        <f t="shared" si="2"/>
+      <c r="D32" s="1">
+        <f t="shared" si="4"/>
         <v>261.74103403329673</v>
       </c>
-      <c r="E32" s="11"/>
-      <c r="F32" s="11"/>
-      <c r="G32" s="11"/>
-      <c r="H32" s="11"/>
-      <c r="I32" s="11"/>
-      <c r="J32" s="11"/>
-      <c r="K32" s="11"/>
-      <c r="L32" s="11"/>
-      <c r="M32" s="11"/>
-      <c r="N32" s="11"/>
-      <c r="O32" s="11"/>
-      <c r="P32" s="11"/>
-      <c r="Q32" s="11"/>
-      <c r="R32" s="13"/>
+      <c r="R32" s="11"/>
     </row>
     <row r="33" spans="1:18">
       <c r="A33" s="10">
         <v>32</v>
       </c>
-      <c r="B33" s="11">
+      <c r="B33">
         <v>2025</v>
       </c>
-      <c r="C33" s="11" t="s">
+      <c r="C33" t="s">
         <v>10</v>
       </c>
-      <c r="D33" s="12">
-        <f t="shared" si="2"/>
+      <c r="D33" s="1">
+        <f t="shared" si="4"/>
         <v>287.91513743662642</v>
       </c>
-      <c r="E33" s="11"/>
-      <c r="F33" s="11"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="11"/>
-      <c r="I33" s="11"/>
-      <c r="J33" s="11"/>
-      <c r="K33" s="11"/>
-      <c r="L33" s="11"/>
-      <c r="M33" s="11"/>
-      <c r="N33" s="11"/>
-      <c r="O33" s="11"/>
-      <c r="P33" s="11"/>
-      <c r="Q33" s="11"/>
-      <c r="R33" s="13"/>
+      <c r="R33" s="11"/>
     </row>
     <row r="34" spans="1:18">
       <c r="A34" s="10">
         <v>33</v>
       </c>
-      <c r="B34" s="11">
+      <c r="B34">
         <v>2025</v>
       </c>
-      <c r="C34" s="11" t="s">
+      <c r="C34" t="s">
         <v>11</v>
       </c>
-      <c r="D34" s="12">
-        <f t="shared" si="2"/>
+      <c r="D34" s="1">
+        <f t="shared" si="4"/>
         <v>316.7066511802891</v>
       </c>
-      <c r="E34" s="11"/>
-      <c r="F34" s="11"/>
-      <c r="G34" s="11"/>
-      <c r="H34" s="11"/>
-      <c r="I34" s="11"/>
-      <c r="J34" s="11"/>
-      <c r="K34" s="11"/>
-      <c r="L34" s="11"/>
-      <c r="M34" s="11"/>
-      <c r="N34" s="11"/>
-      <c r="O34" s="11"/>
-      <c r="P34" s="11"/>
-      <c r="Q34" s="11"/>
-      <c r="R34" s="13"/>
+      <c r="R34" s="11"/>
     </row>
     <row r="35" spans="1:18">
       <c r="A35" s="10">
         <v>34</v>
       </c>
-      <c r="B35" s="11">
+      <c r="B35">
         <v>2025</v>
       </c>
-      <c r="C35" s="11" t="s">
+      <c r="C35" t="s">
         <v>12</v>
       </c>
-      <c r="D35" s="12">
-        <f t="shared" si="2"/>
+      <c r="D35" s="1">
+        <f t="shared" si="4"/>
         <v>348.37731629831802</v>
       </c>
-      <c r="E35" s="11"/>
-      <c r="F35" s="11"/>
-      <c r="G35" s="11"/>
-      <c r="H35" s="11"/>
-      <c r="I35" s="11"/>
-      <c r="J35" s="11"/>
-      <c r="K35" s="11"/>
-      <c r="L35" s="11"/>
-      <c r="M35" s="11"/>
-      <c r="N35" s="11"/>
-      <c r="O35" s="11"/>
-      <c r="P35" s="11"/>
-      <c r="Q35" s="11"/>
-      <c r="R35" s="13"/>
+      <c r="R35" s="11"/>
     </row>
     <row r="36" spans="1:18">
       <c r="A36" s="10">
         <v>35</v>
       </c>
-      <c r="B36" s="11">
+      <c r="B36">
         <v>2025</v>
       </c>
-      <c r="C36" s="11" t="s">
+      <c r="C36" t="s">
         <v>13</v>
       </c>
-      <c r="D36" s="12">
-        <f t="shared" si="2"/>
+      <c r="D36" s="1">
+        <f t="shared" si="4"/>
         <v>383.21504792814983</v>
       </c>
-      <c r="E36" s="11"/>
-      <c r="F36" s="11"/>
-      <c r="G36" s="11"/>
-      <c r="H36" s="11"/>
-      <c r="I36" s="11"/>
-      <c r="J36" s="11"/>
-      <c r="K36" s="11"/>
-      <c r="L36" s="11"/>
-      <c r="M36" s="11"/>
-      <c r="N36" s="11"/>
-      <c r="O36" s="11"/>
-      <c r="P36" s="11"/>
-      <c r="Q36" s="11"/>
-      <c r="R36" s="13"/>
+      <c r="R36" s="11"/>
     </row>
     <row r="37" spans="1:18">
       <c r="A37" s="10">
         <v>36</v>
       </c>
-      <c r="B37" s="11">
+      <c r="B37">
         <v>2025</v>
       </c>
-      <c r="C37" s="11" t="s">
+      <c r="C37" t="s">
         <v>14</v>
       </c>
-      <c r="D37" s="12">
-        <f t="shared" si="2"/>
+      <c r="D37" s="1">
+        <f t="shared" si="4"/>
         <v>421.53655272096483</v>
       </c>
-      <c r="E37" s="11"/>
-      <c r="F37" s="11"/>
-      <c r="G37" s="11"/>
-      <c r="H37" s="11"/>
-      <c r="I37" s="11"/>
-      <c r="J37" s="11"/>
-      <c r="K37" s="11"/>
-      <c r="L37" s="11"/>
-      <c r="M37" s="11"/>
-      <c r="N37" s="11"/>
-      <c r="O37" s="11"/>
-      <c r="P37" s="11"/>
-      <c r="Q37" s="11"/>
-      <c r="R37" s="13"/>
+      <c r="R37" s="11"/>
     </row>
     <row r="38" spans="1:18">
-      <c r="A38" s="19">
+      <c r="A38" s="16">
         <v>37</v>
       </c>
-      <c r="B38" s="20">
+      <c r="B38" s="17">
         <v>2026</v>
       </c>
-      <c r="C38" s="20" t="s">
+      <c r="C38" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="D38" s="21">
-        <f t="shared" si="2"/>
+      <c r="D38" s="18">
+        <f t="shared" si="4"/>
         <v>463.69020799306134</v>
       </c>
-      <c r="E38" s="20"/>
-      <c r="F38" s="20"/>
-      <c r="G38" s="20"/>
-      <c r="H38" s="20"/>
-      <c r="I38" s="20"/>
-      <c r="J38" s="20"/>
-      <c r="K38" s="20"/>
-      <c r="L38" s="20"/>
-      <c r="M38" s="20"/>
-      <c r="N38" s="20"/>
-      <c r="O38" s="20"/>
-      <c r="P38" s="20"/>
-      <c r="Q38" s="20"/>
-      <c r="R38" s="22"/>
+      <c r="E38" s="17"/>
+      <c r="F38" s="17"/>
+      <c r="G38" s="17"/>
+      <c r="H38" s="17"/>
+      <c r="I38" s="17"/>
+      <c r="J38" s="17"/>
+      <c r="K38" s="17"/>
+      <c r="L38" s="17"/>
+      <c r="M38" s="17"/>
+      <c r="N38" s="17"/>
+      <c r="O38" s="17"/>
+      <c r="P38" s="17"/>
+      <c r="Q38" s="17"/>
+      <c r="R38" s="19"/>
     </row>
     <row r="39" spans="1:18">
-      <c r="A39" s="23">
+      <c r="A39" s="20">
         <v>38</v>
       </c>
-      <c r="B39" s="11">
+      <c r="B39">
         <v>2026</v>
       </c>
-      <c r="C39" s="11" t="s">
+      <c r="C39" t="s">
         <v>4</v>
       </c>
-      <c r="D39" s="12">
-        <f t="shared" si="2"/>
+      <c r="D39" s="1">
+        <f t="shared" si="4"/>
         <v>510.05922879236749</v>
       </c>
-      <c r="E39" s="11"/>
-      <c r="F39" s="11"/>
-      <c r="G39" s="11"/>
-      <c r="H39" s="11"/>
-      <c r="I39" s="11"/>
-      <c r="J39" s="11"/>
-      <c r="K39" s="11"/>
-      <c r="L39" s="11"/>
-      <c r="M39" s="11"/>
-      <c r="N39" s="11"/>
-      <c r="O39" s="11"/>
-      <c r="P39" s="11"/>
-      <c r="Q39" s="11"/>
-      <c r="R39" s="24"/>
+      <c r="R39" s="21"/>
     </row>
     <row r="40" spans="1:18">
-      <c r="A40" s="23">
+      <c r="A40" s="20">
         <v>39</v>
       </c>
-      <c r="B40" s="11">
+      <c r="B40">
         <v>2026</v>
       </c>
-      <c r="C40" s="11" t="s">
+      <c r="C40" t="s">
         <v>5</v>
       </c>
-      <c r="D40" s="12">
-        <f t="shared" si="2"/>
+      <c r="D40" s="1">
+        <f t="shared" si="4"/>
         <v>561.06515167160433</v>
       </c>
-      <c r="E40" s="11"/>
-      <c r="F40" s="11"/>
-      <c r="G40" s="11"/>
-      <c r="H40" s="11"/>
-      <c r="I40" s="11"/>
-      <c r="J40" s="11"/>
-      <c r="K40" s="11"/>
-      <c r="L40" s="11"/>
-      <c r="M40" s="11"/>
-      <c r="N40" s="11"/>
-      <c r="O40" s="11"/>
-      <c r="P40" s="11"/>
-      <c r="Q40" s="11"/>
-      <c r="R40" s="24"/>
+      <c r="R40" s="21"/>
     </row>
     <row r="41" spans="1:18">
-      <c r="A41" s="23">
+      <c r="A41" s="20">
         <v>40</v>
       </c>
-      <c r="B41" s="11">
+      <c r="B41">
         <v>2026</v>
       </c>
-      <c r="C41" s="11" t="s">
+      <c r="C41" t="s">
         <v>6</v>
       </c>
-      <c r="D41" s="12">
-        <f t="shared" si="2"/>
+      <c r="D41" s="1">
+        <f t="shared" si="4"/>
         <v>617.17166683876485</v>
       </c>
-      <c r="E41" s="11"/>
-      <c r="F41" s="11"/>
-      <c r="G41" s="11"/>
-      <c r="H41" s="11"/>
-      <c r="I41" s="11"/>
-      <c r="J41" s="11"/>
-      <c r="K41" s="11"/>
-      <c r="L41" s="11"/>
-      <c r="M41" s="11"/>
-      <c r="N41" s="11"/>
-      <c r="O41" s="11"/>
-      <c r="P41" s="11"/>
-      <c r="Q41" s="11"/>
-      <c r="R41" s="24"/>
+      <c r="R41" s="21"/>
     </row>
     <row r="42" spans="1:18">
-      <c r="A42" s="23">
+      <c r="A42" s="20">
         <v>41</v>
       </c>
-      <c r="B42" s="11">
+      <c r="B42">
         <v>2026</v>
       </c>
-      <c r="C42" s="11" t="s">
+      <c r="C42" t="s">
         <v>7</v>
       </c>
-      <c r="D42" s="12">
-        <f t="shared" si="2"/>
+      <c r="D42" s="1">
+        <f t="shared" si="4"/>
         <v>678.88883352264133</v>
       </c>
-      <c r="E42" s="11"/>
-      <c r="F42" s="11"/>
-      <c r="G42" s="11"/>
-      <c r="H42" s="11"/>
-      <c r="I42" s="11"/>
-      <c r="J42" s="11"/>
-      <c r="K42" s="11"/>
-      <c r="L42" s="11"/>
-      <c r="M42" s="11"/>
-      <c r="N42" s="11"/>
-      <c r="O42" s="11"/>
-      <c r="P42" s="11"/>
-      <c r="Q42" s="11"/>
-      <c r="R42" s="24"/>
+      <c r="R42" s="21"/>
     </row>
     <row r="43" spans="1:18">
-      <c r="A43" s="23">
+      <c r="A43" s="20">
         <v>42</v>
       </c>
-      <c r="B43" s="11">
+      <c r="B43">
         <v>2026</v>
       </c>
-      <c r="C43" s="11" t="s">
+      <c r="C43" t="s">
         <v>8</v>
       </c>
-      <c r="D43" s="12">
-        <f t="shared" si="2"/>
+      <c r="D43" s="1">
+        <f t="shared" si="4"/>
         <v>746.77771687490554</v>
       </c>
-      <c r="E43" s="11"/>
-      <c r="F43" s="11"/>
-      <c r="G43" s="11"/>
-      <c r="H43" s="11"/>
-      <c r="I43" s="11"/>
-      <c r="J43" s="11"/>
-      <c r="K43" s="11"/>
-      <c r="L43" s="11"/>
-      <c r="M43" s="11"/>
-      <c r="N43" s="11"/>
-      <c r="O43" s="11"/>
-      <c r="P43" s="11"/>
-      <c r="Q43" s="11"/>
-      <c r="R43" s="24"/>
+      <c r="R43" s="21"/>
     </row>
     <row r="44" spans="1:18">
-      <c r="A44" s="23">
+      <c r="A44" s="20">
         <v>43</v>
       </c>
-      <c r="B44" s="11">
+      <c r="B44">
         <v>2026</v>
       </c>
-      <c r="C44" s="11" t="s">
+      <c r="C44" t="s">
         <v>9</v>
       </c>
-      <c r="D44" s="12">
-        <f t="shared" si="2"/>
+      <c r="D44" s="1">
+        <f t="shared" si="4"/>
         <v>821.45548856239611</v>
       </c>
-      <c r="E44" s="11"/>
-      <c r="F44" s="11"/>
-      <c r="G44" s="11"/>
-      <c r="H44" s="11"/>
-      <c r="I44" s="11"/>
-      <c r="J44" s="11"/>
-      <c r="K44" s="11"/>
-      <c r="L44" s="11"/>
-      <c r="M44" s="11"/>
-      <c r="N44" s="11"/>
-      <c r="O44" s="11"/>
-      <c r="P44" s="11"/>
-      <c r="Q44" s="11"/>
-      <c r="R44" s="24"/>
+      <c r="R44" s="21"/>
     </row>
     <row r="45" spans="1:18">
-      <c r="A45" s="23">
+      <c r="A45" s="20">
         <v>44</v>
       </c>
-      <c r="B45" s="11">
+      <c r="B45">
         <v>2026</v>
       </c>
-      <c r="C45" s="11" t="s">
+      <c r="C45" t="s">
         <v>10</v>
       </c>
-      <c r="D45" s="12">
-        <f t="shared" si="2"/>
+      <c r="D45" s="1">
+        <f t="shared" si="4"/>
         <v>903.60103741863577</v>
       </c>
-      <c r="E45" s="11"/>
-      <c r="F45" s="11"/>
-      <c r="G45" s="11"/>
-      <c r="H45" s="11"/>
-      <c r="I45" s="11"/>
-      <c r="J45" s="11"/>
-      <c r="K45" s="11"/>
-      <c r="L45" s="11"/>
-      <c r="M45" s="11"/>
-      <c r="N45" s="11"/>
-      <c r="O45" s="11"/>
-      <c r="P45" s="11"/>
-      <c r="Q45" s="11"/>
-      <c r="R45" s="24"/>
+      <c r="R45" s="21"/>
     </row>
     <row r="46" spans="1:18">
-      <c r="A46" s="23">
+      <c r="A46" s="20">
         <v>45</v>
       </c>
-      <c r="B46" s="11">
+      <c r="B46">
         <v>2026</v>
       </c>
-      <c r="C46" s="11" t="s">
+      <c r="C46" t="s">
         <v>11</v>
       </c>
-      <c r="D46" s="12">
-        <f t="shared" si="2"/>
+      <c r="D46" s="1">
+        <f t="shared" si="4"/>
         <v>993.96114116049944</v>
       </c>
-      <c r="E46" s="11"/>
-      <c r="F46" s="11"/>
-      <c r="G46" s="11"/>
-      <c r="H46" s="11"/>
-      <c r="I46" s="11"/>
-      <c r="J46" s="11"/>
-      <c r="K46" s="11"/>
-      <c r="L46" s="11"/>
-      <c r="M46" s="11"/>
-      <c r="N46" s="11"/>
-      <c r="O46" s="11"/>
-      <c r="P46" s="11"/>
-      <c r="Q46" s="11"/>
-      <c r="R46" s="24"/>
+      <c r="R46" s="21"/>
     </row>
     <row r="47" spans="1:18">
-      <c r="A47" s="23">
+      <c r="A47" s="20">
         <v>46</v>
       </c>
-      <c r="B47" s="11">
+      <c r="B47">
         <v>2026</v>
       </c>
-      <c r="C47" s="11" t="s">
+      <c r="C47" t="s">
         <v>12</v>
       </c>
-      <c r="D47" s="12">
-        <f t="shared" si="2"/>
+      <c r="D47" s="1">
+        <f t="shared" si="4"/>
         <v>1093.3572552765495</v>
       </c>
-      <c r="E47" s="11"/>
-      <c r="F47" s="11"/>
-      <c r="G47" s="11"/>
-      <c r="H47" s="11"/>
-      <c r="I47" s="11"/>
-      <c r="J47" s="11"/>
-      <c r="K47" s="11"/>
-      <c r="L47" s="11"/>
-      <c r="M47" s="11"/>
-      <c r="N47" s="11"/>
-      <c r="O47" s="11"/>
-      <c r="P47" s="11"/>
-      <c r="Q47" s="11"/>
-      <c r="R47" s="24"/>
+      <c r="R47" s="21"/>
     </row>
     <row r="48" spans="1:18">
-      <c r="A48" s="23">
+      <c r="A48" s="20">
         <v>47</v>
       </c>
-      <c r="B48" s="11">
+      <c r="B48">
         <v>2026</v>
       </c>
-      <c r="C48" s="11" t="s">
+      <c r="C48" t="s">
         <v>13</v>
       </c>
-      <c r="D48" s="12">
-        <f t="shared" si="2"/>
+      <c r="D48" s="1">
+        <f t="shared" si="4"/>
         <v>1202.6929808042046</v>
       </c>
-      <c r="E48" s="11"/>
-      <c r="F48" s="11"/>
-      <c r="G48" s="11"/>
-      <c r="H48" s="11"/>
-      <c r="I48" s="11"/>
-      <c r="J48" s="11"/>
-      <c r="K48" s="11"/>
-      <c r="L48" s="11"/>
-      <c r="M48" s="11"/>
-      <c r="N48" s="11"/>
-      <c r="O48" s="11"/>
-      <c r="P48" s="11"/>
-      <c r="Q48" s="11"/>
-      <c r="R48" s="24"/>
+      <c r="R48" s="21"/>
     </row>
     <row r="49" spans="1:18">
-      <c r="A49" s="25">
+      <c r="A49" s="22">
         <v>48</v>
       </c>
-      <c r="B49" s="26">
+      <c r="B49" s="23">
         <v>2026</v>
       </c>
-      <c r="C49" s="26" t="s">
+      <c r="C49" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="D49" s="27">
-        <f t="shared" si="2"/>
+      <c r="D49" s="24">
+        <f t="shared" si="4"/>
         <v>1322.9622788846252</v>
       </c>
-      <c r="E49" s="26"/>
-      <c r="F49" s="26"/>
-      <c r="G49" s="26"/>
-      <c r="H49" s="26"/>
-      <c r="I49" s="26"/>
-      <c r="J49" s="26"/>
-      <c r="K49" s="26"/>
-      <c r="L49" s="26"/>
-      <c r="M49" s="26"/>
-      <c r="N49" s="26"/>
-      <c r="O49" s="26"/>
-      <c r="P49" s="26"/>
-      <c r="Q49" s="26"/>
-      <c r="R49" s="28"/>
+      <c r="E49" s="23"/>
+      <c r="F49" s="23"/>
+      <c r="G49" s="23"/>
+      <c r="H49" s="23"/>
+      <c r="I49" s="23"/>
+      <c r="J49" s="23"/>
+      <c r="K49" s="23"/>
+      <c r="L49" s="23"/>
+      <c r="M49" s="23"/>
+      <c r="N49" s="23"/>
+      <c r="O49" s="23"/>
+      <c r="P49" s="23"/>
+      <c r="Q49" s="23"/>
+      <c r="R49" s="25"/>
     </row>
     <row r="50" spans="1:18">
-      <c r="A50" s="19">
+      <c r="A50" s="16">
         <v>49</v>
       </c>
-      <c r="B50" s="20">
+      <c r="B50" s="17">
         <v>2027</v>
       </c>
-      <c r="C50" s="20" t="s">
+      <c r="C50" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="D50" s="21">
-        <f t="shared" si="2"/>
+      <c r="D50" s="18">
+        <f t="shared" si="4"/>
         <v>1455.2585067730879</v>
       </c>
-      <c r="E50" s="20"/>
-      <c r="F50" s="20"/>
-      <c r="G50" s="20"/>
-      <c r="H50" s="20"/>
-      <c r="I50" s="20"/>
-      <c r="J50" s="20"/>
-      <c r="K50" s="20"/>
-      <c r="L50" s="20"/>
-      <c r="M50" s="20"/>
-      <c r="N50" s="20"/>
-      <c r="O50" s="20"/>
-      <c r="P50" s="20"/>
-      <c r="Q50" s="20"/>
-      <c r="R50" s="22"/>
+      <c r="E50" s="17"/>
+      <c r="F50" s="17"/>
+      <c r="G50" s="17"/>
+      <c r="H50" s="17"/>
+      <c r="I50" s="17"/>
+      <c r="J50" s="17"/>
+      <c r="K50" s="17"/>
+      <c r="L50" s="17"/>
+      <c r="M50" s="17"/>
+      <c r="N50" s="17"/>
+      <c r="O50" s="17"/>
+      <c r="P50" s="17"/>
+      <c r="Q50" s="17"/>
+      <c r="R50" s="19"/>
     </row>
     <row r="51" spans="1:18">
-      <c r="A51" s="23">
+      <c r="A51" s="20">
         <v>50</v>
       </c>
-      <c r="B51" s="11">
+      <c r="B51">
         <v>2027</v>
       </c>
-      <c r="C51" s="11" t="s">
+      <c r="C51" t="s">
         <v>4</v>
       </c>
-      <c r="D51" s="12">
-        <f t="shared" si="2"/>
+      <c r="D51" s="1">
+        <f t="shared" si="4"/>
         <v>1600.7843574503968</v>
       </c>
-      <c r="E51" s="11"/>
-      <c r="F51" s="11"/>
-      <c r="G51" s="11"/>
-      <c r="H51" s="11"/>
-      <c r="I51" s="11"/>
-      <c r="J51" s="11"/>
-      <c r="K51" s="11"/>
-      <c r="L51" s="11"/>
-      <c r="M51" s="11"/>
-      <c r="N51" s="11"/>
-      <c r="O51" s="11"/>
-      <c r="P51" s="11"/>
-      <c r="Q51" s="11"/>
-      <c r="R51" s="24"/>
+      <c r="R51" s="21"/>
     </row>
     <row r="52" spans="1:18">
-      <c r="A52" s="23">
+      <c r="A52" s="20">
         <v>51</v>
       </c>
-      <c r="B52" s="11">
+      <c r="B52">
         <v>2027</v>
       </c>
-      <c r="C52" s="11" t="s">
+      <c r="C52" t="s">
         <v>5</v>
       </c>
-      <c r="D52" s="12">
-        <f t="shared" si="2"/>
+      <c r="D52" s="1">
+        <f t="shared" si="4"/>
         <v>1760.8627931954366</v>
       </c>
-      <c r="E52" s="11"/>
-      <c r="F52" s="11"/>
-      <c r="G52" s="11"/>
-      <c r="H52" s="11"/>
-      <c r="I52" s="11"/>
-      <c r="J52" s="11"/>
-      <c r="K52" s="11"/>
-      <c r="L52" s="11"/>
-      <c r="M52" s="11"/>
-      <c r="N52" s="11"/>
-      <c r="O52" s="11"/>
-      <c r="P52" s="11"/>
-      <c r="Q52" s="11"/>
-      <c r="R52" s="24"/>
+      <c r="R52" s="21"/>
     </row>
     <row r="53" spans="1:18">
-      <c r="A53" s="23">
+      <c r="A53" s="20">
         <v>52</v>
       </c>
-      <c r="B53" s="11">
+      <c r="B53">
         <v>2027</v>
       </c>
-      <c r="C53" s="11" t="s">
+      <c r="C53" t="s">
         <v>6</v>
       </c>
-      <c r="D53" s="12">
-        <f t="shared" si="2"/>
+      <c r="D53" s="1">
+        <f t="shared" si="4"/>
         <v>1936.9490725149803</v>
       </c>
-      <c r="E53" s="11"/>
-      <c r="F53" s="11"/>
-      <c r="G53" s="11"/>
-      <c r="H53" s="11"/>
-      <c r="I53" s="11"/>
-      <c r="J53" s="11"/>
-      <c r="K53" s="11"/>
-      <c r="L53" s="11"/>
-      <c r="M53" s="11"/>
-      <c r="N53" s="11"/>
-      <c r="O53" s="11"/>
-      <c r="P53" s="11"/>
-      <c r="Q53" s="11"/>
-      <c r="R53" s="24"/>
+      <c r="R53" s="21"/>
     </row>
     <row r="54" spans="1:18">
-      <c r="A54" s="23">
+      <c r="A54" s="20">
         <v>53</v>
       </c>
-      <c r="B54" s="11">
+      <c r="B54">
         <v>2027</v>
       </c>
-      <c r="C54" s="11" t="s">
+      <c r="C54" t="s">
         <v>7</v>
       </c>
-      <c r="D54" s="12">
-        <f t="shared" si="2"/>
+      <c r="D54" s="1">
+        <f t="shared" si="4"/>
         <v>2130.6439797664784</v>
       </c>
-      <c r="E54" s="11"/>
-      <c r="F54" s="11"/>
-      <c r="G54" s="11"/>
-      <c r="H54" s="11"/>
-      <c r="I54" s="11"/>
-      <c r="J54" s="11"/>
-      <c r="K54" s="11"/>
-      <c r="L54" s="11"/>
-      <c r="M54" s="11"/>
-      <c r="N54" s="11"/>
-      <c r="O54" s="11"/>
-      <c r="P54" s="11"/>
-      <c r="Q54" s="11"/>
-      <c r="R54" s="24"/>
+      <c r="R54" s="21"/>
     </row>
     <row r="55" spans="1:18">
-      <c r="A55" s="23">
+      <c r="A55" s="20">
         <v>54</v>
       </c>
-      <c r="B55" s="11">
+      <c r="B55">
         <v>2027</v>
       </c>
-      <c r="C55" s="11" t="s">
+      <c r="C55" t="s">
         <v>8</v>
       </c>
-      <c r="D55" s="12">
-        <f t="shared" si="2"/>
+      <c r="D55" s="1">
+        <f t="shared" si="4"/>
         <v>2343.7083777431267</v>
       </c>
-      <c r="E55" s="11"/>
-      <c r="F55" s="11"/>
-      <c r="G55" s="11"/>
-      <c r="H55" s="11"/>
-      <c r="I55" s="11"/>
-      <c r="J55" s="11"/>
-      <c r="K55" s="11"/>
-      <c r="L55" s="11"/>
-      <c r="M55" s="11"/>
-      <c r="N55" s="11"/>
-      <c r="O55" s="11"/>
-      <c r="P55" s="11"/>
-      <c r="Q55" s="11"/>
-      <c r="R55" s="24"/>
+      <c r="R55" s="21"/>
     </row>
     <row r="56" spans="1:18">
-      <c r="A56" s="23">
+      <c r="A56" s="20">
         <v>55</v>
       </c>
-      <c r="B56" s="11">
+      <c r="B56">
         <v>2027</v>
       </c>
-      <c r="C56" s="11" t="s">
+      <c r="C56" t="s">
         <v>9</v>
       </c>
-      <c r="D56" s="12">
-        <f t="shared" si="2"/>
+      <c r="D56" s="1">
+        <f t="shared" si="4"/>
         <v>2578.0792155174395</v>
       </c>
-      <c r="E56" s="11"/>
-      <c r="F56" s="11"/>
-      <c r="G56" s="11"/>
-      <c r="H56" s="11"/>
-      <c r="I56" s="11"/>
-      <c r="J56" s="11"/>
-      <c r="K56" s="11"/>
-      <c r="L56" s="11"/>
-      <c r="M56" s="11"/>
-      <c r="N56" s="11"/>
-      <c r="O56" s="11"/>
-      <c r="P56" s="11"/>
-      <c r="Q56" s="11"/>
-      <c r="R56" s="24"/>
+      <c r="R56" s="21"/>
     </row>
     <row r="57" spans="1:18">
-      <c r="A57" s="23">
+      <c r="A57" s="20">
         <v>56</v>
       </c>
-      <c r="B57" s="11">
+      <c r="B57">
         <v>2027</v>
       </c>
-      <c r="C57" s="11" t="s">
+      <c r="C57" t="s">
         <v>10</v>
       </c>
-      <c r="D57" s="12">
-        <f t="shared" si="2"/>
+      <c r="D57" s="1">
+        <f t="shared" si="4"/>
         <v>2835.8871370691836</v>
       </c>
-      <c r="E57" s="11"/>
-      <c r="F57" s="11"/>
-      <c r="G57" s="11"/>
-      <c r="H57" s="11"/>
-      <c r="I57" s="11"/>
-      <c r="J57" s="11"/>
-      <c r="K57" s="11"/>
-      <c r="L57" s="11"/>
-      <c r="M57" s="11"/>
-      <c r="N57" s="11"/>
-      <c r="O57" s="11"/>
-      <c r="P57" s="11"/>
-      <c r="Q57" s="11"/>
-      <c r="R57" s="24"/>
+      <c r="R57" s="21"/>
     </row>
     <row r="58" spans="1:18">
-      <c r="A58" s="23">
+      <c r="A58" s="20">
         <v>57</v>
       </c>
-      <c r="B58" s="11">
+      <c r="B58">
         <v>2027</v>
       </c>
-      <c r="C58" s="11" t="s">
+      <c r="C58" t="s">
         <v>11</v>
       </c>
-      <c r="D58" s="12">
-        <f t="shared" si="2"/>
+      <c r="D58" s="1">
+        <f t="shared" si="4"/>
         <v>3119.4758507761021</v>
       </c>
-      <c r="E58" s="11"/>
-      <c r="F58" s="11"/>
-      <c r="G58" s="11"/>
-      <c r="H58" s="11"/>
-      <c r="I58" s="11"/>
-      <c r="J58" s="11"/>
-      <c r="K58" s="11"/>
-      <c r="L58" s="11"/>
-      <c r="M58" s="11"/>
-      <c r="N58" s="11"/>
-      <c r="O58" s="11"/>
-      <c r="P58" s="11"/>
-      <c r="Q58" s="11"/>
-      <c r="R58" s="24"/>
+      <c r="R58" s="21"/>
     </row>
     <row r="59" spans="1:18">
-      <c r="A59" s="23">
+      <c r="A59" s="20">
         <v>58</v>
       </c>
-      <c r="B59" s="11">
+      <c r="B59">
         <v>2027</v>
       </c>
-      <c r="C59" s="11" t="s">
+      <c r="C59" t="s">
         <v>12</v>
       </c>
-      <c r="D59" s="12">
-        <f t="shared" si="2"/>
+      <c r="D59" s="1">
+        <f t="shared" si="4"/>
         <v>3431.4234358537128</v>
       </c>
-      <c r="E59" s="11"/>
-      <c r="F59" s="11"/>
-      <c r="G59" s="11"/>
-      <c r="H59" s="11"/>
-      <c r="I59" s="11"/>
-      <c r="J59" s="11"/>
-      <c r="K59" s="11"/>
-      <c r="L59" s="11"/>
-      <c r="M59" s="11"/>
-      <c r="N59" s="11"/>
-      <c r="O59" s="11"/>
-      <c r="P59" s="11"/>
-      <c r="Q59" s="11"/>
-      <c r="R59" s="24"/>
+      <c r="R59" s="21"/>
     </row>
     <row r="60" spans="1:18">
-      <c r="A60" s="23">
+      <c r="A60" s="20">
         <v>59</v>
       </c>
-      <c r="B60" s="11">
+      <c r="B60">
         <v>2027</v>
       </c>
-      <c r="C60" s="11" t="s">
+      <c r="C60" t="s">
         <v>13</v>
       </c>
-      <c r="D60" s="12">
-        <f t="shared" si="2"/>
+      <c r="D60" s="1">
+        <f t="shared" si="4"/>
         <v>3774.5657794390845</v>
       </c>
-      <c r="E60" s="11"/>
-      <c r="F60" s="11"/>
-      <c r="G60" s="11"/>
-      <c r="H60" s="11"/>
-      <c r="I60" s="11"/>
-      <c r="J60" s="11"/>
-      <c r="K60" s="11"/>
-      <c r="L60" s="11"/>
-      <c r="M60" s="11"/>
-      <c r="N60" s="11"/>
-      <c r="O60" s="11"/>
-      <c r="P60" s="11"/>
-      <c r="Q60" s="11"/>
-      <c r="R60" s="24"/>
+      <c r="R60" s="21"/>
     </row>
     <row r="61" spans="1:18">
-      <c r="A61" s="25">
+      <c r="A61" s="22">
         <v>60</v>
       </c>
-      <c r="B61" s="26">
+      <c r="B61" s="23">
         <v>2027</v>
       </c>
-      <c r="C61" s="26" t="s">
+      <c r="C61" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="D61" s="27">
-        <f t="shared" si="2"/>
+      <c r="D61" s="24">
+        <f t="shared" si="4"/>
         <v>4152.0223573829935</v>
       </c>
-      <c r="E61" s="26"/>
-      <c r="F61" s="26"/>
-      <c r="G61" s="26"/>
-      <c r="H61" s="26"/>
-      <c r="I61" s="26"/>
-      <c r="J61" s="26"/>
-      <c r="K61" s="26"/>
-      <c r="L61" s="26"/>
-      <c r="M61" s="26"/>
-      <c r="N61" s="26"/>
-      <c r="O61" s="26"/>
-      <c r="P61" s="26"/>
-      <c r="Q61" s="26"/>
-      <c r="R61" s="28"/>
+      <c r="E61" s="23"/>
+      <c r="F61" s="23"/>
+      <c r="G61" s="23"/>
+      <c r="H61" s="23"/>
+      <c r="I61" s="23"/>
+      <c r="J61" s="23"/>
+      <c r="K61" s="23"/>
+      <c r="L61" s="23"/>
+      <c r="M61" s="23"/>
+      <c r="N61" s="23"/>
+      <c r="O61" s="23"/>
+      <c r="P61" s="23"/>
+      <c r="Q61" s="23"/>
+      <c r="R61" s="25"/>
     </row>
     <row r="62" spans="1:18">
       <c r="A62">
@@ -4021,7 +3761,7 @@
         <v>3</v>
       </c>
       <c r="D62" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4567.2245931212929</v>
       </c>
     </row>
@@ -4036,7 +3776,7 @@
         <v>4</v>
       </c>
       <c r="D63" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>5023.9470524334229</v>
       </c>
     </row>
@@ -4051,7 +3791,7 @@
         <v>5</v>
       </c>
       <c r="D64" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>5526.3417576767652</v>
       </c>
     </row>
@@ -4066,7 +3806,7 @@
         <v>6</v>
       </c>
       <c r="D65" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6078.9759334444425</v>
       </c>
     </row>
@@ -4081,7 +3821,7 @@
         <v>7</v>
       </c>
       <c r="D66" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6686.8735267888869</v>
       </c>
     </row>
@@ -4096,7 +3836,7 @@
         <v>8</v>
       </c>
       <c r="D67" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>7355.5608794677764</v>
       </c>
     </row>
@@ -4111,7 +3851,7 @@
         <v>9</v>
       </c>
       <c r="D68" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>8091.1169674145549</v>
       </c>
     </row>
@@ -4126,7 +3866,7 @@
         <v>10</v>
       </c>
       <c r="D69" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>8900.2286641560113</v>
       </c>
     </row>
@@ -4141,7 +3881,7 @@
         <v>11</v>
       </c>
       <c r="D70" s="1">
-        <f t="shared" ref="D70:D97" si="4">D69*1.1</f>
+        <f t="shared" ref="D70:D97" si="8">D69*1.1</f>
         <v>9790.2515305716133</v>
       </c>
     </row>
@@ -4156,7 +3896,7 @@
         <v>12</v>
       </c>
       <c r="D71" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>10769.276683628776</v>
       </c>
     </row>
@@ -4171,7 +3911,7 @@
         <v>13</v>
       </c>
       <c r="D72" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>11846.204351991653</v>
       </c>
     </row>
@@ -4186,7 +3926,7 @@
         <v>14</v>
       </c>
       <c r="D73" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>13030.824787190819</v>
       </c>
     </row>
@@ -4201,7 +3941,7 @@
         <v>3</v>
       </c>
       <c r="D74" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>14333.907265909902</v>
       </c>
     </row>
@@ -4216,7 +3956,7 @@
         <v>4</v>
       </c>
       <c r="D75" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>15767.297992500893</v>
       </c>
     </row>
@@ -4231,7 +3971,7 @@
         <v>5</v>
       </c>
       <c r="D76" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>17344.027791750985</v>
       </c>
     </row>
@@ -4246,7 +3986,7 @@
         <v>6</v>
       </c>
       <c r="D77" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>19078.430570926084</v>
       </c>
     </row>
@@ -4261,7 +4001,7 @@
         <v>7</v>
       </c>
       <c r="D78" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>20986.273628018695</v>
       </c>
     </row>
@@ -4276,7 +4016,7 @@
         <v>8</v>
       </c>
       <c r="D79" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>23084.900990820566</v>
       </c>
     </row>
@@ -4291,7 +4031,7 @@
         <v>9</v>
       </c>
       <c r="D80" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>25393.391089902623</v>
       </c>
     </row>
@@ -4306,7 +4046,7 @@
         <v>10</v>
       </c>
       <c r="D81" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>27932.730198892888</v>
       </c>
     </row>
@@ -4321,7 +4061,7 @@
         <v>11</v>
       </c>
       <c r="D82" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>30726.003218782178</v>
       </c>
     </row>
@@ -4336,7 +4076,7 @@
         <v>12</v>
       </c>
       <c r="D83" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>33798.603540660399</v>
       </c>
     </row>
@@ -4351,7 +4091,7 @@
         <v>13</v>
       </c>
       <c r="D84" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>37178.463894726439</v>
       </c>
     </row>
@@ -4366,7 +4106,7 @@
         <v>14</v>
       </c>
       <c r="D85" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>40896.310284199084</v>
       </c>
     </row>
@@ -4381,7 +4121,7 @@
         <v>3</v>
       </c>
       <c r="D86" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>44985.941312618997</v>
       </c>
     </row>
@@ -4396,7 +4136,7 @@
         <v>4</v>
       </c>
       <c r="D87" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>49484.535443880901</v>
       </c>
     </row>
@@ -4411,7 +4151,7 @@
         <v>5</v>
       </c>
       <c r="D88" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>54432.988988268997</v>
       </c>
     </row>
@@ -4426,7 +4166,7 @@
         <v>6</v>
       </c>
       <c r="D89" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>59876.287887095903</v>
       </c>
     </row>
@@ -4441,7 +4181,7 @@
         <v>7</v>
       </c>
       <c r="D90" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>65863.916675805493</v>
       </c>
     </row>
@@ -4456,7 +4196,7 @@
         <v>8</v>
       </c>
       <c r="D91" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>72450.308343386045</v>
       </c>
     </row>
@@ -4471,7 +4211,7 @@
         <v>9</v>
       </c>
       <c r="D92" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>79695.339177724658</v>
       </c>
     </row>
@@ -4486,7 +4226,7 @@
         <v>10</v>
       </c>
       <c r="D93" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>87664.873095497125</v>
       </c>
     </row>
@@ -4501,7 +4241,7 @@
         <v>11</v>
       </c>
       <c r="D94" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>96431.360405046842</v>
       </c>
     </row>
@@ -4516,7 +4256,7 @@
         <v>12</v>
       </c>
       <c r="D95" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>106074.49644555153</v>
       </c>
     </row>
@@ -4531,7 +4271,7 @@
         <v>13</v>
       </c>
       <c r="D96" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>116681.94609010669</v>
       </c>
     </row>
@@ -4546,7 +4286,7 @@
         <v>14</v>
       </c>
       <c r="D97" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>128350.14069911737</v>
       </c>
     </row>

</xml_diff>